<commit_message>
funding cliam 1619 report template changes
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479777B5-B8B6-4577-9661-8508441A007A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42694EB-F53A-4EFA-B19C-D1E37184A8BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="69720" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
   <si>
     <t>Provider :</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Large Employer Data:</t>
   </si>
   <si>
-    <t>Page: 2 of 2</t>
-  </si>
-  <si>
     <t>16-19 Students (including High Needs Students)</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>1920 Condition of Funding Removal</t>
   </si>
   <si>
-    <t>Component Set Version:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Application Version: </t>
   </si>
   <si>
@@ -201,9 +195,6 @@
   </si>
   <si>
     <t>&amp;=FundingClaim.ApplicationVersion</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaim.ComponentSetVersion</t>
   </si>
   <si>
     <t>&amp;=FundingClaim.ReportGeneratedAt</t>
@@ -592,7 +583,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -798,32 +789,48 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1281,31 +1288,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The ESFA </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" strike="sngStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>now only </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>requires a single final claim return with the 16-19 out-turn summary data being included with the other funding streams on the online funding claim form.</a:t>
+            <a:t>The ESFA requires a single final claim return with the 16-19 out-turn summary data being included with the other funding streams on the online funding claim form.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1394,31 +1377,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The purpose of the final claim is to provide the ESFA with an assurance statement by the relevant accounting officer over the regularity of the institution’s funding claim and ILR data returns, as well as being used for providers where reconciliation is appropriate to determine whether any funds paid for 2019 to 2020 will be recovered for underperformance. As stated in ILR Funding Returns 2019 to 2020 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" strike="sngStrike" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>paragraph 24</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>, any adjustment of funds will be finally determined using the final funding claim 2019 to 2020, taking account of any audit qualifications and, in exceptional circumstances, the results of any separate audit or Agency investigation.</a:t>
+            <a:t>The purpose of the final claim is to provide the ESFA with an assurance statement by the relevant accounting officer over the regularity of the institution’s funding claim and ILR data returns, as well as being used for providers where reconciliation is appropriate to determine whether any funds paid for 2019 to 2020 will be recovered for underperformance. As stated in ILR Funding Returns 2019 to 2020, any adjustment of funds will be finally determined using the final funding claim 2019 to 2020, taking account of any audit qualifications and, in exceptional circumstances, the results of any separate audit or Agency investigation.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2022,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A118" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A103" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2040,7 +1999,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
@@ -2066,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="9"/>
@@ -2079,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="9"/>
@@ -2092,16 +2051,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="66" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="9"/>
       <c r="E5" s="27"/>
       <c r="F5" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" s="66" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
@@ -2132,12 +2091,12 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="69"/>
+      <c r="A9" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="71"/>
       <c r="C9" s="32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -2149,29 +2108,29 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="69"/>
+      <c r="A10" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="71"/>
       <c r="C10" s="32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="58" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="69"/>
+      <c r="A11" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="71"/>
       <c r="C11" s="32" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -2179,12 +2138,12 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="69"/>
+      <c r="A12" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="71"/>
       <c r="C12" s="32" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -2192,12 +2151,12 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="69"/>
+      <c r="A13" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="71"/>
       <c r="C13" s="32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -2224,63 +2183,63 @@
         <v>4</v>
       </c>
       <c r="F15" s="43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="43" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="72" t="s">
+    <row r="16" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="67" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="32" t="s">
-        <v>69</v>
+      <c r="D16" s="75" t="s">
+        <v>66</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="73"/>
-      <c r="B17" s="73"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="68"/>
       <c r="C17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="73"/>
-      <c r="B18" s="73"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="68"/>
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="68"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
@@ -2289,13 +2248,13 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
@@ -2304,13 +2263,13 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="68"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="44" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E21" s="46"/>
       <c r="F21" s="46"/>
@@ -2319,10 +2278,10 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
       <c r="C22" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="11">
         <f>SUM(D16:D21)</f>
@@ -2356,7 +2315,7 @@
         <v>4</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>8</v>
@@ -2365,20 +2324,20 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="72" t="s">
-        <v>30</v>
+      <c r="B25" s="67" t="s">
+        <v>29</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>93</v>
+      <c r="D25" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="76" t="s">
+        <v>90</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
@@ -2386,16 +2345,16 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="68"/>
+      <c r="B26" s="68"/>
       <c r="C26" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>94</v>
+        <v>73</v>
+      </c>
+      <c r="E26" s="77" t="s">
+        <v>91</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
@@ -2403,16 +2362,16 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+      <c r="A27" s="68"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>95</v>
+        <v>74</v>
+      </c>
+      <c r="E27" s="77" t="s">
+        <v>92</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -2420,16 +2379,16 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="68"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>96</v>
+        <v>75</v>
+      </c>
+      <c r="E28" s="77" t="s">
+        <v>93</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -2437,16 +2396,16 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
+      <c r="A29" s="68"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>97</v>
+        <v>76</v>
+      </c>
+      <c r="E29" s="77" t="s">
+        <v>94</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
@@ -2454,16 +2413,16 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="68"/>
       <c r="C30" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="E30" s="45" t="s">
-        <v>98</v>
+        <v>77</v>
+      </c>
+      <c r="E30" s="78" t="s">
+        <v>95</v>
       </c>
       <c r="F30" s="16"/>
       <c r="G30" s="16"/>
@@ -2471,10 +2430,10 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="74"/>
-      <c r="B31" s="74"/>
+      <c r="A31" s="69"/>
+      <c r="B31" s="69"/>
       <c r="C31" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="47">
         <f>SUM(D25:D30)</f>
@@ -2511,7 +2470,7 @@
         <v>4</v>
       </c>
       <c r="F33" s="43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>8</v>
@@ -2520,20 +2479,20 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="72" t="s">
-        <v>43</v>
+      <c r="B34" s="67" t="s">
+        <v>42</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>99</v>
+      <c r="D34" s="75" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="76" t="s">
+        <v>96</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -2541,16 +2500,16 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
+      <c r="A35" s="68"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>100</v>
+        <v>79</v>
+      </c>
+      <c r="E35" s="77" t="s">
+        <v>97</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
@@ -2558,16 +2517,16 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="73"/>
-      <c r="B36" s="73"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>101</v>
+        <v>80</v>
+      </c>
+      <c r="E36" s="77" t="s">
+        <v>98</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
@@ -2575,16 +2534,16 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
+      <c r="A37" s="68"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>102</v>
+        <v>81</v>
+      </c>
+      <c r="E37" s="77" t="s">
+        <v>99</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
@@ -2592,16 +2551,16 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="68"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>103</v>
+        <v>82</v>
+      </c>
+      <c r="E38" s="77" t="s">
+        <v>100</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
@@ -2609,16 +2568,16 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="73"/>
-      <c r="B39" s="73"/>
+      <c r="A39" s="68"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D39" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E39" s="45" t="s">
-        <v>104</v>
+        <v>83</v>
+      </c>
+      <c r="E39" s="78" t="s">
+        <v>101</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
@@ -2626,10 +2585,10 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="74"/>
-      <c r="B40" s="74"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="69"/>
       <c r="C40" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" s="47">
         <f>SUM(D34:D39)</f>
@@ -2677,7 +2636,7 @@
         <v>4</v>
       </c>
       <c r="F43" s="43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>8</v>
@@ -2686,20 +2645,20 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="72" t="s">
+      <c r="A44" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="72" t="s">
-        <v>44</v>
+      <c r="B44" s="67" t="s">
+        <v>43</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" s="32" t="s">
-        <v>105</v>
+      <c r="D44" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="E44" s="76" t="s">
+        <v>102</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
@@ -2707,16 +2666,16 @@
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A45" s="73"/>
-      <c r="B45" s="73"/>
+      <c r="A45" s="68"/>
+      <c r="B45" s="68"/>
       <c r="C45" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>106</v>
+        <v>85</v>
+      </c>
+      <c r="E45" s="76" t="s">
+        <v>103</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
@@ -2724,16 +2683,16 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A46" s="73"/>
-      <c r="B46" s="73"/>
+      <c r="A46" s="68"/>
+      <c r="B46" s="68"/>
       <c r="C46" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>107</v>
+        <v>86</v>
+      </c>
+      <c r="E46" s="76" t="s">
+        <v>104</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
@@ -2741,16 +2700,16 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
+      <c r="A47" s="68"/>
+      <c r="B47" s="68"/>
       <c r="C47" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>108</v>
+        <v>87</v>
+      </c>
+      <c r="E47" s="76" t="s">
+        <v>105</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
@@ -2758,16 +2717,16 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A48" s="73"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="68"/>
+      <c r="B48" s="68"/>
       <c r="C48" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="E48" s="76" t="s">
+        <v>106</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
@@ -2775,16 +2734,16 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
+      <c r="A49" s="68"/>
+      <c r="B49" s="68"/>
       <c r="C49" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="45" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E49" s="45" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="18"/>
@@ -2792,10 +2751,10 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="74"/>
-      <c r="B50" s="74"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="69"/>
       <c r="C50" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D50" s="47">
         <f>SUM(D44:D49)</f>
@@ -2836,7 +2795,7 @@
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D53" s="37">
         <f>SUM(D22, D31, D40, D50)</f>
@@ -2872,11 +2831,11 @@
       <c r="A55" s="19"/>
       <c r="B55" s="19"/>
       <c r="C55" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="35" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
@@ -2945,105 +2904,105 @@
       <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="67" t="s">
+      <c r="A61" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="67"/>
-      <c r="C61" s="70" t="s">
+      <c r="B61" s="74"/>
+      <c r="C61" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="70"/>
-      <c r="E61" s="70"/>
+      <c r="D61" s="72"/>
+      <c r="E61" s="72"/>
       <c r="F61" s="31" t="s">
         <v>5</v>
       </c>
       <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="67" t="s">
+      <c r="A62" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B62" s="67"/>
-      <c r="C62" s="67" t="s">
+      <c r="B62" s="74"/>
+      <c r="C62" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="71"/>
-      <c r="E62" s="71"/>
+      <c r="D62" s="73"/>
+      <c r="E62" s="73"/>
       <c r="F62" s="23">
         <v>4000</v>
       </c>
       <c r="G62" s="9"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="67" t="s">
+      <c r="A63" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="67"/>
-      <c r="C63" s="71" t="s">
+      <c r="B63" s="74"/>
+      <c r="C63" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="71"/>
-      <c r="E63" s="71"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
       <c r="F63" s="23">
         <v>3300</v>
       </c>
       <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="67" t="s">
+      <c r="A64" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="67"/>
-      <c r="C64" s="71" t="s">
+      <c r="B64" s="74"/>
+      <c r="C64" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D64" s="71"/>
-      <c r="E64" s="71"/>
+      <c r="D64" s="73"/>
+      <c r="E64" s="73"/>
       <c r="F64" s="23">
         <v>3300</v>
       </c>
       <c r="G64" s="9"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="67" t="s">
+      <c r="A65" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="67"/>
-      <c r="C65" s="71" t="s">
+      <c r="B65" s="74"/>
+      <c r="C65" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="71"/>
-      <c r="E65" s="71"/>
+      <c r="D65" s="73"/>
+      <c r="E65" s="73"/>
       <c r="F65" s="23">
         <v>2700</v>
       </c>
       <c r="G65" s="9"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="67" t="s">
+      <c r="A66" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="67"/>
-      <c r="C66" s="71" t="s">
+      <c r="B66" s="74"/>
+      <c r="C66" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="D66" s="71"/>
-      <c r="E66" s="71"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="73"/>
       <c r="F66" s="23">
         <v>2133</v>
       </c>
       <c r="G66" s="9"/>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="67" t="s">
+      <c r="A67" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B67" s="67"/>
-      <c r="C67" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="D67" s="71"/>
-      <c r="E67" s="71"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="73"/>
+      <c r="E67" s="73"/>
       <c r="F67" s="23">
         <v>4000</v>
       </c>
@@ -4185,19 +4144,19 @@
     </row>
     <row r="194" spans="1:18" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B194" s="60"/>
       <c r="C194" s="60" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D194" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="E194" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="F194" s="68"/>
+        <v>32</v>
+      </c>
+      <c r="E194" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="F194" s="70"/>
       <c r="G194" s="50"/>
       <c r="H194" s="51"/>
       <c r="I194" s="51"/>
@@ -4213,17 +4172,17 @@
     </row>
     <row r="195" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A195" s="61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B195" s="61"/>
       <c r="C195" s="61" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D195" s="62" t="s">
         <v>27</v>
       </c>
       <c r="E195" s="61" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F195" s="61"/>
       <c r="G195" s="59"/>
@@ -4240,18 +4199,11 @@
       <c r="R195" s="51"/>
     </row>
     <row r="196" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A196" s="61" t="s">
-        <v>50</v>
-      </c>
-      <c r="B196" s="61"/>
-      <c r="C196" s="61" t="s">
-        <v>56</v>
-      </c>
       <c r="D196" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E196" s="61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F196" s="61"/>
       <c r="G196" s="54"/>
@@ -4275,7 +4227,7 @@
         <v>28</v>
       </c>
       <c r="E197" s="61" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F197" s="61"/>
       <c r="G197" s="54"/>
@@ -4295,10 +4247,10 @@
       <c r="B198" s="61"/>
       <c r="C198" s="61"/>
       <c r="D198" s="65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E198" s="61" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F198" s="61"/>
       <c r="G198" s="54"/>
@@ -4316,16 +4268,14 @@
     </row>
     <row r="199" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A199" s="61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B199" s="59"/>
       <c r="C199" s="59"/>
       <c r="D199" s="59"/>
       <c r="E199" s="59"/>
       <c r="F199" s="59"/>
-      <c r="G199" s="53" t="s">
-        <v>29</v>
-      </c>
+      <c r="G199" s="53"/>
       <c r="H199" s="51"/>
       <c r="I199" s="51"/>
       <c r="J199" s="51"/>
@@ -4339,11 +4289,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="E194:F194"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C61:E61"/>
@@ -4360,13 +4312,11 @@
     <mergeCell ref="A25:A31"/>
     <mergeCell ref="B25:B31"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="B44:B50"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="58" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -4382,6 +4332,30 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -4525,30 +4499,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
@@ -4558,6 +4508,29 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4572,27 +4545,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Bug fix 87182, 86870,
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F314DD-1F33-4E87-9F4E-A215589B23F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1F71CE-5D9D-42E5-B3A4-E8401992FC98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16-19 Funding Claim" sheetId="3" r:id="rId1"/>
@@ -805,32 +805,32 @@
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1981,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2091,10 +2091,10 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="73"/>
+      <c r="B9" s="75"/>
       <c r="C9" s="32" t="s">
         <v>61</v>
       </c>
@@ -2108,10 +2108,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="73"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="32" t="s">
         <v>62</v>
       </c>
@@ -2125,10 +2125,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="73"/>
+      <c r="B11" s="75"/>
       <c r="C11" s="32" t="s">
         <v>64</v>
       </c>
@@ -2138,10 +2138,10 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="73"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="32" t="s">
         <v>65</v>
       </c>
@@ -2151,10 +2151,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="73"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2190,10 +2190,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="71" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="11" t="s">
@@ -2207,8 +2207,8 @@
       <c r="G16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="77"/>
-      <c r="B17" s="77"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="11" t="s">
         <v>12</v>
       </c>
@@ -2220,8 +2220,8 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="77"/>
-      <c r="B18" s="77"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
@@ -2233,8 +2233,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="11" t="s">
         <v>14</v>
       </c>
@@ -2248,8 +2248,8 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
@@ -2263,8 +2263,8 @@
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="72"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="44" t="s">
         <v>16</v>
       </c>
@@ -2278,8 +2278,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="78"/>
-      <c r="B22" s="78"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="11" t="s">
         <v>30</v>
       </c>
@@ -2324,10 +2324,10 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="76" t="s">
+      <c r="A25" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="71" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -2345,8 +2345,8 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
+      <c r="A26" s="72"/>
+      <c r="B26" s="72"/>
       <c r="C26" s="11" t="s">
         <v>12</v>
       </c>
@@ -2362,8 +2362,8 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="11" t="s">
         <v>13</v>
       </c>
@@ -2379,8 +2379,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="72"/>
+      <c r="B28" s="72"/>
       <c r="C28" s="11" t="s">
         <v>14</v>
       </c>
@@ -2396,8 +2396,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="77"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="72"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="11" t="s">
         <v>15</v>
       </c>
@@ -2413,8 +2413,8 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="11" t="s">
         <v>16</v>
       </c>
@@ -2430,8 +2430,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="78"/>
-      <c r="B31" s="78"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="11" t="s">
         <v>30</v>
       </c>
@@ -2479,10 +2479,10 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="71" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -2500,8 +2500,8 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
+      <c r="A35" s="72"/>
+      <c r="B35" s="72"/>
       <c r="C35" s="11" t="s">
         <v>12</v>
       </c>
@@ -2517,8 +2517,8 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="77"/>
-      <c r="B36" s="77"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="72"/>
       <c r="C36" s="11" t="s">
         <v>13</v>
       </c>
@@ -2534,8 +2534,8 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="77"/>
-      <c r="B37" s="77"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="72"/>
       <c r="C37" s="11" t="s">
         <v>14</v>
       </c>
@@ -2551,8 +2551,8 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="72"/>
+      <c r="B38" s="72"/>
       <c r="C38" s="11" t="s">
         <v>15</v>
       </c>
@@ -2568,8 +2568,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="72"/>
       <c r="C39" s="11" t="s">
         <v>16</v>
       </c>
@@ -2585,8 +2585,8 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="78"/>
-      <c r="B40" s="78"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="11" t="s">
         <v>30</v>
       </c>
@@ -2645,10 +2645,10 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="76" t="s">
+      <c r="A44" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="76" t="s">
+      <c r="B44" s="71" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="11" t="s">
@@ -2666,8 +2666,8 @@
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A45" s="77"/>
-      <c r="B45" s="77"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="72"/>
       <c r="C45" s="11" t="s">
         <v>12</v>
       </c>
@@ -2683,8 +2683,8 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A46" s="77"/>
-      <c r="B46" s="77"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="11" t="s">
         <v>13</v>
       </c>
@@ -2700,8 +2700,8 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A47" s="77"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="72"/>
+      <c r="B47" s="72"/>
       <c r="C47" s="11" t="s">
         <v>14</v>
       </c>
@@ -2717,8 +2717,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A48" s="77"/>
-      <c r="B48" s="77"/>
+      <c r="A48" s="72"/>
+      <c r="B48" s="72"/>
       <c r="C48" s="11" t="s">
         <v>15</v>
       </c>
@@ -2734,15 +2734,15 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A49" s="77"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="72"/>
+      <c r="B49" s="72"/>
       <c r="C49" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="45" t="s">
+      <c r="E49" s="70" t="s">
         <v>107</v>
       </c>
       <c r="F49" s="17"/>
@@ -2751,8 +2751,8 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="78"/>
-      <c r="B50" s="78"/>
+      <c r="A50" s="73"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="11" t="s">
         <v>30</v>
       </c>
@@ -2904,105 +2904,105 @@
       <c r="G60" s="9"/>
     </row>
     <row r="61" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="71" t="s">
+      <c r="A61" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="71"/>
-      <c r="C61" s="74" t="s">
+      <c r="B61" s="78"/>
+      <c r="C61" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="74"/>
-      <c r="E61" s="74"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
       <c r="F61" s="31" t="s">
         <v>5</v>
       </c>
       <c r="G61" s="9"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="71" t="s">
+      <c r="A62" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B62" s="71"/>
-      <c r="C62" s="71" t="s">
+      <c r="B62" s="78"/>
+      <c r="C62" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="75"/>
-      <c r="E62" s="75"/>
+      <c r="D62" s="77"/>
+      <c r="E62" s="77"/>
       <c r="F62" s="23">
         <v>4000</v>
       </c>
       <c r="G62" s="9"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="71" t="s">
+      <c r="A63" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="71"/>
-      <c r="C63" s="75" t="s">
+      <c r="B63" s="78"/>
+      <c r="C63" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
+      <c r="D63" s="77"/>
+      <c r="E63" s="77"/>
       <c r="F63" s="23">
         <v>3300</v>
       </c>
       <c r="G63" s="9"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="71" t="s">
+      <c r="A64" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="71"/>
-      <c r="C64" s="75" t="s">
+      <c r="B64" s="78"/>
+      <c r="C64" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
+      <c r="D64" s="77"/>
+      <c r="E64" s="77"/>
       <c r="F64" s="23">
         <v>3300</v>
       </c>
       <c r="G64" s="9"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="71" t="s">
+      <c r="A65" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="71"/>
-      <c r="C65" s="75" t="s">
+      <c r="B65" s="78"/>
+      <c r="C65" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="77"/>
       <c r="F65" s="23">
         <v>2700</v>
       </c>
       <c r="G65" s="9"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="71" t="s">
+      <c r="A66" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="71"/>
-      <c r="C66" s="75" t="s">
+      <c r="B66" s="78"/>
+      <c r="C66" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
+      <c r="D66" s="77"/>
+      <c r="E66" s="77"/>
       <c r="F66" s="23">
         <v>2133</v>
       </c>
       <c r="G66" s="9"/>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="71" t="s">
+      <c r="A67" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="B67" s="71"/>
-      <c r="C67" s="75" t="s">
+      <c r="B67" s="78"/>
+      <c r="C67" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="77"/>
       <c r="F67" s="23">
         <v>4000</v>
       </c>
@@ -4153,10 +4153,10 @@
       <c r="D194" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="E194" s="72" t="s">
+      <c r="E194" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="F194" s="72"/>
+      <c r="F194" s="74"/>
       <c r="G194" s="50"/>
       <c r="H194" s="51"/>
       <c r="I194" s="51"/>
@@ -4289,11 +4289,13 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
     <mergeCell ref="E194:F194"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C61:E61"/>
@@ -4310,13 +4312,11 @@
     <mergeCell ref="A25:A31"/>
     <mergeCell ref="B25:B31"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="B44:B50"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="58" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -4331,7 +4331,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4479,12 +4484,7 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4503,9 +4503,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4528,9 +4528,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Bug 88814- FISReportFilterDate ReferenceDate
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1F71CE-5D9D-42E5-B3A4-E8401992FC98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D827F54-E9A0-4660-A7D6-28B805786A85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16-19 Funding Claim" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="110">
   <si>
     <t>Provider :</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>&amp;=FundingClaim.CofRemoval</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.ReferenceDate</t>
   </si>
 </sst>
 </file>
@@ -583,7 +586,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
@@ -685,9 +688,6 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -805,14 +805,9 @@
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -828,9 +823,14 @@
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1981,23 +1981,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.73046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.73046875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.265625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>40</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2020,11 +2020,11 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="65" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="26"/>
@@ -2033,11 +2033,11 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="65" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="26"/>
@@ -2046,11 +2046,11 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="65" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="28"/>
@@ -2059,11 +2059,11 @@
       <c r="F5" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="66" t="s">
+      <c r="G5" s="65" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2072,7 +2072,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2081,7 +2081,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -2090,45 +2090,45 @@
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="75" t="s">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="75"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="32" t="s">
         <v>61</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="36" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="75" t="s">
+      <c r="G9" s="57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="75"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="32" t="s">
         <v>62</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="58" t="s">
+      <c r="G10" s="57" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="75" t="s">
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="75"/>
+      <c r="B11" s="72"/>
       <c r="C11" s="32" t="s">
         <v>64</v>
       </c>
@@ -2137,11 +2137,11 @@
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="75" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="75"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="32" t="s">
         <v>65</v>
       </c>
@@ -2150,11 +2150,11 @@
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="75"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2163,7 +2163,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -2172,43 +2172,43 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="42" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="71" t="s">
+    <row r="16" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="71" t="s">
+      <c r="B16" s="75" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="67" t="s">
+      <c r="D16" s="66" t="s">
         <v>66</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
     </row>
-    <row r="17" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="72"/>
-      <c r="B17" s="72"/>
+    <row r="17" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="76"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="11" t="s">
         <v>12</v>
       </c>
@@ -2219,9 +2219,9 @@
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
     </row>
-    <row r="18" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="72"/>
-      <c r="B18" s="72"/>
+    <row r="18" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="76"/>
+      <c r="B18" s="76"/>
       <c r="C18" s="11" t="s">
         <v>13</v>
       </c>
@@ -2232,9 +2232,9 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="72"/>
-      <c r="B19" s="72"/>
+    <row r="19" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="76"/>
+      <c r="B19" s="76"/>
       <c r="C19" s="11" t="s">
         <v>14</v>
       </c>
@@ -2247,9 +2247,9 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="72"/>
-      <c r="B20" s="72"/>
+    <row r="20" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="76"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="11" t="s">
         <v>15</v>
       </c>
@@ -2262,24 +2262,24 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="72"/>
-      <c r="B21" s="72"/>
-      <c r="C21" s="44" t="s">
+    <row r="21" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="76"/>
+      <c r="B21" s="76"/>
+      <c r="C21" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
       <c r="G21" s="13"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+    <row r="22" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
         <v>30</v>
       </c>
@@ -2293,7 +2293,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -2304,7 +2304,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -2314,7 +2314,7 @@
       <c r="E24" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="42" t="s">
         <v>41</v>
       </c>
       <c r="G24" s="10" t="s">
@@ -2323,20 +2323,20 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="71" t="s">
+    <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="71" t="s">
+      <c r="B25" s="75" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="67" t="s">
+      <c r="D25" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="68" t="s">
+      <c r="E25" s="67" t="s">
         <v>90</v>
       </c>
       <c r="F25" s="17"/>
@@ -2344,16 +2344,16 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="72"/>
-      <c r="B26" s="72"/>
+    <row r="26" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="76"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="69" t="s">
+      <c r="E26" s="68" t="s">
         <v>91</v>
       </c>
       <c r="F26" s="17"/>
@@ -2361,16 +2361,16 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="72"/>
-      <c r="B27" s="72"/>
+    <row r="27" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="76"/>
+      <c r="B27" s="76"/>
       <c r="C27" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="69" t="s">
+      <c r="E27" s="68" t="s">
         <v>92</v>
       </c>
       <c r="F27" s="17"/>
@@ -2378,16 +2378,16 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="72"/>
-      <c r="B28" s="72"/>
+    <row r="28" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="76"/>
+      <c r="B28" s="76"/>
       <c r="C28" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="69" t="s">
+      <c r="E28" s="68" t="s">
         <v>93</v>
       </c>
       <c r="F28" s="17"/>
@@ -2395,16 +2395,16 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="72"/>
-      <c r="B29" s="72"/>
+    <row r="29" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="76"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E29" s="69" t="s">
+      <c r="E29" s="68" t="s">
         <v>94</v>
       </c>
       <c r="F29" s="17"/>
@@ -2412,16 +2412,16 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="72"/>
-      <c r="B30" s="72"/>
+    <row r="30" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="76"/>
+      <c r="B30" s="76"/>
       <c r="C30" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="45" t="s">
+      <c r="D30" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="70" t="s">
+      <c r="E30" s="69" t="s">
         <v>95</v>
       </c>
       <c r="F30" s="16"/>
@@ -2429,17 +2429,17 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
+    <row r="31" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="47">
+      <c r="D31" s="46">
         <f>SUM(D25:D30)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="48">
+      <c r="E31" s="47">
         <f>SUM(E25:E30)</f>
         <v>0</v>
       </c>
@@ -2448,7 +2448,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -2459,7 +2459,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A33" s="14"/>
       <c r="B33" s="14"/>
       <c r="C33" s="15"/>
@@ -2469,7 +2469,7 @@
       <c r="E33" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="43" t="s">
+      <c r="F33" s="42" t="s">
         <v>41</v>
       </c>
       <c r="G33" s="10" t="s">
@@ -2478,20 +2478,20 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="71" t="s">
+    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="75" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="67" t="s">
+      <c r="D34" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="68" t="s">
+      <c r="E34" s="67" t="s">
         <v>96</v>
       </c>
       <c r="F34" s="17"/>
@@ -2499,16 +2499,16 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="72"/>
-      <c r="B35" s="72"/>
+    <row r="35" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="76"/>
+      <c r="B35" s="76"/>
       <c r="C35" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="69" t="s">
+      <c r="E35" s="68" t="s">
         <v>97</v>
       </c>
       <c r="F35" s="17"/>
@@ -2516,16 +2516,16 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="72"/>
-      <c r="B36" s="72"/>
+    <row r="36" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="76"/>
+      <c r="B36" s="76"/>
       <c r="C36" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="69" t="s">
+      <c r="E36" s="68" t="s">
         <v>98</v>
       </c>
       <c r="F36" s="17"/>
@@ -2533,16 +2533,16 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="72"/>
-      <c r="B37" s="72"/>
+    <row r="37" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="76"/>
+      <c r="B37" s="76"/>
       <c r="C37" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="E37" s="69" t="s">
+      <c r="E37" s="68" t="s">
         <v>99</v>
       </c>
       <c r="F37" s="17"/>
@@ -2550,16 +2550,16 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="72"/>
-      <c r="B38" s="72"/>
+    <row r="38" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A38" s="76"/>
+      <c r="B38" s="76"/>
       <c r="C38" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="69" t="s">
+      <c r="E38" s="68" t="s">
         <v>100</v>
       </c>
       <c r="F38" s="17"/>
@@ -2567,16 +2567,16 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="72"/>
-      <c r="B39" s="72"/>
+    <row r="39" spans="1:9" ht="40.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="76"/>
+      <c r="B39" s="76"/>
       <c r="C39" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D39" s="45" t="s">
+      <c r="D39" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="E39" s="70" t="s">
+      <c r="E39" s="69" t="s">
         <v>101</v>
       </c>
       <c r="F39" s="17"/>
@@ -2584,17 +2584,17 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="73"/>
-      <c r="B40" s="73"/>
+    <row r="40" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="47">
+      <c r="D40" s="46">
         <f>SUM(D34:D39)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="48">
+      <c r="E40" s="47">
         <f>SUM(E34:E39)</f>
         <v>0</v>
       </c>
@@ -2603,7 +2603,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A41" s="19"/>
       <c r="B41" s="19"/>
       <c r="C41" s="20"/>
@@ -2614,7 +2614,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
@@ -2625,7 +2625,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A43" s="14"/>
       <c r="B43" s="14"/>
       <c r="C43" s="15"/>
@@ -2635,7 +2635,7 @@
       <c r="E43" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="43" t="s">
+      <c r="F43" s="42" t="s">
         <v>41</v>
       </c>
       <c r="G43" s="10" t="s">
@@ -2644,20 +2644,20 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="71" t="s">
+    <row r="44" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="71" t="s">
+      <c r="B44" s="75" t="s">
         <v>43</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="67" t="s">
+      <c r="D44" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="68" t="s">
+      <c r="E44" s="67" t="s">
         <v>102</v>
       </c>
       <c r="F44" s="17"/>
@@ -2665,16 +2665,16 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A45" s="72"/>
-      <c r="B45" s="72"/>
+    <row r="45" spans="1:9" ht="54" x14ac:dyDescent="0.35">
+      <c r="A45" s="76"/>
+      <c r="B45" s="76"/>
       <c r="C45" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E45" s="68" t="s">
+      <c r="E45" s="67" t="s">
         <v>103</v>
       </c>
       <c r="F45" s="17"/>
@@ -2682,16 +2682,16 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A46" s="72"/>
-      <c r="B46" s="72"/>
+    <row r="46" spans="1:9" ht="54" x14ac:dyDescent="0.35">
+      <c r="A46" s="76"/>
+      <c r="B46" s="76"/>
       <c r="C46" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="68" t="s">
+      <c r="E46" s="67" t="s">
         <v>104</v>
       </c>
       <c r="F46" s="17"/>
@@ -2699,16 +2699,16 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A47" s="72"/>
-      <c r="B47" s="72"/>
+    <row r="47" spans="1:9" ht="54" x14ac:dyDescent="0.35">
+      <c r="A47" s="76"/>
+      <c r="B47" s="76"/>
       <c r="C47" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E47" s="68" t="s">
+      <c r="E47" s="67" t="s">
         <v>105</v>
       </c>
       <c r="F47" s="17"/>
@@ -2716,16 +2716,16 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A48" s="72"/>
-      <c r="B48" s="72"/>
+    <row r="48" spans="1:9" ht="54" x14ac:dyDescent="0.35">
+      <c r="A48" s="76"/>
+      <c r="B48" s="76"/>
       <c r="C48" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E48" s="68" t="s">
+      <c r="E48" s="67" t="s">
         <v>106</v>
       </c>
       <c r="F48" s="17"/>
@@ -2733,16 +2733,16 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A49" s="72"/>
-      <c r="B49" s="72"/>
+    <row r="49" spans="1:9" ht="54" x14ac:dyDescent="0.35">
+      <c r="A49" s="76"/>
+      <c r="B49" s="76"/>
       <c r="C49" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="45" t="s">
+      <c r="D49" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="E49" s="70" t="s">
+      <c r="E49" s="69" t="s">
         <v>107</v>
       </c>
       <c r="F49" s="17"/>
@@ -2750,17 +2750,17 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="73"/>
-      <c r="B50" s="73"/>
+    <row r="50" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D50" s="47">
+      <c r="D50" s="46">
         <f>SUM(D44:D49)</f>
         <v>0</v>
       </c>
-      <c r="E50" s="48">
+      <c r="E50" s="47">
         <f>SUM(E44:E49)</f>
         <v>0</v>
       </c>
@@ -2769,7 +2769,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
       <c r="C51" s="20"/>
@@ -2780,7 +2780,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A52" s="19"/>
       <c r="B52" s="19"/>
       <c r="C52" s="20"/>
@@ -2791,13 +2791,13 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="37">
+      <c r="D53" s="36">
         <f>SUM(D22, D31, D40, D50)</f>
         <v>0</v>
       </c>
@@ -2816,7 +2816,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A54" s="19"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
@@ -2827,7 +2827,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" ht="41.65" x14ac:dyDescent="0.35">
       <c r="A55" s="19"/>
       <c r="B55" s="19"/>
       <c r="C55" s="11" t="s">
@@ -2842,7 +2842,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20"/>
@@ -2853,13 +2853,13 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="37">
+      <c r="D57" s="36">
         <f>SUM(D53)</f>
         <v>0</v>
       </c>
@@ -2876,25 +2876,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="20"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="38"/>
-      <c r="F58" s="38"/>
-      <c r="G58" s="38"/>
-    </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="D58" s="54"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+    </row>
+    <row r="59" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A59" s="19"/>
       <c r="B59" s="19"/>
       <c r="C59" s="20"/>
-      <c r="D59" s="55"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-    </row>
-    <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D59" s="54"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+    </row>
+    <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -2903,121 +2903,121 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="78" t="s">
+    <row r="61" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A61" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="B61" s="78"/>
-      <c r="C61" s="76" t="s">
+      <c r="B61" s="70"/>
+      <c r="C61" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="D61" s="76"/>
-      <c r="E61" s="76"/>
+      <c r="D61" s="73"/>
+      <c r="E61" s="73"/>
       <c r="F61" s="31" t="s">
         <v>5</v>
       </c>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="78" t="s">
+    <row r="62" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A62" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B62" s="78"/>
-      <c r="C62" s="78" t="s">
+      <c r="B62" s="70"/>
+      <c r="C62" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D62" s="77"/>
-      <c r="E62" s="77"/>
+      <c r="D62" s="74"/>
+      <c r="E62" s="74"/>
       <c r="F62" s="23">
         <v>4000</v>
       </c>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="78" t="s">
+    <row r="63" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A63" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B63" s="78"/>
-      <c r="C63" s="77" t="s">
+      <c r="B63" s="70"/>
+      <c r="C63" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="77"/>
-      <c r="E63" s="77"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
       <c r="F63" s="23">
         <v>3300</v>
       </c>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="78" t="s">
+    <row r="64" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A64" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B64" s="78"/>
-      <c r="C64" s="77" t="s">
+      <c r="B64" s="70"/>
+      <c r="C64" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="D64" s="77"/>
-      <c r="E64" s="77"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
       <c r="F64" s="23">
         <v>3300</v>
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="78" t="s">
+    <row r="65" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A65" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="78"/>
-      <c r="C65" s="77" t="s">
+      <c r="B65" s="70"/>
+      <c r="C65" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="77"/>
-      <c r="E65" s="77"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
       <c r="F65" s="23">
         <v>2700</v>
       </c>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="78" t="s">
+    <row r="66" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A66" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="78"/>
-      <c r="C66" s="77" t="s">
+      <c r="B66" s="70"/>
+      <c r="C66" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D66" s="77"/>
-      <c r="E66" s="77"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
       <c r="F66" s="23">
         <v>2133</v>
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="78" t="s">
+    <row r="67" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A67" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="B67" s="78"/>
-      <c r="C67" s="77" t="s">
+      <c r="B67" s="70"/>
+      <c r="C67" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D67" s="77"/>
-      <c r="E67" s="77"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
       <c r="F67" s="23">
         <v>4000</v>
       </c>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="39"/>
-      <c r="B68" s="39"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="41"/>
+    <row r="68" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A68" s="38"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="40"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -3026,7 +3026,7 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -3035,7 +3035,7 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -3044,7 +3044,7 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -3053,7 +3053,7 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -3062,7 +3062,7 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -3071,7 +3071,7 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -3080,7 +3080,7 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -3089,7 +3089,7 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -3098,7 +3098,7 @@
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -3107,7 +3107,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -3116,7 +3116,7 @@
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -3125,7 +3125,7 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -3134,7 +3134,7 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
     </row>
-    <row r="82" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -3143,7 +3143,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -3152,7 +3152,7 @@
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -3161,7 +3161,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -3170,7 +3170,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -3179,7 +3179,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -3188,7 +3188,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -3197,7 +3197,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -3206,7 +3206,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -3215,7 +3215,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -3224,7 +3224,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -3233,7 +3233,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -3242,7 +3242,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3251,7 +3251,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3260,7 +3260,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3269,7 +3269,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -3278,7 +3278,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3287,7 +3287,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
@@ -3296,7 +3296,7 @@
       <c r="F99" s="6"/>
       <c r="G99" s="6"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
@@ -3305,7 +3305,7 @@
       <c r="F100" s="6"/>
       <c r="G100" s="6"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
@@ -3314,7 +3314,7 @@
       <c r="F101" s="6"/>
       <c r="G101" s="6"/>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
@@ -3323,7 +3323,7 @@
       <c r="F102" s="6"/>
       <c r="G102" s="6"/>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
@@ -3332,7 +3332,7 @@
       <c r="F103" s="6"/>
       <c r="G103" s="6"/>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
@@ -3341,7 +3341,7 @@
       <c r="F104" s="6"/>
       <c r="G104" s="6"/>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
@@ -3350,7 +3350,7 @@
       <c r="F105" s="6"/>
       <c r="G105" s="6"/>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
@@ -3359,7 +3359,7 @@
       <c r="F106" s="6"/>
       <c r="G106" s="6"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -3368,7 +3368,7 @@
       <c r="F107" s="6"/>
       <c r="G107" s="6"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
@@ -3377,7 +3377,7 @@
       <c r="F108" s="6"/>
       <c r="G108" s="6"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -3386,7 +3386,7 @@
       <c r="F109" s="6"/>
       <c r="G109" s="6"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -3395,7 +3395,7 @@
       <c r="F110" s="6"/>
       <c r="G110" s="6"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
@@ -3404,7 +3404,7 @@
       <c r="F111" s="6"/>
       <c r="G111" s="6"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" s="6"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
@@ -3413,7 +3413,7 @@
       <c r="F112" s="6"/>
       <c r="G112" s="6"/>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -3422,7 +3422,7 @@
       <c r="F113" s="6"/>
       <c r="G113" s="6"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
@@ -3431,7 +3431,7 @@
       <c r="F114" s="6"/>
       <c r="G114" s="6"/>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -3440,7 +3440,7 @@
       <c r="F115" s="6"/>
       <c r="G115" s="6"/>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
@@ -3449,7 +3449,7 @@
       <c r="F116" s="6"/>
       <c r="G116" s="6"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
@@ -3458,7 +3458,7 @@
       <c r="F117" s="6"/>
       <c r="G117" s="6"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A118" s="6"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
@@ -3467,7 +3467,7 @@
       <c r="F118" s="6"/>
       <c r="G118" s="6"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
@@ -3476,7 +3476,7 @@
       <c r="F119" s="6"/>
       <c r="G119" s="6"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -3485,7 +3485,7 @@
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
@@ -3494,7 +3494,7 @@
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -3503,7 +3503,7 @@
       <c r="F122" s="6"/>
       <c r="G122" s="6"/>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
@@ -3512,7 +3512,7 @@
       <c r="F123" s="6"/>
       <c r="G123" s="6"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A124" s="6"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
@@ -3521,7 +3521,7 @@
       <c r="F124" s="6"/>
       <c r="G124" s="6"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
@@ -3530,7 +3530,7 @@
       <c r="F125" s="6"/>
       <c r="G125" s="6"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
@@ -3539,7 +3539,7 @@
       <c r="F126" s="6"/>
       <c r="G126" s="6"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
@@ -3548,7 +3548,7 @@
       <c r="F127" s="6"/>
       <c r="G127" s="6"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
@@ -3557,7 +3557,7 @@
       <c r="F128" s="6"/>
       <c r="G128" s="6"/>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
@@ -3566,7 +3566,7 @@
       <c r="F129" s="6"/>
       <c r="G129" s="6"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A130" s="6"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
@@ -3575,7 +3575,7 @@
       <c r="F130" s="6"/>
       <c r="G130" s="6"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" s="6"/>
       <c r="B131" s="6"/>
       <c r="C131" s="6"/>
@@ -3584,7 +3584,7 @@
       <c r="F131" s="6"/>
       <c r="G131" s="6"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" s="6"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
@@ -3593,7 +3593,7 @@
       <c r="F132" s="6"/>
       <c r="G132" s="6"/>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
@@ -3602,7 +3602,7 @@
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" s="6"/>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
@@ -3611,7 +3611,7 @@
       <c r="F134" s="6"/>
       <c r="G134" s="6"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" s="6"/>
       <c r="B135" s="6"/>
       <c r="C135" s="6"/>
@@ -3620,7 +3620,7 @@
       <c r="F135" s="6"/>
       <c r="G135" s="6"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" s="6"/>
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
@@ -3629,7 +3629,7 @@
       <c r="F136" s="6"/>
       <c r="G136" s="6"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" s="6"/>
       <c r="B137" s="6"/>
       <c r="C137" s="6"/>
@@ -3638,7 +3638,7 @@
       <c r="F137" s="6"/>
       <c r="G137" s="6"/>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" s="6"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
@@ -3647,7 +3647,7 @@
       <c r="F138" s="6"/>
       <c r="G138" s="6"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" s="6"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
@@ -3656,7 +3656,7 @@
       <c r="F139" s="6"/>
       <c r="G139" s="6"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" s="6"/>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
@@ -3665,7 +3665,7 @@
       <c r="F140" s="6"/>
       <c r="G140" s="6"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
@@ -3674,7 +3674,7 @@
       <c r="F141" s="6"/>
       <c r="G141" s="6"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
@@ -3683,7 +3683,7 @@
       <c r="F142" s="6"/>
       <c r="G142" s="6"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" s="6"/>
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
@@ -3692,7 +3692,7 @@
       <c r="F143" s="6"/>
       <c r="G143" s="6"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" s="6"/>
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
@@ -3701,7 +3701,7 @@
       <c r="F144" s="6"/>
       <c r="G144" s="6"/>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="6"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6"/>
@@ -3710,7 +3710,7 @@
       <c r="F145" s="6"/>
       <c r="G145" s="6"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A146" s="6"/>
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
@@ -3719,7 +3719,7 @@
       <c r="F146" s="6"/>
       <c r="G146" s="6"/>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A147" s="6"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
@@ -3728,7 +3728,7 @@
       <c r="F147" s="6"/>
       <c r="G147" s="6"/>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A148" s="6"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
@@ -3737,7 +3737,7 @@
       <c r="F148" s="6"/>
       <c r="G148" s="6"/>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A149" s="6"/>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
@@ -3746,7 +3746,7 @@
       <c r="F149" s="6"/>
       <c r="G149" s="6"/>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A150" s="6"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
@@ -3755,7 +3755,7 @@
       <c r="F150" s="6"/>
       <c r="G150" s="6"/>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
@@ -3764,7 +3764,7 @@
       <c r="F151" s="6"/>
       <c r="G151" s="6"/>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A152" s="6"/>
       <c r="B152" s="6"/>
       <c r="C152" s="6"/>
@@ -3773,7 +3773,7 @@
       <c r="F152" s="6"/>
       <c r="G152" s="6"/>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A153" s="6"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
@@ -3782,7 +3782,7 @@
       <c r="F153" s="6"/>
       <c r="G153" s="6"/>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A154" s="6"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
@@ -3791,7 +3791,7 @@
       <c r="F154" s="6"/>
       <c r="G154" s="6"/>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
@@ -3800,7 +3800,7 @@
       <c r="F155" s="6"/>
       <c r="G155" s="6"/>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A156" s="6"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
@@ -3809,7 +3809,7 @@
       <c r="F156" s="6"/>
       <c r="G156" s="6"/>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
@@ -3818,7 +3818,7 @@
       <c r="F157" s="6"/>
       <c r="G157" s="6"/>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
@@ -3827,7 +3827,7 @@
       <c r="F158" s="6"/>
       <c r="G158" s="6"/>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
@@ -3836,7 +3836,7 @@
       <c r="F159" s="6"/>
       <c r="G159" s="6"/>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A160" s="6"/>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
@@ -3845,7 +3845,7 @@
       <c r="F160" s="6"/>
       <c r="G160" s="6"/>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" s="6"/>
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
@@ -3854,7 +3854,7 @@
       <c r="F161" s="6"/>
       <c r="G161" s="6"/>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" s="6"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
@@ -3863,7 +3863,7 @@
       <c r="F162" s="6"/>
       <c r="G162" s="6"/>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
@@ -3872,7 +3872,7 @@
       <c r="F163" s="6"/>
       <c r="G163" s="6"/>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A164" s="6"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
@@ -3881,7 +3881,7 @@
       <c r="F164" s="6"/>
       <c r="G164" s="6"/>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" s="6"/>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
@@ -3890,7 +3890,7 @@
       <c r="F165" s="6"/>
       <c r="G165" s="6"/>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" s="6"/>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
@@ -3899,7 +3899,7 @@
       <c r="F166" s="6"/>
       <c r="G166" s="6"/>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" s="6"/>
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
@@ -3908,7 +3908,7 @@
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" s="6"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
@@ -3917,7 +3917,7 @@
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
@@ -3926,7 +3926,7 @@
       <c r="F169" s="6"/>
       <c r="G169" s="6"/>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" s="6"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
@@ -3935,7 +3935,7 @@
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
@@ -3944,7 +3944,7 @@
       <c r="F171" s="6"/>
       <c r="G171" s="6"/>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" s="6"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
@@ -3953,7 +3953,7 @@
       <c r="F172" s="6"/>
       <c r="G172" s="6"/>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" s="6"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
@@ -3962,7 +3962,7 @@
       <c r="F173" s="6"/>
       <c r="G173" s="6"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
@@ -3971,7 +3971,7 @@
       <c r="F174" s="6"/>
       <c r="G174" s="6"/>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" s="6"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
@@ -3980,7 +3980,7 @@
       <c r="F175" s="6"/>
       <c r="G175" s="6"/>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
@@ -3989,7 +3989,7 @@
       <c r="F176" s="6"/>
       <c r="G176" s="6"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" s="6"/>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
@@ -3998,7 +3998,7 @@
       <c r="F177" s="6"/>
       <c r="G177" s="6"/>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" s="6"/>
       <c r="B178" s="6"/>
       <c r="C178" s="6"/>
@@ -4007,7 +4007,7 @@
       <c r="F178" s="6"/>
       <c r="G178" s="6"/>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" s="6"/>
       <c r="B179" s="6"/>
       <c r="C179" s="6"/>
@@ -4016,7 +4016,7 @@
       <c r="F179" s="6"/>
       <c r="G179" s="6"/>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" s="6"/>
       <c r="B180" s="6"/>
       <c r="C180" s="6"/>
@@ -4025,7 +4025,7 @@
       <c r="F180" s="6"/>
       <c r="G180" s="6"/>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181" s="6"/>
       <c r="B181" s="6"/>
       <c r="C181" s="6"/>
@@ -4034,7 +4034,7 @@
       <c r="F181" s="6"/>
       <c r="G181" s="6"/>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A182" s="6"/>
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
@@ -4043,7 +4043,7 @@
       <c r="F182" s="6"/>
       <c r="G182" s="6"/>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183" s="6"/>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
@@ -4052,7 +4052,7 @@
       <c r="F183" s="6"/>
       <c r="G183" s="6"/>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A184" s="6"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
@@ -4061,7 +4061,7 @@
       <c r="F184" s="6"/>
       <c r="G184" s="6"/>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
@@ -4070,7 +4070,7 @@
       <c r="F185" s="6"/>
       <c r="G185" s="6"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" s="6"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
@@ -4079,7 +4079,7 @@
       <c r="F186" s="6"/>
       <c r="G186" s="6"/>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187" s="6"/>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
@@ -4088,7 +4088,7 @@
       <c r="F187" s="6"/>
       <c r="G187" s="6"/>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188" s="6"/>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
@@ -4097,7 +4097,7 @@
       <c r="F188" s="6"/>
       <c r="G188" s="6"/>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" s="6"/>
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
@@ -4106,7 +4106,7 @@
       <c r="F189" s="6"/>
       <c r="G189" s="6"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A190" s="6"/>
       <c r="B190" s="6"/>
       <c r="C190" s="6"/>
@@ -4115,7 +4115,7 @@
       <c r="F190" s="6"/>
       <c r="G190" s="6"/>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191" s="6"/>
       <c r="B191" s="6"/>
       <c r="C191" s="6"/>
@@ -4124,7 +4124,7 @@
       <c r="F191" s="6"/>
       <c r="G191" s="6"/>
     </row>
-    <row r="192" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="6"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
@@ -4133,7 +4133,7 @@
       <c r="F192" s="6"/>
       <c r="G192" s="6"/>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A193" s="6"/>
       <c r="B193" s="6"/>
       <c r="C193" s="6"/>
@@ -4142,160 +4142,158 @@
       <c r="F193" s="6"/>
       <c r="G193" s="6"/>
     </row>
-    <row r="194" spans="1:18" s="52" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="60" t="s">
+    <row r="194" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A194" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="B194" s="60"/>
-      <c r="C194" s="60" t="s">
+      <c r="B194" s="59"/>
+      <c r="C194" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="D194" s="49" t="s">
+      <c r="D194" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E194" s="74" t="s">
+      <c r="E194" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="F194" s="74"/>
-      <c r="G194" s="50"/>
-      <c r="H194" s="51"/>
-      <c r="I194" s="51"/>
-      <c r="J194" s="51"/>
-      <c r="K194" s="51"/>
-      <c r="L194" s="51"/>
-      <c r="M194" s="51"/>
-      <c r="N194" s="51"/>
-      <c r="O194" s="51"/>
-      <c r="P194" s="51"/>
-      <c r="Q194" s="51"/>
-      <c r="R194" s="51"/>
-    </row>
-    <row r="195" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A195" s="61" t="s">
+      <c r="F194" s="71"/>
+      <c r="G194" s="49"/>
+      <c r="H194" s="50"/>
+      <c r="I194" s="50"/>
+      <c r="J194" s="50"/>
+      <c r="K194" s="50"/>
+      <c r="L194" s="50"/>
+      <c r="M194" s="50"/>
+      <c r="N194" s="50"/>
+      <c r="O194" s="50"/>
+      <c r="P194" s="50"/>
+      <c r="Q194" s="50"/>
+      <c r="R194" s="50"/>
+    </row>
+    <row r="195" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A195" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="B195" s="61"/>
-      <c r="C195" s="61" t="s">
+      <c r="B195" s="60"/>
+      <c r="C195" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D195" s="62" t="s">
+      <c r="D195" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="E195" s="61" t="s">
+      <c r="E195" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="F195" s="61"/>
-      <c r="G195" s="59"/>
-      <c r="H195" s="51"/>
-      <c r="I195" s="51"/>
-      <c r="J195" s="51"/>
-      <c r="K195" s="51"/>
-      <c r="L195" s="51"/>
-      <c r="M195" s="51"/>
-      <c r="N195" s="51"/>
-      <c r="O195" s="51"/>
-      <c r="P195" s="51"/>
-      <c r="Q195" s="51"/>
-      <c r="R195" s="51"/>
-    </row>
-    <row r="196" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="D196" s="62" t="s">
+      <c r="F195" s="60"/>
+      <c r="G195" s="58"/>
+      <c r="H195" s="50"/>
+      <c r="I195" s="50"/>
+      <c r="J195" s="50"/>
+      <c r="K195" s="50"/>
+      <c r="L195" s="50"/>
+      <c r="M195" s="50"/>
+      <c r="N195" s="50"/>
+      <c r="O195" s="50"/>
+      <c r="P195" s="50"/>
+      <c r="Q195" s="50"/>
+      <c r="R195" s="50"/>
+    </row>
+    <row r="196" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="D196" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="E196" s="61" t="s">
+      <c r="E196" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="F196" s="61"/>
-      <c r="G196" s="54"/>
-      <c r="H196" s="51"/>
-      <c r="I196" s="51"/>
-      <c r="J196" s="51"/>
-      <c r="K196" s="51"/>
-      <c r="L196" s="51"/>
-      <c r="M196" s="51"/>
-      <c r="N196" s="51"/>
-      <c r="O196" s="51"/>
-      <c r="P196" s="51"/>
-      <c r="Q196" s="51"/>
-      <c r="R196" s="51"/>
-    </row>
-    <row r="197" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A197" s="63"/>
-      <c r="B197" s="63"/>
-      <c r="C197" s="64"/>
-      <c r="D197" s="65" t="s">
+      <c r="F196" s="60"/>
+      <c r="G196" s="53"/>
+      <c r="H196" s="50"/>
+      <c r="I196" s="50"/>
+      <c r="J196" s="50"/>
+      <c r="K196" s="50"/>
+      <c r="L196" s="50"/>
+      <c r="M196" s="50"/>
+      <c r="N196" s="50"/>
+      <c r="O196" s="50"/>
+      <c r="P196" s="50"/>
+      <c r="Q196" s="50"/>
+      <c r="R196" s="50"/>
+    </row>
+    <row r="197" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A197" s="62"/>
+      <c r="B197" s="62"/>
+      <c r="C197" s="63"/>
+      <c r="D197" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="E197" s="61" t="s">
+      <c r="E197" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="F197" s="61"/>
-      <c r="G197" s="54"/>
-      <c r="H197" s="51"/>
-      <c r="I197" s="51"/>
-      <c r="J197" s="51"/>
-      <c r="K197" s="51"/>
-      <c r="L197" s="51"/>
-      <c r="M197" s="51"/>
-      <c r="N197" s="51"/>
-      <c r="O197" s="51"/>
-      <c r="P197" s="51"/>
-      <c r="Q197" s="51"/>
-      <c r="R197" s="51"/>
-    </row>
-    <row r="198" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B198" s="61"/>
-      <c r="C198" s="61"/>
-      <c r="D198" s="65" t="s">
+      <c r="F197" s="60"/>
+      <c r="G197" s="53"/>
+      <c r="H197" s="50"/>
+      <c r="I197" s="50"/>
+      <c r="J197" s="50"/>
+      <c r="K197" s="50"/>
+      <c r="L197" s="50"/>
+      <c r="M197" s="50"/>
+      <c r="N197" s="50"/>
+      <c r="O197" s="50"/>
+      <c r="P197" s="50"/>
+      <c r="Q197" s="50"/>
+      <c r="R197" s="50"/>
+    </row>
+    <row r="198" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B198" s="60"/>
+      <c r="C198" s="60"/>
+      <c r="D198" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="E198" s="61" t="s">
+      <c r="E198" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="F198" s="61"/>
-      <c r="G198" s="54"/>
-      <c r="H198" s="51"/>
-      <c r="I198" s="51"/>
-      <c r="J198" s="51"/>
-      <c r="K198" s="51"/>
-      <c r="L198" s="51"/>
-      <c r="M198" s="51"/>
-      <c r="N198" s="51"/>
-      <c r="O198" s="51"/>
-      <c r="P198" s="51"/>
-      <c r="Q198" s="51"/>
-      <c r="R198" s="51"/>
-    </row>
-    <row r="199" spans="1:18" s="52" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A199" s="61" t="s">
+      <c r="F198" s="60"/>
+      <c r="G198" s="53"/>
+      <c r="H198" s="50"/>
+      <c r="I198" s="50"/>
+      <c r="J198" s="50"/>
+      <c r="K198" s="50"/>
+      <c r="L198" s="50"/>
+      <c r="M198" s="50"/>
+      <c r="N198" s="50"/>
+      <c r="O198" s="50"/>
+      <c r="P198" s="50"/>
+      <c r="Q198" s="50"/>
+      <c r="R198" s="50"/>
+    </row>
+    <row r="199" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A199" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="B199" s="59"/>
-      <c r="C199" s="59"/>
-      <c r="D199" s="59"/>
-      <c r="E199" s="59"/>
-      <c r="F199" s="59"/>
-      <c r="G199" s="53"/>
-      <c r="H199" s="51"/>
-      <c r="I199" s="51"/>
-      <c r="J199" s="51"/>
-      <c r="K199" s="51"/>
-      <c r="L199" s="51"/>
-      <c r="M199" s="51"/>
-      <c r="N199" s="51"/>
-      <c r="O199" s="51"/>
-      <c r="P199" s="51"/>
-      <c r="Q199" s="51"/>
+      <c r="B199" s="58"/>
+      <c r="C199" s="58"/>
+      <c r="D199" s="58"/>
+      <c r="E199" s="58"/>
+      <c r="F199" s="58"/>
+      <c r="G199" s="52"/>
+      <c r="H199" s="50"/>
+      <c r="I199" s="50"/>
+      <c r="J199" s="50"/>
+      <c r="K199" s="50"/>
+      <c r="L199" s="50"/>
+      <c r="M199" s="50"/>
+      <c r="N199" s="50"/>
+      <c r="O199" s="50"/>
+      <c r="P199" s="50"/>
+      <c r="Q199" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="B44:B50"/>
     <mergeCell ref="E194:F194"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C61:E61"/>
@@ -4312,11 +4310,13 @@
     <mergeCell ref="A25:A31"/>
     <mergeCell ref="B25:B31"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="B34:B40"/>
-    <mergeCell ref="A16:A22"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="58" fitToHeight="2" orientation="portrait" r:id="rId1"/>
@@ -4340,6 +4340,25 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -4483,25 +4502,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
   <ds:schemaRefs>
@@ -4511,6 +4511,29 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4525,27 +4548,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
1619 Funding Claim Report Template changes to RateBands
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26704CD4-CBD6-48F9-9B61-F27E949A0141}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9B6934-D22F-4337-820A-02F0F0331126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-405" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="149">
   <si>
     <t>Provider :</t>
   </si>
@@ -369,9 +369,6 @@
     <t>1650+ hours (Band 9)</t>
   </si>
   <si>
-    <t>All students</t>
-  </si>
-  <si>
     <t>1500 to 1649 hours (Band 8)</t>
   </si>
   <si>
@@ -466,6 +463,21 @@
   </si>
   <si>
     <t>&amp;=FundingClaim.FundingFactor.PrvHistL3ProgMathEngProp</t>
+  </si>
+  <si>
+    <t>All T Level Students</t>
+  </si>
+  <si>
+    <t>1650 hours (T Level Band 9)</t>
+  </si>
+  <si>
+    <t>1500 hours (T Level Band 8)</t>
+  </si>
+  <si>
+    <t>1300 hours (T Level Band 7)</t>
+  </si>
+  <si>
+    <t>1100 hours (T Level Band 6)</t>
   </si>
 </sst>
 </file>
@@ -931,20 +943,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -954,6 +952,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -961,6 +963,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2378,7 +2390,7 @@
   <dimension ref="A1:R104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -2478,11 +2490,11 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="80"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -2498,10 +2510,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -2515,10 +2527,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -2528,10 +2540,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="25.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2541,10 +2553,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2554,10 +2566,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -2567,12 +2579,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2606,10 +2618,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2623,8 +2635,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2636,8 +2648,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2649,8 +2661,8 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2664,8 +2676,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2679,8 +2691,8 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A23" s="77"/>
-      <c r="B23" s="77"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2694,8 +2706,8 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A24" s="78"/>
-      <c r="B24" s="78"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2740,10 +2752,10 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="72" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2761,8 +2773,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2778,8 +2790,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A29" s="77"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2795,8 +2807,8 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2812,8 +2824,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2829,8 +2841,8 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2846,8 +2858,8 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A33" s="78"/>
-      <c r="B33" s="78"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2895,10 +2907,10 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="76" t="s">
+      <c r="A36" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2916,8 +2928,8 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A37" s="77"/>
-      <c r="B37" s="77"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2933,8 +2945,8 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="73"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2950,8 +2962,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="73"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2967,8 +2979,8 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -2984,8 +2996,8 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3001,8 +3013,8 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A42" s="78"/>
-      <c r="B42" s="78"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="74"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3061,10 +3073,10 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="76" t="s">
+      <c r="A46" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="76" t="s">
+      <c r="B46" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3082,8 +3094,8 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A47" s="77"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3099,8 +3111,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A48" s="77"/>
-      <c r="B48" s="77"/>
+      <c r="A48" s="73"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3116,8 +3128,8 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A49" s="77"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3133,8 +3145,8 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A50" s="77"/>
-      <c r="B50" s="77"/>
+      <c r="A50" s="73"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3150,8 +3162,8 @@
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A51" s="77"/>
-      <c r="B51" s="77"/>
+      <c r="A51" s="73"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3167,8 +3179,8 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A52" s="78"/>
-      <c r="B52" s="78"/>
+      <c r="A52" s="74"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3324,11 +3336,11 @@
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="73" t="s">
+      <c r="C63" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="80"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
@@ -3342,8 +3354,8 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
+      <c r="D64" s="81"/>
+      <c r="E64" s="81"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
@@ -3354,11 +3366,11 @@
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="74" t="s">
+      <c r="C65" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="81"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
@@ -3369,11 +3381,11 @@
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="74" t="s">
+      <c r="C66" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="81"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
@@ -3384,11 +3396,11 @@
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="74" t="s">
+      <c r="C67" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
+      <c r="D67" s="81"/>
+      <c r="E67" s="81"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
@@ -3399,11 +3411,11 @@
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="74" t="s">
+      <c r="C68" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
+      <c r="D68" s="81"/>
+      <c r="E68" s="81"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
@@ -3414,11 +3426,11 @@
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="74" t="s">
+      <c r="C69" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
+      <c r="D69" s="81"/>
+      <c r="E69" s="81"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
@@ -3696,10 +3708,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="72" t="s">
+      <c r="E99" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="72"/>
+      <c r="F99" s="79"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3832,15 +3844,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3854,14 +3865,15 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3880,7 +3892,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B29"/>
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -3980,10 +3992,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="79"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -4000,10 +4012,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -4017,10 +4029,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -4030,10 +4042,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="25.35" x14ac:dyDescent="0.4">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -4043,10 +4055,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -4056,10 +4068,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -4069,12 +4081,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4108,56 +4120,56 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -4166,8 +4178,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A22" s="78"/>
-      <c r="B22" s="78"/>
+      <c r="A22" s="74"/>
+      <c r="B22" s="74"/>
       <c r="C22" s="11" t="s">
         <v>29</v>
       </c>
@@ -4212,20 +4224,20 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="76" t="s">
+      <c r="A25" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="72" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D25" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="67" t="s">
         <v>120</v>
-      </c>
-      <c r="E25" s="67" t="s">
-        <v>121</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
@@ -4233,16 +4245,16 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
+      <c r="A26" s="73"/>
+      <c r="B26" s="73"/>
       <c r="C26" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D26" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="68" t="s">
         <v>126</v>
-      </c>
-      <c r="E26" s="68" t="s">
-        <v>127</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
@@ -4250,16 +4262,16 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D27" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="68" t="s">
         <v>132</v>
-      </c>
-      <c r="E27" s="68" t="s">
-        <v>133</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -4267,16 +4279,16 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D28" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="68" t="s">
         <v>138</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>139</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -4284,8 +4296,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A29" s="78"/>
-      <c r="B29" s="78"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
@@ -4333,20 +4345,20 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="76" t="s">
+      <c r="A32" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D32" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="67" t="s">
         <v>122</v>
-      </c>
-      <c r="E32" s="67" t="s">
-        <v>123</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
@@ -4354,16 +4366,16 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D33" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="68" t="s">
         <v>128</v>
-      </c>
-      <c r="E33" s="68" t="s">
-        <v>129</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
@@ -4371,16 +4383,16 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D34" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="68" t="s">
         <v>134</v>
-      </c>
-      <c r="E34" s="68" t="s">
-        <v>135</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -4388,16 +4400,16 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D35" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E35" s="68" t="s">
         <v>140</v>
-      </c>
-      <c r="E35" s="68" t="s">
-        <v>141</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
@@ -4405,8 +4417,8 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A36" s="78"/>
-      <c r="B36" s="78"/>
+      <c r="A36" s="74"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="11" t="s">
         <v>29</v>
       </c>
@@ -4465,20 +4477,20 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="76" t="s">
+      <c r="A40" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="76" t="s">
+      <c r="B40" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D40" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" s="67" t="s">
         <v>124</v>
-      </c>
-      <c r="E40" s="67" t="s">
-        <v>125</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
@@ -4486,16 +4498,16 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D41" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="67" t="s">
         <v>130</v>
-      </c>
-      <c r="E41" s="67" t="s">
-        <v>131</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
@@ -4503,16 +4515,16 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
+      <c r="A42" s="73"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D42" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="67" t="s">
         <v>136</v>
-      </c>
-      <c r="E42" s="67" t="s">
-        <v>137</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
@@ -4520,16 +4532,16 @@
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A43" s="77"/>
-      <c r="B43" s="77"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="73"/>
       <c r="C43" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D43" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" s="67" t="s">
         <v>142</v>
-      </c>
-      <c r="E43" s="67" t="s">
-        <v>143</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
@@ -4537,8 +4549,8 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A44" s="78"/>
-      <c r="B44" s="78"/>
+      <c r="A44" s="74"/>
+      <c r="B44" s="74"/>
       <c r="C44" s="11" t="s">
         <v>29</v>
       </c>
@@ -4625,11 +4637,11 @@
         <v>5</v>
       </c>
       <c r="B50" s="75"/>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
       <c r="F50" s="31" t="s">
         <v>4</v>
       </c>
@@ -4637,14 +4649,14 @@
     </row>
     <row r="51" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="70" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="B51" s="71"/>
       <c r="C51" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
+        <v>144</v>
+      </c>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
       <c r="F51" s="23">
         <v>6108</v>
       </c>
@@ -4652,14 +4664,14 @@
     </row>
     <row r="52" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="70" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="B52" s="71"/>
       <c r="C52" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
+        <v>144</v>
+      </c>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
       <c r="F52" s="23">
         <v>5584</v>
       </c>
@@ -4667,14 +4679,14 @@
     </row>
     <row r="53" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="70" t="s">
-        <v>114</v>
+        <v>147</v>
       </c>
       <c r="B53" s="71"/>
       <c r="C53" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
+        <v>144</v>
+      </c>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
       <c r="F53" s="23">
         <v>5061</v>
       </c>
@@ -4682,14 +4694,14 @@
     </row>
     <row r="54" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="70" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="B54" s="71"/>
       <c r="C54" s="75" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
+        <v>144</v>
+      </c>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
       <c r="F54" s="23">
         <v>4363</v>
       </c>
@@ -5084,10 +5096,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E97" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="72"/>
+      <c r="F97" s="79"/>
       <c r="G97" s="49"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
@@ -5220,6 +5232,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
     <mergeCell ref="E97:F97"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5236,12 +5254,6 @@
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -6196,10 +6208,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E97" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="72"/>
+      <c r="F97" s="79"/>
       <c r="G97" s="49"/>
     </row>
     <row r="98" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
@@ -6400,6 +6412,34 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6543,35 +6583,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6586,35 +6629,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
More 1619 Funding Claim Template tweaks - Cosmetic
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9B6934-D22F-4337-820A-02F0F0331126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B17C6FB-42D0-4E8E-BD74-185CB967F691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="146">
   <si>
     <t>Provider :</t>
   </si>
@@ -367,15 +367,6 @@
   </si>
   <si>
     <t>1650+ hours (Band 9)</t>
-  </si>
-  <si>
-    <t>1500 to 1649 hours (Band 8)</t>
-  </si>
-  <si>
-    <t>1300 to 1499 hours (Band 7)</t>
-  </si>
-  <si>
-    <t>1100 to 1299 hours (Band 6)</t>
   </si>
   <si>
     <t>&amp;=FundingClaim.DirectFundingStudents.Band9StudentNumbers</t>
@@ -943,6 +934,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -952,10 +957,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -963,16 +964,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2490,11 +2481,11 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -2510,10 +2501,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -2527,10 +2518,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -2540,10 +2531,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="25.35" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2553,10 +2544,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2566,10 +2557,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -2579,12 +2570,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2618,10 +2609,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2635,8 +2626,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2648,8 +2639,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2661,8 +2652,8 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2676,8 +2667,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2691,8 +2682,8 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A23" s="73"/>
-      <c r="B23" s="73"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2706,8 +2697,8 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2752,10 +2743,10 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2773,8 +2764,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2790,8 +2781,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2807,8 +2798,8 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2824,8 +2815,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2841,8 +2832,8 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2858,8 +2849,8 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2907,10 +2898,10 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="72" t="s">
+      <c r="A36" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2928,8 +2919,8 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2945,8 +2936,8 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2962,8 +2953,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A39" s="73"/>
-      <c r="B39" s="73"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2979,8 +2970,8 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A40" s="73"/>
-      <c r="B40" s="73"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -2996,8 +2987,8 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3013,8 +3004,8 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3073,10 +3064,10 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3094,8 +3085,8 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3111,8 +3102,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A48" s="73"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3128,8 +3119,8 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3145,8 +3136,8 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A50" s="73"/>
-      <c r="B50" s="73"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3162,8 +3153,8 @@
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A51" s="73"/>
-      <c r="B51" s="73"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3179,8 +3170,8 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A52" s="74"/>
-      <c r="B52" s="74"/>
+      <c r="A52" s="78"/>
+      <c r="B52" s="78"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3336,11 +3327,11 @@
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="80" t="s">
+      <c r="C63" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="80"/>
-      <c r="E63" s="80"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
@@ -3354,8 +3345,8 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="81"/>
-      <c r="E64" s="81"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
@@ -3366,11 +3357,11 @@
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="81" t="s">
+      <c r="C65" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
@@ -3381,11 +3372,11 @@
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="81" t="s">
+      <c r="C66" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
@@ -3396,11 +3387,11 @@
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="81" t="s">
+      <c r="C67" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="81"/>
-      <c r="E67" s="81"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
@@ -3411,11 +3402,11 @@
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="81" t="s">
+      <c r="C68" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
@@ -3426,11 +3417,11 @@
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
@@ -3708,10 +3699,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="79" t="s">
+      <c r="E99" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="79"/>
+      <c r="F99" s="72"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3844,14 +3835,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3865,15 +3857,14 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3892,7 +3883,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -3992,10 +3983,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -4012,10 +4003,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -4029,10 +4020,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -4042,10 +4033,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="25.35" x14ac:dyDescent="0.4">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -4055,10 +4046,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -4068,10 +4059,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -4081,12 +4072,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4120,56 +4111,56 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -4178,8 +4169,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="11" t="s">
         <v>29</v>
       </c>
@@ -4224,20 +4215,20 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D25" s="66" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E25" s="67" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
@@ -4245,16 +4236,16 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="11" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E26" s="68" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
@@ -4262,16 +4253,16 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="11" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -4279,16 +4270,16 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -4296,8 +4287,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A29" s="74"/>
-      <c r="B29" s="74"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
@@ -4345,20 +4336,20 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D32" s="66" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E32" s="67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
@@ -4366,16 +4357,16 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A33" s="73"/>
-      <c r="B33" s="73"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="11" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E33" s="68" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
@@ -4383,16 +4374,16 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A34" s="73"/>
-      <c r="B34" s="73"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="11" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E34" s="68" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -4400,16 +4391,16 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="41" x14ac:dyDescent="0.4">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="11" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E35" s="68" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
@@ -4417,8 +4408,8 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
+      <c r="A36" s="78"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="11" t="s">
         <v>29</v>
       </c>
@@ -4477,20 +4468,20 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="72" t="s">
+      <c r="A40" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>111</v>
       </c>
       <c r="D40" s="66" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E40" s="67" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
@@ -4498,16 +4489,16 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E41" s="67" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
@@ -4515,16 +4506,16 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A42" s="73"/>
-      <c r="B42" s="73"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="11" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E42" s="67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
@@ -4532,16 +4523,16 @@
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
-      <c r="A43" s="73"/>
-      <c r="B43" s="73"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="11" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
@@ -4549,8 +4540,8 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
-      <c r="A44" s="74"/>
-      <c r="B44" s="74"/>
+      <c r="A44" s="78"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="11" t="s">
         <v>29</v>
       </c>
@@ -4637,11 +4628,11 @@
         <v>5</v>
       </c>
       <c r="B50" s="75"/>
-      <c r="C50" s="80" t="s">
+      <c r="C50" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
       <c r="F50" s="31" t="s">
         <v>4</v>
       </c>
@@ -4649,14 +4640,14 @@
     </row>
     <row r="51" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="70" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B51" s="71"/>
       <c r="C51" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
+        <v>141</v>
+      </c>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
       <c r="F51" s="23">
         <v>6108</v>
       </c>
@@ -4664,14 +4655,14 @@
     </row>
     <row r="52" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="70" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B52" s="71"/>
       <c r="C52" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="D52" s="81"/>
-      <c r="E52" s="81"/>
+        <v>141</v>
+      </c>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
       <c r="F52" s="23">
         <v>5584</v>
       </c>
@@ -4679,14 +4670,14 @@
     </row>
     <row r="53" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="70" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B53" s="71"/>
       <c r="C53" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" s="81"/>
-      <c r="E53" s="81"/>
+        <v>141</v>
+      </c>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
       <c r="F53" s="23">
         <v>5061</v>
       </c>
@@ -4694,14 +4685,14 @@
     </row>
     <row r="54" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="70" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B54" s="71"/>
       <c r="C54" s="75" t="s">
-        <v>144</v>
-      </c>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
+        <v>141</v>
+      </c>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
       <c r="F54" s="23">
         <v>4363</v>
       </c>
@@ -5096,10 +5087,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
@@ -5232,12 +5223,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
     <mergeCell ref="E97:F97"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5254,6 +5239,12 @@
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -6208,10 +6199,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
     </row>
     <row r="98" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
@@ -6412,34 +6403,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6583,15 +6546,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6606,27 +6614,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated row heights on template
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B17C6FB-42D0-4E8E-BD74-185CB967F691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9C0BC6-9EC7-4A14-9801-5234A1B453C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12840" yWindow="9507" windowWidth="25787" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -2381,22 +2381,22 @@
   <dimension ref="A1:R104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="39" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.64453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.41015625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1171875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.234375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -2410,7 +2410,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2419,7 +2419,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2432,7 +2432,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2471,7 +2471,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2480,7 +2480,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>108</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2500,7 +2500,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
@@ -2530,7 +2530,7 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="25.35" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
@@ -2540,10 +2540,10 @@
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
@@ -2556,7 +2556,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
@@ -2569,7 +2569,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
@@ -2582,7 +2582,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2591,7 +2591,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -2608,7 +2608,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
@@ -2625,7 +2625,7 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="77"/>
       <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
@@ -2638,7 +2638,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="77"/>
       <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
@@ -2651,7 +2651,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77"/>
       <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
@@ -2666,7 +2666,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="77"/>
       <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
@@ -2681,7 +2681,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="77"/>
       <c r="B23" s="77"/>
       <c r="C23" s="43" t="s">
@@ -2696,7 +2696,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="78"/>
       <c r="B24" s="78"/>
       <c r="C24" s="11" t="s">
@@ -2712,7 +2712,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2723,7 +2723,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -2742,7 +2742,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="76" t="s">
         <v>16</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="77"/>
       <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
@@ -2780,7 +2780,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="77"/>
       <c r="B29" s="77"/>
       <c r="C29" s="11" t="s">
@@ -2797,7 +2797,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="77"/>
       <c r="B30" s="77"/>
       <c r="C30" s="11" t="s">
@@ -2814,7 +2814,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="77"/>
       <c r="B31" s="77"/>
       <c r="C31" s="11" t="s">
@@ -2831,7 +2831,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="77"/>
       <c r="B32" s="77"/>
       <c r="C32" s="11" t="s">
@@ -2848,7 +2848,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="78"/>
       <c r="B33" s="78"/>
       <c r="C33" s="11" t="s">
@@ -2867,7 +2867,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -2878,7 +2878,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -2897,7 +2897,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="76" t="s">
         <v>17</v>
       </c>
@@ -2918,7 +2918,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="77"/>
       <c r="B37" s="77"/>
       <c r="C37" s="11" t="s">
@@ -2935,7 +2935,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="77"/>
       <c r="B38" s="77"/>
       <c r="C38" s="11" t="s">
@@ -2952,7 +2952,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="77"/>
       <c r="B39" s="77"/>
       <c r="C39" s="11" t="s">
@@ -2969,7 +2969,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="77"/>
       <c r="B40" s="77"/>
       <c r="C40" s="11" t="s">
@@ -2986,7 +2986,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="77"/>
       <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
@@ -3003,7 +3003,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="78"/>
       <c r="B42" s="78"/>
       <c r="C42" s="11" t="s">
@@ -3022,7 +3022,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
@@ -3033,7 +3033,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3044,7 +3044,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -3063,7 +3063,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="76" t="s">
         <v>18</v>
       </c>
@@ -3084,7 +3084,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="77"/>
       <c r="B47" s="77"/>
       <c r="C47" s="11" t="s">
@@ -3101,7 +3101,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="77"/>
       <c r="B48" s="77"/>
       <c r="C48" s="11" t="s">
@@ -3118,7 +3118,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="77"/>
       <c r="B49" s="77"/>
       <c r="C49" s="11" t="s">
@@ -3135,7 +3135,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="77"/>
       <c r="B50" s="77"/>
       <c r="C50" s="11" t="s">
@@ -3152,7 +3152,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="77"/>
       <c r="B51" s="77"/>
       <c r="C51" s="11" t="s">
@@ -3169,7 +3169,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="78"/>
       <c r="B52" s="78"/>
       <c r="C52" s="11" t="s">
@@ -3188,7 +3188,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="20"/>
@@ -3199,7 +3199,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A54" s="19"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
@@ -3210,7 +3210,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A55" s="19"/>
       <c r="B55" s="19"/>
       <c r="C55" s="11" t="s">
@@ -3235,7 +3235,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20"/>
@@ -3246,7 +3246,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11" t="s">
@@ -3261,7 +3261,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="20"/>
@@ -3272,7 +3272,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="19"/>
       <c r="C59" s="11" t="s">
@@ -3295,7 +3295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A60" s="19"/>
       <c r="B60" s="19"/>
       <c r="C60" s="20"/>
@@ -3304,7 +3304,7 @@
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
     </row>
-    <row r="61" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A61" s="19"/>
       <c r="B61" s="19"/>
       <c r="C61" s="20"/>
@@ -3313,7 +3313,7 @@
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>
     </row>
-    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -3322,7 +3322,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="75" t="s">
         <v>5</v>
       </c>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A64" s="75" t="s">
         <v>10</v>
       </c>
@@ -3352,7 +3352,7 @@
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A65" s="75" t="s">
         <v>11</v>
       </c>
@@ -3367,7 +3367,7 @@
       </c>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A66" s="75" t="s">
         <v>12</v>
       </c>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A67" s="75" t="s">
         <v>13</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A68" s="75" t="s">
         <v>14</v>
       </c>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A69" s="75" t="s">
         <v>15</v>
       </c>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A70" s="38"/>
       <c r="B70" s="38"/>
       <c r="C70" s="39"/>
@@ -3436,7 +3436,7 @@
       <c r="F70" s="40"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -3445,7 +3445,7 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -3454,7 +3454,7 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -3463,7 +3463,7 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -3472,7 +3472,7 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -3481,7 +3481,7 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -3490,7 +3490,7 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -3499,7 +3499,7 @@
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -3508,7 +3508,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -3517,7 +3517,7 @@
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -3526,7 +3526,7 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -3535,7 +3535,7 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
     </row>
-    <row r="82" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -3544,7 +3544,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -3553,7 +3553,7 @@
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -3562,7 +3562,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -3571,7 +3571,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -3580,7 +3580,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -3589,7 +3589,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -3598,7 +3598,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -3607,7 +3607,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -3616,7 +3616,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -3625,7 +3625,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -3634,7 +3634,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -3643,7 +3643,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3652,7 +3652,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3661,7 +3661,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3670,7 +3670,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -3679,7 +3679,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3688,7 +3688,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="59" t="s">
         <v>45</v>
       </c>
@@ -3716,7 +3716,7 @@
       <c r="Q99" s="50"/>
       <c r="R99" s="50"/>
     </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A100" s="60" t="s">
         <v>46</v>
       </c>
@@ -3744,7 +3744,7 @@
       <c r="Q100" s="50"/>
       <c r="R100" s="50"/>
     </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D101" s="61" t="s">
         <v>32</v>
       </c>
@@ -3765,7 +3765,7 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A102" s="62"/>
       <c r="B102" s="62"/>
       <c r="C102" s="63"/>
@@ -3789,7 +3789,7 @@
       <c r="Q102" s="50"/>
       <c r="R102" s="50"/>
     </row>
-    <row r="103" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B103" s="60"/>
       <c r="C103" s="60"/>
       <c r="D103" s="64" t="s">
@@ -3812,7 +3812,7 @@
       <c r="Q103" s="50"/>
       <c r="R103" s="50"/>
     </row>
-    <row r="104" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A104" s="60" t="s">
         <v>54</v>
       </c>
@@ -3883,22 +3883,22 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C40" sqref="A40:XFD44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.76171875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.41015625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1171875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.234375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -3912,7 +3912,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3921,7 +3921,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -3934,7 +3934,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -3947,7 +3947,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -3973,7 +3973,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -3982,7 +3982,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A8" s="79" t="s">
         <v>109</v>
       </c>
@@ -3993,7 +3993,7 @@
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -4002,7 +4002,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
@@ -4032,7 +4032,7 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="25.35" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
@@ -4045,7 +4045,7 @@
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
@@ -4058,7 +4058,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
@@ -4071,7 +4071,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
@@ -4084,7 +4084,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="12.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4093,7 +4093,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4110,7 +4110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
@@ -4127,7 +4127,7 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="77"/>
       <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
@@ -4140,7 +4140,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="77"/>
       <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
@@ -4153,7 +4153,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="77"/>
       <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
@@ -4168,7 +4168,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="78"/>
       <c r="B22" s="78"/>
       <c r="C22" s="11" t="s">
@@ -4184,7 +4184,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -4195,7 +4195,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -4214,7 +4214,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="76" t="s">
         <v>16</v>
       </c>
@@ -4235,7 +4235,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="77"/>
       <c r="B26" s="77"/>
       <c r="C26" s="11" t="s">
@@ -4252,7 +4252,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="77"/>
       <c r="B27" s="77"/>
       <c r="C27" s="11" t="s">
@@ -4269,7 +4269,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="77"/>
       <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
@@ -4286,7 +4286,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="78"/>
       <c r="B29" s="78"/>
       <c r="C29" s="11" t="s">
@@ -4305,7 +4305,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -4316,7 +4316,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -4335,7 +4335,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="76" t="s">
         <v>17</v>
       </c>
@@ -4356,7 +4356,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="77"/>
       <c r="B33" s="77"/>
       <c r="C33" s="11" t="s">
@@ -4373,7 +4373,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="77"/>
       <c r="B34" s="77"/>
       <c r="C34" s="11" t="s">
@@ -4390,7 +4390,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="77"/>
       <c r="B35" s="77"/>
       <c r="C35" s="11" t="s">
@@ -4407,7 +4407,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="78"/>
       <c r="B36" s="78"/>
       <c r="C36" s="11" t="s">
@@ -4426,7 +4426,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
@@ -4437,7 +4437,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -4448,7 +4448,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -4467,7 +4467,7 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="76" t="s">
         <v>18</v>
       </c>
@@ -4488,7 +4488,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="77"/>
       <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
@@ -4505,7 +4505,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="77"/>
       <c r="B42" s="77"/>
       <c r="C42" s="11" t="s">
@@ -4522,7 +4522,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="54.7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="77"/>
       <c r="B43" s="77"/>
       <c r="C43" s="11" t="s">
@@ -4539,7 +4539,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="78"/>
       <c r="B44" s="78"/>
       <c r="C44" s="11" t="s">
@@ -4558,7 +4558,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="20"/>
@@ -4569,7 +4569,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
       <c r="C46" s="20"/>
@@ -4580,7 +4580,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
       <c r="C47" s="11" t="s">
@@ -4605,7 +4605,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
@@ -4614,7 +4614,7 @@
       <c r="F48" s="37"/>
       <c r="G48" s="37"/>
     </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -4623,7 +4623,7 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="75" t="s">
         <v>5</v>
       </c>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="70" t="s">
         <v>142</v>
       </c>
@@ -4653,7 +4653,7 @@
       </c>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="70" t="s">
         <v>143</v>
       </c>
@@ -4668,7 +4668,7 @@
       </c>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="70" t="s">
         <v>144</v>
       </c>
@@ -4683,7 +4683,7 @@
       </c>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="70" t="s">
         <v>145</v>
       </c>
@@ -4698,7 +4698,7 @@
       </c>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A55" s="38"/>
       <c r="B55" s="38"/>
       <c r="C55" s="39"/>
@@ -4707,7 +4707,7 @@
       <c r="F55" s="40"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -4716,7 +4716,7 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -4725,7 +4725,7 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -4734,7 +4734,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -4743,7 +4743,7 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -4752,7 +4752,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -4761,7 +4761,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -4770,7 +4770,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -4779,7 +4779,7 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -4788,7 +4788,7 @@
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -4797,7 +4797,7 @@
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -4806,7 +4806,7 @@
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -4815,7 +4815,7 @@
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -4824,7 +4824,7 @@
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -4833,7 +4833,7 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -4842,7 +4842,7 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -4851,7 +4851,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -4860,7 +4860,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -4869,7 +4869,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -4878,7 +4878,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -4887,7 +4887,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -4896,7 +4896,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -4905,7 +4905,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -4914,7 +4914,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -4923,7 +4923,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -4932,7 +4932,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -4941,7 +4941,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -4950,7 +4950,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -4959,7 +4959,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -4968,7 +4968,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -4977,7 +4977,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -4986,7 +4986,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -4995,7 +4995,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -5004,7 +5004,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -5013,7 +5013,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -5022,7 +5022,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -5031,7 +5031,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" ht="11.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" ht="11.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -5040,7 +5040,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -5049,7 +5049,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -5058,7 +5058,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -5067,7 +5067,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -5076,7 +5076,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="59" t="s">
         <v>45</v>
       </c>
@@ -5104,7 +5104,7 @@
       <c r="Q97" s="50"/>
       <c r="R97" s="50"/>
     </row>
-    <row r="98" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A98" s="60" t="s">
         <v>46</v>
       </c>
@@ -5132,7 +5132,7 @@
       <c r="Q98" s="50"/>
       <c r="R98" s="50"/>
     </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="D99" s="61" t="s">
         <v>32</v>
       </c>
@@ -5153,7 +5153,7 @@
       <c r="Q99" s="50"/>
       <c r="R99" s="50"/>
     </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A100" s="62"/>
       <c r="B100" s="62"/>
       <c r="C100" s="63"/>
@@ -5177,7 +5177,7 @@
       <c r="Q100" s="50"/>
       <c r="R100" s="50"/>
     </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B101" s="60"/>
       <c r="C101" s="60"/>
       <c r="D101" s="64" t="s">
@@ -5200,7 +5200,7 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A102" s="60" t="s">
         <v>54</v>
       </c>
@@ -5261,19 +5261,19 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.1171875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.41015625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1171875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.234375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.21875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -5287,7 +5287,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5296,7 +5296,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -5309,7 +5309,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -5322,7 +5322,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -5348,7 +5348,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -5357,7 +5357,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -5368,7 +5368,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5379,7 +5379,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5390,7 +5390,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -5401,7 +5401,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -5412,7 +5412,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5423,7 +5423,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -5434,7 +5434,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -5445,7 +5445,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5456,7 +5456,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5467,7 +5467,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5478,7 +5478,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5489,7 +5489,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -5500,7 +5500,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -5511,7 +5511,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -5522,7 +5522,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -5531,7 +5531,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -5540,7 +5540,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -5549,7 +5549,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -5558,7 +5558,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -5567,7 +5567,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -5576,7 +5576,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5585,7 +5585,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -5594,7 +5594,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -5603,7 +5603,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -5612,7 +5612,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -5621,7 +5621,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -5630,7 +5630,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -5639,7 +5639,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -5648,7 +5648,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -5657,7 +5657,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -5666,7 +5666,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -5675,7 +5675,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -5684,7 +5684,7 @@
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -5693,7 +5693,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -5702,7 +5702,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -5711,7 +5711,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -5720,7 +5720,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -5729,7 +5729,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -5738,7 +5738,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -5747,7 +5747,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -5756,7 +5756,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -5765,7 +5765,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -5774,7 +5774,7 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -5783,7 +5783,7 @@
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -5792,7 +5792,7 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -5801,7 +5801,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -5810,7 +5810,7 @@
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -5819,7 +5819,7 @@
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -5828,7 +5828,7 @@
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -5837,7 +5837,7 @@
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -5846,7 +5846,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -5855,7 +5855,7 @@
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -5864,7 +5864,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -5873,7 +5873,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -5882,7 +5882,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -5891,7 +5891,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -5900,7 +5900,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -5909,7 +5909,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -5918,7 +5918,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -5927,7 +5927,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -5936,7 +5936,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -5945,7 +5945,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -5954,7 +5954,7 @@
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -5963,7 +5963,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -5972,7 +5972,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -5981,7 +5981,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -5990,7 +5990,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -5999,7 +5999,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -6008,7 +6008,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -6017,7 +6017,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -6026,7 +6026,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -6035,7 +6035,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -6044,7 +6044,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -6053,7 +6053,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -6062,7 +6062,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -6071,7 +6071,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -6080,7 +6080,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -6089,7 +6089,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -6098,7 +6098,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -6107,7 +6107,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -6116,7 +6116,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -6125,7 +6125,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -6134,7 +6134,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -6143,7 +6143,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -6152,7 +6152,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -6161,7 +6161,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -6170,7 +6170,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -6179,7 +6179,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -6188,7 +6188,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A97" s="59" t="s">
         <v>45</v>
       </c>
@@ -6205,7 +6205,7 @@
       <c r="F97" s="72"/>
       <c r="G97" s="49"/>
     </row>
-    <row r="98" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A98" s="60" t="s">
         <v>46</v>
       </c>
@@ -6222,7 +6222,7 @@
       <c r="F98" s="60"/>
       <c r="G98" s="58"/>
     </row>
-    <row r="99" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A99" s="51"/>
       <c r="B99" s="51"/>
       <c r="C99" s="51"/>
@@ -6235,7 +6235,7 @@
       <c r="F99" s="60"/>
       <c r="G99" s="53"/>
     </row>
-    <row r="100" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A100" s="62"/>
       <c r="B100" s="62"/>
       <c r="C100" s="63"/>
@@ -6248,7 +6248,7 @@
       <c r="F100" s="60"/>
       <c r="G100" s="53"/>
     </row>
-    <row r="101" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A101" s="51"/>
       <c r="B101" s="60"/>
       <c r="C101" s="60"/>
@@ -6261,7 +6261,7 @@
       <c r="F101" s="60"/>
       <c r="G101" s="53"/>
     </row>
-    <row r="102" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A102" s="60" t="s">
         <v>54</v>
       </c>
@@ -6272,8 +6272,8 @@
       <c r="F102" s="58"/>
       <c r="G102" s="52"/>
     </row>
-    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -6293,7 +6293,7 @@
       <c r="Q148" s="50"/>
       <c r="R148" s="50"/>
     </row>
-    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -6313,7 +6313,7 @@
       <c r="Q149" s="50"/>
       <c r="R149" s="50"/>
     </row>
-    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -6333,7 +6333,7 @@
       <c r="Q150" s="50"/>
       <c r="R150" s="50"/>
     </row>
-    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -6353,7 +6353,7 @@
       <c r="Q151" s="50"/>
       <c r="R151" s="50"/>
     </row>
-    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -6373,7 +6373,7 @@
       <c r="Q152" s="50"/>
       <c r="R152" s="50"/>
     </row>
-    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>

</xml_diff>

<commit_message>
#102371 - T Level Band Description fix
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF42A43F-C94D-4418-B61A-697D07F5B894}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39449D80-908B-414D-8754-5AB446ED5C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,9 +366,6 @@
     <t>Level 3 Programme Maths and English Proportion (allocation) %</t>
   </si>
   <si>
-    <t>1650+ hours (Band 9)</t>
-  </si>
-  <si>
     <t>&amp;=FundingClaim.DirectFundingStudents.Band9StudentNumbers</t>
   </si>
   <si>
@@ -469,6 +466,9 @@
   </si>
   <si>
     <t>1100 hours (T Level Band 6)</t>
+  </si>
+  <si>
+    <t>1650+ hours (T Level Band 9)</t>
   </si>
 </sst>
 </file>
@@ -934,6 +934,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -943,10 +957,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -954,16 +964,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2481,11 +2481,11 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -2501,10 +2501,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -2518,10 +2518,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -2531,10 +2531,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2544,10 +2544,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2557,10 +2557,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -2570,12 +2570,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2609,10 +2609,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2626,8 +2626,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2639,8 +2639,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2652,8 +2652,8 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2667,8 +2667,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2682,8 +2682,8 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="73"/>
-      <c r="B23" s="73"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2697,8 +2697,8 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2743,10 +2743,10 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2764,8 +2764,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2781,8 +2781,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2798,8 +2798,8 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2815,8 +2815,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2832,8 +2832,8 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2849,8 +2849,8 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2898,10 +2898,10 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="72" t="s">
+      <c r="A36" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2919,8 +2919,8 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2936,8 +2936,8 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2953,8 +2953,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="73"/>
-      <c r="B39" s="73"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2970,8 +2970,8 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="73"/>
-      <c r="B40" s="73"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -2987,8 +2987,8 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3004,8 +3004,8 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3064,10 +3064,10 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3085,8 +3085,8 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3102,8 +3102,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="73"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3119,8 +3119,8 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3136,8 +3136,8 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="73"/>
-      <c r="B50" s="73"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3153,8 +3153,8 @@
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="73"/>
-      <c r="B51" s="73"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3170,8 +3170,8 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="74"/>
-      <c r="B52" s="74"/>
+      <c r="A52" s="78"/>
+      <c r="B52" s="78"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3327,11 +3327,11 @@
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="80" t="s">
+      <c r="C63" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="80"/>
-      <c r="E63" s="80"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
@@ -3345,8 +3345,8 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="81"/>
-      <c r="E64" s="81"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
@@ -3357,11 +3357,11 @@
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="81" t="s">
+      <c r="C65" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
@@ -3372,11 +3372,11 @@
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="81" t="s">
+      <c r="C66" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
@@ -3387,11 +3387,11 @@
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="81" t="s">
+      <c r="C67" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="81"/>
-      <c r="E67" s="81"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
@@ -3402,11 +3402,11 @@
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="81" t="s">
+      <c r="C68" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
@@ -3417,11 +3417,11 @@
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
@@ -3699,10 +3699,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="79" t="s">
+      <c r="E99" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="79"/>
+      <c r="F99" s="72"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3835,14 +3835,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3856,15 +3857,14 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3883,7 +3883,7 @@
   <dimension ref="A1:R102"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="A40:XFD44"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
@@ -3983,10 +3983,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -4003,10 +4003,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -4020,10 +4020,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -4033,10 +4033,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -4046,10 +4046,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -4059,10 +4059,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -4072,12 +4072,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4111,56 +4111,56 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -4169,8 +4169,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="11" t="s">
         <v>29</v>
       </c>
@@ -4215,20 +4215,20 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="72" t="s">
+      <c r="A25" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D25" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="67" t="s">
         <v>116</v>
-      </c>
-      <c r="E25" s="67" t="s">
-        <v>117</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
@@ -4236,16 +4236,16 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D26" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="68" t="s">
         <v>122</v>
-      </c>
-      <c r="E26" s="68" t="s">
-        <v>123</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
@@ -4253,16 +4253,16 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D27" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="E27" s="68" t="s">
         <v>128</v>
-      </c>
-      <c r="E27" s="68" t="s">
-        <v>129</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -4270,16 +4270,16 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D28" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="68" t="s">
         <v>134</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>135</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -4287,8 +4287,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="74"/>
-      <c r="B29" s="74"/>
+      <c r="A29" s="78"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
@@ -4336,20 +4336,20 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="72" t="s">
+      <c r="A32" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D32" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="67" t="s">
         <v>118</v>
-      </c>
-      <c r="E32" s="67" t="s">
-        <v>119</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
@@ -4357,16 +4357,16 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="73"/>
-      <c r="B33" s="73"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D33" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="68" t="s">
         <v>124</v>
-      </c>
-      <c r="E33" s="68" t="s">
-        <v>125</v>
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
@@ -4374,16 +4374,16 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="73"/>
-      <c r="B34" s="73"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D34" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="68" t="s">
         <v>130</v>
-      </c>
-      <c r="E34" s="68" t="s">
-        <v>131</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -4391,16 +4391,16 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D35" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="68" t="s">
         <v>136</v>
-      </c>
-      <c r="E35" s="68" t="s">
-        <v>137</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
@@ -4408,8 +4408,8 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
+      <c r="A36" s="78"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="11" t="s">
         <v>29</v>
       </c>
@@ -4468,20 +4468,20 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="72" t="s">
+      <c r="A40" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D40" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="E40" s="67" t="s">
         <v>120</v>
-      </c>
-      <c r="E40" s="67" t="s">
-        <v>121</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
@@ -4489,16 +4489,16 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D41" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" s="67" t="s">
         <v>126</v>
-      </c>
-      <c r="E41" s="67" t="s">
-        <v>127</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
@@ -4506,16 +4506,16 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="73"/>
-      <c r="B42" s="73"/>
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D42" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="67" t="s">
         <v>132</v>
-      </c>
-      <c r="E42" s="67" t="s">
-        <v>133</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
@@ -4523,16 +4523,16 @@
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="73"/>
-      <c r="B43" s="73"/>
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="67" t="s">
         <v>138</v>
-      </c>
-      <c r="E43" s="67" t="s">
-        <v>139</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
@@ -4540,8 +4540,8 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="74"/>
-      <c r="B44" s="74"/>
+      <c r="A44" s="78"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="11" t="s">
         <v>29</v>
       </c>
@@ -4628,11 +4628,11 @@
         <v>5</v>
       </c>
       <c r="B50" s="75"/>
-      <c r="C50" s="80" t="s">
+      <c r="C50" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
       <c r="F50" s="31" t="s">
         <v>4</v>
       </c>
@@ -4640,14 +4640,14 @@
     </row>
     <row r="51" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B51" s="71"/>
       <c r="C51" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
+        <v>140</v>
+      </c>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
       <c r="F51" s="23">
         <v>6108</v>
       </c>
@@ -4655,14 +4655,14 @@
     </row>
     <row r="52" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B52" s="71"/>
       <c r="C52" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="D52" s="81"/>
-      <c r="E52" s="81"/>
+        <v>140</v>
+      </c>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
       <c r="F52" s="23">
         <v>5584</v>
       </c>
@@ -4670,14 +4670,14 @@
     </row>
     <row r="53" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B53" s="71"/>
       <c r="C53" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="D53" s="81"/>
-      <c r="E53" s="81"/>
+        <v>140</v>
+      </c>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
       <c r="F53" s="23">
         <v>5061</v>
       </c>
@@ -4685,14 +4685,14 @@
     </row>
     <row r="54" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B54" s="71"/>
       <c r="C54" s="75" t="s">
-        <v>141</v>
-      </c>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
+        <v>140</v>
+      </c>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
       <c r="F54" s="23">
         <v>4363</v>
       </c>
@@ -5087,10 +5087,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
@@ -5223,12 +5223,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
     <mergeCell ref="E97:F97"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5245,6 +5239,12 @@
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -6199,10 +6199,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
     </row>
     <row r="98" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
@@ -6403,34 +6403,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6574,15 +6546,60 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6597,27 +6614,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
103079 Funding claim 16-19 footer changes
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853DDF2F-7FF8-4CE4-B146-0FDCE6DC8858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E6F97E-97A2-473C-BFC3-1A0381DC0D82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-8580" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -16,13 +16,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">Declaration!$A$1:$G$104</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'T Levels'!$A$1:$G$104</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -931,6 +933,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -940,10 +956,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -951,16 +963,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1124,6 +1126,27 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>2)     English and maths payment premium will also be added to the outturn based on the percentage of the premium paid within the total programme funding allocation.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPct val="100000"/>
@@ -1149,7 +1172,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>2)     </a:t>
+            <a:t>3)     </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -1181,7 +1204,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>3)     This page includes all students who have 16 to 19 funding and are identified in the ILR as 16 to 19 funded (that is, source of funding code = 107).</a:t>
+            <a:t>4)     This report includes all students who have 16 to 19 funding and are identified in the ILR as 16 to 19 funded (that is, source of funding code = 107).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1202,7 +1225,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>4)     Any students coded as Adult funded (that is, source of funding code = 105) will not appear on this report, even if their funding model is set to 25 (16 to 19 (excluding Apprenticeships) funding).</a:t>
+            <a:t>5)     Any students coded as Adult funded (that is, source of funding code = 105) will not appear on this report, even if their funding model is set to 25 (16 to 19 (excluding Apprenticeships) funding).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1223,7 +1246,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>5)     Row C includes students aged 19 to 24 on 31</a:t>
+            <a:t>6)     Row C includes students aged 19 to 24 on 31</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -1255,7 +1278,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>6)     Row D includes students aged 19 or over on 31 August 2020 </a:t>
+            <a:t>7)     Row D includes students aged 19 or over on 31 August 2020 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -1297,7 +1320,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>7)     All factors displayed in this report and used in funding calculations are those used in your 2020 to 2021 allocation.</a:t>
+            <a:t>8)     All factors displayed in this report and used in funding calculations are those used in your 2020 to 2021 allocation.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1320,7 +1343,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>8)     The 2020 to 2021 condition of funding removal reflects the funding that has been removed from your 2020 to 2021 allocation in relation to students who did not comply with the condition of funding on English and mathematics in 2018 to 2019. The total funding (less condition of funding removal) figure will form the basis of the outturn used for all institutions, to ensure that the outturn and allocation figures are calculated on a consistent basis.</a:t>
+            <a:t>9)     The 2020 to 2021 condition of funding removal reflects the funding that has been removed from your 2020 to 2021 allocation in relation to students who did not comply with the condition of funding on English and mathematics in 2018 to 2019. The total funding (less condition of funding removal) figure will form the basis of the outturn used for all institutions, to ensure that the outturn and allocation figures are calculated on a consistent basis.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1404,6 +1427,27 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>2)     English and maths payment premium will also be added to the outturn based on the percentage of the premium paid within the total programme funding allocation.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
             <a:lnSpc>
               <a:spcPct val="100000"/>
@@ -1429,7 +1473,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>2)     </a:t>
+            <a:t>3)     </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -1461,7 +1505,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>3)     This page includes all students who have 16 to 19 funding and are identified in the ILR as 16 to 19 funded (that is, source of funding code = 107).</a:t>
+            <a:t>4)     This report includes all students who have 16 to 19 funding and are identified in the ILR as 16 to 19 funded (that is, source of funding code = 107).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1482,7 +1526,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>4)     Any students coded as Adult funded (that is, source of funding code = 105) will not appear on this report, even if their funding model is set to 25 (16 to 19 (excluding Apprenticeships) funding).</a:t>
+            <a:t>5)     Any students coded as Adult funded (that is, source of funding code = 105) will not appear on this report, even if their funding model is set to 25 (16 to 19 (excluding Apprenticeships) funding).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1503,7 +1547,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>5)     Row C includes students aged 19 to 24 on 31</a:t>
+            <a:t>6)     Row C includes students aged 19 to 24 on 31</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -1535,7 +1579,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>6)     Row D includes students aged 19 or over on 31 August 2020 </a:t>
+            <a:t>7)     Row D includes students aged 19 or over on 31 August 2020 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
@@ -1577,7 +1621,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>7)     All factors displayed in this report and used in funding calculations are those used in your 2020 to 2021 allocation.</a:t>
+            <a:t>8)     All factors displayed in this report and used in funding calculations are those used in your 2020 to 2021 allocation.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1600,6 +1644,7 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="3" name="TextBox 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16DF0F67-6C4E-4080-AC74-F8C429886670}"/>
@@ -1695,7 +1740,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>The only circumstances in which the ESFA will need the signed 16-19 final claim report (available through FIS or the Data Collections portal) are: </a:t>
+            <a:t>The only circumstances in which the ESFA will need the signed 16-19 final claim report (available through FIS or the Submit Learner Data) are: </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2022,23 +2067,9 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>https://www.gov.uk/guidance/how-to-return-ilr-final-funding-claims-to-the-efa</a:t>
+            <a:t>returning ILR funding claims to the ESFA.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100">
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" u="sng">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -2377,23 +2408,23 @@
   </sheetPr>
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.64453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="39" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.64453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.64453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.41015625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1171875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.234375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -2407,7 +2438,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2416,7 +2447,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2429,7 +2460,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -2442,7 +2473,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -2459,7 +2490,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2468,7 +2499,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2477,18 +2508,18 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="76" t="s">
+    <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2497,11 +2528,11 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="78" t="s">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -2514,11 +2545,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="78" t="s">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -2527,11 +2558,11 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2540,11 +2571,11 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="78" t="s">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2553,11 +2584,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="78" t="s">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -2566,11 +2597,11 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="78" t="s">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -2579,7 +2610,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2588,7 +2619,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -2605,11 +2636,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="72" t="s">
+    <row r="18" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2622,9 +2653,9 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+    <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2635,9 +2666,9 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+    <row r="20" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2648,9 +2679,9 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+    <row r="21" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2663,9 +2694,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+    <row r="22" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2678,9 +2709,9 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="73"/>
-      <c r="B23" s="73"/>
+    <row r="23" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="77"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2693,9 +2724,9 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
+    <row r="24" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="78"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2709,7 +2740,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2720,7 +2751,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -2739,11 +2770,11 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="72" t="s">
+    <row r="27" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2760,9 +2791,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+    <row r="28" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2777,9 +2808,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
+    <row r="29" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2794,9 +2825,9 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
+    <row r="30" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2811,9 +2842,9 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
+    <row r="31" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2828,9 +2859,9 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
+    <row r="32" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2845,9 +2876,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
+    <row r="33" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2864,7 +2895,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -2875,7 +2906,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -2894,11 +2925,11 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="72" t="s">
+    <row r="36" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2915,9 +2946,9 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
+    <row r="37" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2932,9 +2963,9 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
+    <row r="38" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2949,9 +2980,9 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="73"/>
-      <c r="B39" s="73"/>
+    <row r="39" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2966,9 +2997,9 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="73"/>
-      <c r="B40" s="73"/>
+    <row r="40" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -2983,9 +3014,9 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+    <row r="41" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3000,9 +3031,9 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
+    <row r="42" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="78"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3019,7 +3050,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
@@ -3030,7 +3061,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3041,7 +3072,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -3060,11 +3091,11 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="72" t="s">
+    <row r="46" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3081,9 +3112,9 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
+    <row r="47" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3098,9 +3129,9 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="73"/>
-      <c r="B48" s="73"/>
+    <row r="48" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3115,9 +3146,9 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
+    <row r="49" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3132,9 +3163,9 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="73"/>
-      <c r="B50" s="73"/>
+    <row r="50" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3149,9 +3180,9 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="73"/>
-      <c r="B51" s="73"/>
+    <row r="51" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3166,9 +3197,9 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="74"/>
-      <c r="B52" s="74"/>
+    <row r="52" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="78"/>
+      <c r="B52" s="78"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3185,7 +3216,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="20"/>
@@ -3196,7 +3227,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A54" s="19"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
@@ -3207,7 +3238,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A55" s="19"/>
       <c r="B55" s="19"/>
       <c r="C55" s="11" t="s">
@@ -3232,7 +3263,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20"/>
@@ -3243,7 +3274,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="41" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" ht="41.65" x14ac:dyDescent="0.35">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11" t="s">
@@ -3258,7 +3289,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="20"/>
@@ -3269,7 +3300,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A59" s="19"/>
       <c r="B59" s="19"/>
       <c r="C59" s="11" t="s">
@@ -3292,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A60" s="19"/>
       <c r="B60" s="19"/>
       <c r="C60" s="20"/>
@@ -3301,7 +3332,7 @@
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
     </row>
-    <row r="61" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A61" s="19"/>
       <c r="B61" s="19"/>
       <c r="C61" s="20"/>
@@ -3310,7 +3341,7 @@
       <c r="F61" s="37"/>
       <c r="G61" s="37"/>
     </row>
-    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -3324,17 +3355,17 @@
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="80" t="s">
+      <c r="C63" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="80"/>
-      <c r="E63" s="80"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A64" s="75" t="s">
         <v>10</v>
       </c>
@@ -3342,89 +3373,89 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="81"/>
-      <c r="E64" s="81"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A65" s="75" t="s">
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="81" t="s">
+      <c r="C65" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A66" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="81" t="s">
+      <c r="C66" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A67" s="75" t="s">
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="81" t="s">
+      <c r="C67" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="81"/>
-      <c r="E67" s="81"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A68" s="75" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="81" t="s">
+      <c r="C68" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A69" s="75" t="s">
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A70" s="38"/>
       <c r="B70" s="38"/>
       <c r="C70" s="39"/>
@@ -3433,7 +3464,7 @@
       <c r="F70" s="40"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -3442,7 +3473,7 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -3451,7 +3482,7 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -3460,7 +3491,7 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -3469,7 +3500,7 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -3478,7 +3509,7 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -3487,7 +3518,7 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -3496,7 +3527,7 @@
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -3505,7 +3536,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -3514,7 +3545,7 @@
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -3523,7 +3554,7 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -3532,7 +3563,7 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
     </row>
-    <row r="82" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -3541,7 +3572,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -3550,7 +3581,7 @@
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -3559,7 +3590,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -3568,7 +3599,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -3577,7 +3608,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -3586,7 +3617,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -3595,7 +3626,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -3604,7 +3635,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -3613,7 +3644,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -3622,7 +3653,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -3631,7 +3662,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -3640,7 +3671,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3649,7 +3680,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3658,7 +3689,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3667,7 +3698,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -3676,7 +3707,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3685,7 +3716,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="59" t="s">
         <v>45</v>
       </c>
@@ -3696,10 +3727,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="79" t="s">
+      <c r="E99" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="79"/>
+      <c r="F99" s="72"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3713,7 +3744,7 @@
       <c r="Q99" s="50"/>
       <c r="R99" s="50"/>
     </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A100" s="60" t="s">
         <v>46</v>
       </c>
@@ -3741,7 +3772,7 @@
       <c r="Q100" s="50"/>
       <c r="R100" s="50"/>
     </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D101" s="61" t="s">
         <v>32</v>
       </c>
@@ -3762,7 +3793,7 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="62"/>
       <c r="B102" s="62"/>
       <c r="C102" s="63"/>
@@ -3786,7 +3817,7 @@
       <c r="Q102" s="50"/>
       <c r="R102" s="50"/>
     </row>
-    <row r="103" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B103" s="60"/>
       <c r="C103" s="60"/>
       <c r="D103" s="64" t="s">
@@ -3809,7 +3840,7 @@
       <c r="Q103" s="50"/>
       <c r="R103" s="50"/>
     </row>
-    <row r="104" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A104" s="60" t="s">
         <v>54</v>
       </c>
@@ -3832,14 +3863,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3853,15 +3885,14 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3879,23 +3910,23 @@
   </sheetPr>
   <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.64453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.76171875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.64453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.64453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.41015625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1171875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.234375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.73046875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -3909,7 +3940,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3918,7 +3949,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -3931,7 +3962,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -3944,7 +3975,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -3961,7 +3992,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -3970,7 +4001,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -3979,18 +4010,18 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.7" x14ac:dyDescent="0.4">
-      <c r="A8" s="76" t="s">
+    <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3999,11 +4030,11 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="78" t="s">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -4016,11 +4047,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="78" t="s">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -4029,11 +4060,11 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -4042,11 +4073,11 @@
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="78" t="s">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -4055,11 +4086,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="78" t="s">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -4068,11 +4099,11 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="78" t="s">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -4081,7 +4112,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4090,7 +4121,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4107,11 +4138,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="72" t="s">
+    <row r="18" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -4124,9 +4155,9 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+    <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
         <v>142</v>
       </c>
@@ -4137,9 +4168,9 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+    <row r="20" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
         <v>143</v>
       </c>
@@ -4150,9 +4181,9 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+    <row r="21" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
         <v>144</v>
       </c>
@@ -4165,9 +4196,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
+    <row r="22" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="78"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="11" t="s">
         <v>29</v>
       </c>
@@ -4181,7 +4212,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -4192,7 +4223,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -4211,11 +4242,11 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="72" t="s">
+    <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -4232,9 +4263,9 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+    <row r="26" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="11" t="s">
         <v>142</v>
       </c>
@@ -4249,9 +4280,9 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+    <row r="27" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="11" t="s">
         <v>143</v>
       </c>
@@ -4266,9 +4297,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+    <row r="28" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
         <v>144</v>
       </c>
@@ -4283,9 +4314,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="74"/>
-      <c r="B29" s="74"/>
+    <row r="29" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="78"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
@@ -4302,7 +4333,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -4313,7 +4344,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -4332,11 +4363,11 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="72" t="s">
+    <row r="32" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -4353,9 +4384,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="73"/>
-      <c r="B33" s="73"/>
+    <row r="33" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="11" t="s">
         <v>142</v>
       </c>
@@ -4370,9 +4401,9 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="73"/>
-      <c r="B34" s="73"/>
+    <row r="34" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="11" t="s">
         <v>143</v>
       </c>
@@ -4387,9 +4418,9 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
+    <row r="35" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="11" t="s">
         <v>144</v>
       </c>
@@ -4404,9 +4435,9 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
+    <row r="36" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="78"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="11" t="s">
         <v>29</v>
       </c>
@@ -4423,7 +4454,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
@@ -4434,7 +4465,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -4445,7 +4476,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -4464,11 +4495,11 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="72" t="s">
+    <row r="40" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -4485,9 +4516,9 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+    <row r="41" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
         <v>142</v>
       </c>
@@ -4502,9 +4533,9 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="73"/>
-      <c r="B42" s="73"/>
+    <row r="42" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="11" t="s">
         <v>143</v>
       </c>
@@ -4519,9 +4550,9 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="73"/>
-      <c r="B43" s="73"/>
+    <row r="43" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="11" t="s">
         <v>144</v>
       </c>
@@ -4536,9 +4567,9 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="74"/>
-      <c r="B44" s="74"/>
+    <row r="44" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="78"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="11" t="s">
         <v>29</v>
       </c>
@@ -4555,7 +4586,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="20"/>
@@ -4566,7 +4597,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
       <c r="C46" s="20"/>
@@ -4577,7 +4608,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
       <c r="C47" s="11" t="s">
@@ -4602,7 +4633,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
@@ -4611,7 +4642,7 @@
       <c r="F48" s="37"/>
       <c r="G48" s="37"/>
     </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -4625,11 +4656,11 @@
         <v>5</v>
       </c>
       <c r="B50" s="75"/>
-      <c r="C50" s="80" t="s">
+      <c r="C50" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
       <c r="F50" s="31" t="s">
         <v>4</v>
       </c>
@@ -4643,8 +4674,8 @@
       <c r="C51" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
       <c r="F51" s="23">
         <v>6108</v>
       </c>
@@ -4658,8 +4689,8 @@
       <c r="C52" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="81"/>
-      <c r="E52" s="81"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
       <c r="F52" s="23">
         <v>5584</v>
       </c>
@@ -4673,8 +4704,8 @@
       <c r="C53" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="81"/>
-      <c r="E53" s="81"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
       <c r="F53" s="23">
         <v>5061</v>
       </c>
@@ -4688,14 +4719,14 @@
       <c r="C54" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
       <c r="F54" s="23">
         <v>4363</v>
       </c>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A55" s="38"/>
       <c r="B55" s="38"/>
       <c r="C55" s="39"/>
@@ -4704,7 +4735,7 @@
       <c r="F55" s="40"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -4713,7 +4744,7 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -4722,7 +4753,7 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -4731,7 +4762,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -4740,7 +4771,7 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -4749,7 +4780,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -4758,7 +4789,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -4767,7 +4798,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -4776,7 +4807,7 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -4785,7 +4816,7 @@
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -4794,7 +4825,7 @@
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -4803,7 +4834,7 @@
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -4812,7 +4843,7 @@
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -4821,7 +4852,7 @@
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -4830,7 +4861,7 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -4839,7 +4870,7 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -4848,7 +4879,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -4857,7 +4888,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -4866,7 +4897,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -4875,7 +4906,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -4884,7 +4915,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -4893,7 +4924,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -4902,7 +4933,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -4911,7 +4942,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -4920,7 +4951,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -4929,7 +4960,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -4938,7 +4969,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -4947,7 +4978,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -4956,7 +4987,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -4965,7 +4996,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -4974,7 +5005,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -4983,7 +5014,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -4992,7 +5023,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -5001,7 +5032,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -5010,7 +5041,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -5019,7 +5050,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -5028,7 +5059,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" ht="11.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" ht="11.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -5037,7 +5068,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -5046,7 +5077,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -5055,7 +5086,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -5064,7 +5095,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -5073,7 +5104,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="59" t="s">
         <v>45</v>
       </c>
@@ -5084,10 +5115,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
@@ -5101,7 +5132,7 @@
       <c r="Q97" s="50"/>
       <c r="R97" s="50"/>
     </row>
-    <row r="98" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A98" s="60" t="s">
         <v>46</v>
       </c>
@@ -5129,7 +5160,7 @@
       <c r="Q98" s="50"/>
       <c r="R98" s="50"/>
     </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D99" s="61" t="s">
         <v>32</v>
       </c>
@@ -5150,7 +5181,7 @@
       <c r="Q99" s="50"/>
       <c r="R99" s="50"/>
     </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A100" s="62"/>
       <c r="B100" s="62"/>
       <c r="C100" s="63"/>
@@ -5174,7 +5205,7 @@
       <c r="Q100" s="50"/>
       <c r="R100" s="50"/>
     </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B101" s="60"/>
       <c r="C101" s="60"/>
       <c r="D101" s="64" t="s">
@@ -5197,7 +5228,7 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="60" t="s">
         <v>54</v>
       </c>
@@ -5220,12 +5251,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
     <mergeCell ref="E97:F97"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5242,6 +5267,12 @@
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -5256,21 +5287,23 @@
   </sheetPr>
   <dimension ref="A1:R153"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.64453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.64453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.1171875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.64453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.41015625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1171875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.234375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1171875" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -5284,7 +5317,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5293,7 +5326,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -5306,7 +5339,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -5319,7 +5352,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -5336,7 +5369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -5345,7 +5378,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -5354,7 +5387,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -5365,7 +5398,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5376,7 +5409,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5387,7 +5420,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -5398,7 +5431,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -5409,7 +5442,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5420,7 +5453,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -5431,7 +5464,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -5442,7 +5475,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5453,7 +5486,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5464,7 +5497,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5475,7 +5508,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5486,7 +5519,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -5497,7 +5530,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -5508,7 +5541,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -5519,7 +5552,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -5528,7 +5561,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -5537,7 +5570,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -5546,7 +5579,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -5555,7 +5588,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -5564,7 +5597,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -5573,7 +5606,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5582,7 +5615,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -5591,7 +5624,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -5600,7 +5633,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -5609,7 +5642,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -5618,7 +5651,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -5627,7 +5660,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -5636,7 +5669,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -5645,7 +5678,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -5654,7 +5687,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -5663,7 +5696,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -5672,7 +5705,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -5681,7 +5714,7 @@
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -5690,7 +5723,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -5699,7 +5732,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -5708,7 +5741,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -5717,7 +5750,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -5726,7 +5759,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -5735,7 +5768,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -5744,7 +5777,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -5753,7 +5786,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -5762,7 +5795,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -5771,7 +5804,7 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -5780,7 +5813,7 @@
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -5789,7 +5822,7 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -5798,7 +5831,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -5807,7 +5840,7 @@
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -5816,7 +5849,7 @@
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -5825,7 +5858,7 @@
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -5834,7 +5867,7 @@
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -5843,7 +5876,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -5852,7 +5885,7 @@
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -5861,7 +5894,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -5870,7 +5903,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -5879,7 +5912,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -5888,7 +5921,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -5897,7 +5930,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -5906,7 +5939,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -5915,7 +5948,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -5924,7 +5957,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -5933,7 +5966,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -5942,7 +5975,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -5951,7 +5984,7 @@
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -5960,7 +5993,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -5969,7 +6002,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -5978,7 +6011,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -5987,7 +6020,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -5996,7 +6029,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -6005,7 +6038,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -6014,7 +6047,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -6023,7 +6056,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -6032,7 +6065,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -6041,7 +6074,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -6050,7 +6083,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -6059,7 +6092,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -6068,7 +6101,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -6077,7 +6110,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -6086,7 +6119,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -6095,7 +6128,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -6104,7 +6137,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -6113,7 +6146,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -6122,7 +6155,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -6131,7 +6164,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -6140,7 +6173,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -6149,7 +6182,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -6158,7 +6191,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -6167,7 +6200,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -6176,7 +6209,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -6185,7 +6218,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A97" s="59" t="s">
         <v>45</v>
       </c>
@@ -6196,13 +6229,13 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
     </row>
-    <row r="98" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A98" s="60" t="s">
         <v>46</v>
       </c>
@@ -6219,7 +6252,7 @@
       <c r="F98" s="60"/>
       <c r="G98" s="58"/>
     </row>
-    <row r="99" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A99" s="51"/>
       <c r="B99" s="51"/>
       <c r="C99" s="51"/>
@@ -6232,7 +6265,7 @@
       <c r="F99" s="60"/>
       <c r="G99" s="53"/>
     </row>
-    <row r="100" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A100" s="62"/>
       <c r="B100" s="62"/>
       <c r="C100" s="63"/>
@@ -6245,7 +6278,7 @@
       <c r="F100" s="60"/>
       <c r="G100" s="53"/>
     </row>
-    <row r="101" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A101" s="51"/>
       <c r="B101" s="60"/>
       <c r="C101" s="60"/>
@@ -6258,7 +6291,7 @@
       <c r="F101" s="60"/>
       <c r="G101" s="53"/>
     </row>
-    <row r="102" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="60" t="s">
         <v>54</v>
       </c>
@@ -6269,8 +6302,8 @@
       <c r="F102" s="58"/>
       <c r="G102" s="52"/>
     </row>
-    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -6290,7 +6323,7 @@
       <c r="Q148" s="50"/>
       <c r="R148" s="50"/>
     </row>
-    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -6310,7 +6343,7 @@
       <c r="Q149" s="50"/>
       <c r="R149" s="50"/>
     </row>
-    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -6330,7 +6363,7 @@
       <c r="Q150" s="50"/>
       <c r="R150" s="50"/>
     </row>
-    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -6350,7 +6383,7 @@
       <c r="Q151" s="50"/>
       <c r="R151" s="50"/>
     </row>
-    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -6370,7 +6403,7 @@
       <c r="Q152" s="50"/>
       <c r="R152" s="50"/>
     </row>
-    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -6400,10 +6433,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6547,39 +6600,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6596,25 +6644,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
103168 16-19 funding - footer format fix
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E6F97E-97A2-473C-BFC3-1A0381DC0D82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07F93B1-382D-431C-BCC2-0130F566C786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="-8580" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -933,20 +933,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -956,6 +942,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -963,6 +953,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1061,7 +1061,7 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="9586913" cy="3676652"/>
+    <xdr:ext cx="9586913" cy="4295776"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -1075,8 +1075,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9524" y="12815887"/>
-          <a:ext cx="9586913" cy="3676652"/>
+          <a:off x="9524" y="12896849"/>
+          <a:ext cx="9586913" cy="4295776"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2408,8 +2408,8 @@
   </sheetPr>
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -2509,11 +2509,11 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="80"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -2529,10 +2529,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -2546,10 +2546,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -2559,10 +2559,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2572,10 +2572,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2585,10 +2585,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -2598,10 +2598,10 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -2637,10 +2637,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2654,8 +2654,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2667,8 +2667,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2680,8 +2680,8 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2695,8 +2695,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2710,8 +2710,8 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="77"/>
-      <c r="B23" s="77"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2725,8 +2725,8 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="78"/>
-      <c r="B24" s="78"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2771,10 +2771,10 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="72" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2792,8 +2792,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2809,8 +2809,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="77"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2826,8 +2826,8 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2843,8 +2843,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2860,8 +2860,8 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2877,8 +2877,8 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="78"/>
-      <c r="B33" s="78"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2926,10 +2926,10 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="76" t="s">
+      <c r="A36" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2947,8 +2947,8 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="77"/>
-      <c r="B37" s="77"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2964,8 +2964,8 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="73"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2981,8 +2981,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="73"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2998,8 +2998,8 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -3015,8 +3015,8 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3032,8 +3032,8 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="78"/>
-      <c r="B42" s="78"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="74"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3092,10 +3092,10 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="76" t="s">
+      <c r="A46" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="76" t="s">
+      <c r="B46" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3113,8 +3113,8 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="77"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3130,8 +3130,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="77"/>
-      <c r="B48" s="77"/>
+      <c r="A48" s="73"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3147,8 +3147,8 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="77"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3164,8 +3164,8 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="77"/>
-      <c r="B50" s="77"/>
+      <c r="A50" s="73"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3181,8 +3181,8 @@
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="77"/>
-      <c r="B51" s="77"/>
+      <c r="A51" s="73"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3198,8 +3198,8 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="78"/>
-      <c r="B52" s="78"/>
+      <c r="A52" s="74"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3355,11 +3355,11 @@
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="73" t="s">
+      <c r="C63" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="80"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
@@ -3373,8 +3373,8 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
+      <c r="D64" s="81"/>
+      <c r="E64" s="81"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
@@ -3385,11 +3385,11 @@
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="74" t="s">
+      <c r="C65" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="81"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
@@ -3400,11 +3400,11 @@
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="74" t="s">
+      <c r="C66" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="81"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
@@ -3415,11 +3415,11 @@
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="74" t="s">
+      <c r="C67" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
+      <c r="D67" s="81"/>
+      <c r="E67" s="81"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
@@ -3430,11 +3430,11 @@
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="74" t="s">
+      <c r="C68" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
+      <c r="D68" s="81"/>
+      <c r="E68" s="81"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
@@ -3445,11 +3445,11 @@
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="74" t="s">
+      <c r="C69" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
+      <c r="D69" s="81"/>
+      <c r="E69" s="81"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
@@ -3727,10 +3727,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="72" t="s">
+      <c r="E99" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="72"/>
+      <c r="F99" s="79"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3863,15 +3863,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3885,14 +3884,15 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3910,7 +3910,7 @@
   </sheetPr>
   <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -4011,10 +4011,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="79"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -4031,10 +4031,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -4048,10 +4048,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -4061,10 +4061,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -4074,10 +4074,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -4087,10 +4087,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -4100,10 +4100,10 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -4139,10 +4139,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -4156,8 +4156,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
         <v>142</v>
       </c>
@@ -4169,8 +4169,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
         <v>143</v>
       </c>
@@ -4182,8 +4182,8 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
         <v>144</v>
       </c>
@@ -4197,8 +4197,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="78"/>
-      <c r="B22" s="78"/>
+      <c r="A22" s="74"/>
+      <c r="B22" s="74"/>
       <c r="C22" s="11" t="s">
         <v>29</v>
       </c>
@@ -4243,10 +4243,10 @@
       <c r="I24" s="1"/>
     </row>
     <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="76" t="s">
+      <c r="A25" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="72" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -4264,8 +4264,8 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
+      <c r="A26" s="73"/>
+      <c r="B26" s="73"/>
       <c r="C26" s="11" t="s">
         <v>142</v>
       </c>
@@ -4281,8 +4281,8 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="11" t="s">
         <v>143</v>
       </c>
@@ -4298,8 +4298,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
         <v>144</v>
       </c>
@@ -4315,8 +4315,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="78"/>
-      <c r="B29" s="78"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="74"/>
       <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
@@ -4364,10 +4364,10 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="76" t="s">
+      <c r="A32" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -4385,8 +4385,8 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
       <c r="C33" s="11" t="s">
         <v>142</v>
       </c>
@@ -4402,8 +4402,8 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="73"/>
       <c r="C34" s="11" t="s">
         <v>143</v>
       </c>
@@ -4419,8 +4419,8 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="11" t="s">
         <v>144</v>
       </c>
@@ -4436,8 +4436,8 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="78"/>
-      <c r="B36" s="78"/>
+      <c r="A36" s="74"/>
+      <c r="B36" s="74"/>
       <c r="C36" s="11" t="s">
         <v>29</v>
       </c>
@@ -4496,10 +4496,10 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="76" t="s">
+      <c r="A40" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="76" t="s">
+      <c r="B40" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -4517,8 +4517,8 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="11" t="s">
         <v>142</v>
       </c>
@@ -4534,8 +4534,8 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
+      <c r="A42" s="73"/>
+      <c r="B42" s="73"/>
       <c r="C42" s="11" t="s">
         <v>143</v>
       </c>
@@ -4551,8 +4551,8 @@
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="77"/>
-      <c r="B43" s="77"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="73"/>
       <c r="C43" s="11" t="s">
         <v>144</v>
       </c>
@@ -4568,8 +4568,8 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="78"/>
-      <c r="B44" s="78"/>
+      <c r="A44" s="74"/>
+      <c r="B44" s="74"/>
       <c r="C44" s="11" t="s">
         <v>29</v>
       </c>
@@ -4656,11 +4656,11 @@
         <v>5</v>
       </c>
       <c r="B50" s="75"/>
-      <c r="C50" s="73" t="s">
+      <c r="C50" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="80"/>
       <c r="F50" s="31" t="s">
         <v>4</v>
       </c>
@@ -4674,8 +4674,8 @@
       <c r="C51" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
+      <c r="D51" s="81"/>
+      <c r="E51" s="81"/>
       <c r="F51" s="23">
         <v>6108</v>
       </c>
@@ -4689,8 +4689,8 @@
       <c r="C52" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
       <c r="F52" s="23">
         <v>5584</v>
       </c>
@@ -4704,8 +4704,8 @@
       <c r="C53" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
+      <c r="D53" s="81"/>
+      <c r="E53" s="81"/>
       <c r="F53" s="23">
         <v>5061</v>
       </c>
@@ -4719,8 +4719,8 @@
       <c r="C54" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
+      <c r="D54" s="81"/>
+      <c r="E54" s="81"/>
       <c r="F54" s="23">
         <v>4363</v>
       </c>
@@ -5115,10 +5115,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E97" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="72"/>
+      <c r="F97" s="79"/>
       <c r="G97" s="49"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
@@ -5251,6 +5251,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
     <mergeCell ref="E97:F97"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5267,12 +5273,6 @@
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -5287,7 +5287,7 @@
   </sheetPr>
   <dimension ref="A1:R153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
@@ -6229,10 +6229,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E97" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="72"/>
+      <c r="F97" s="79"/>
       <c r="G97" s="49"/>
     </row>
     <row r="98" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
@@ -6433,30 +6433,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6600,34 +6580,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6644,10 +6629,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated to latest DC-IO packages
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07F93B1-382D-431C-BCC2-0130F566C786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFE00A5-8FCA-496C-B313-C283B92E2A87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="891" yWindow="-103" windowWidth="24926" windowHeight="17349" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -933,6 +933,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -942,10 +956,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -953,16 +963,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2408,23 +2408,21 @@
   </sheetPr>
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="39" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="2"/>
+    <col min="3" max="3" width="27.69140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3828125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.15234375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.23046875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -2438,7 +2436,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2447,7 +2445,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2460,7 +2458,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -2473,7 +2471,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -2490,7 +2488,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2499,7 +2497,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2508,18 +2506,18 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="76" t="s">
+    <row r="8" spans="1:9" ht="17.600000000000001" x14ac:dyDescent="0.35">
+      <c r="A8" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2528,11 +2526,11 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="78" t="s">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -2546,10 +2544,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -2558,11 +2556,11 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2571,11 +2569,11 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="78" t="s">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2584,11 +2582,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="78" t="s">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -2597,11 +2595,11 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="78" t="s">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -2610,7 +2608,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2619,7 +2617,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -2636,11 +2634,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="72" t="s">
+    <row r="18" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2653,9 +2651,9 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+    <row r="19" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2666,9 +2664,9 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+    <row r="20" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2679,9 +2677,9 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+    <row r="21" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2694,9 +2692,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+    <row r="22" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2709,9 +2707,9 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="73"/>
-      <c r="B23" s="73"/>
+    <row r="23" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="77"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2724,9 +2722,9 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
+    <row r="24" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="78"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2740,7 +2738,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2751,7 +2749,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -2770,11 +2768,11 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="72" t="s">
+    <row r="27" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2791,9 +2789,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+    <row r="28" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2808,9 +2806,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
+    <row r="29" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2825,9 +2823,9 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
+    <row r="30" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2842,9 +2840,9 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
+    <row r="31" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2859,9 +2857,9 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
+    <row r="32" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2876,9 +2874,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
+    <row r="33" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2895,7 +2893,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -2906,7 +2904,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -2925,11 +2923,11 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="72" t="s">
+    <row r="36" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2946,9 +2944,9 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
+    <row r="37" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2963,9 +2961,9 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
+    <row r="38" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2980,9 +2978,9 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="73"/>
-      <c r="B39" s="73"/>
+    <row r="39" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2997,9 +2995,9 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="73"/>
-      <c r="B40" s="73"/>
+    <row r="40" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -3014,9 +3012,9 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+    <row r="41" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3031,9 +3029,9 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
+    <row r="42" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="78"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3050,7 +3048,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
@@ -3061,7 +3059,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3072,7 +3070,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -3091,11 +3089,11 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="72" t="s">
+    <row r="46" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3112,9 +3110,9 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
+    <row r="47" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3129,9 +3127,9 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="73"/>
-      <c r="B48" s="73"/>
+    <row r="48" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3146,9 +3144,9 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
+    <row r="49" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3163,9 +3161,9 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="73"/>
-      <c r="B50" s="73"/>
+    <row r="50" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3180,9 +3178,9 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="73"/>
-      <c r="B51" s="73"/>
+    <row r="51" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3197,9 +3195,9 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="74"/>
-      <c r="B52" s="74"/>
+    <row r="52" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="78"/>
+      <c r="B52" s="78"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3216,7 +3214,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="20"/>
@@ -3227,7 +3225,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A54" s="19"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
@@ -3238,7 +3236,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A55" s="19"/>
       <c r="B55" s="19"/>
       <c r="C55" s="11" t="s">
@@ -3263,7 +3261,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20"/>
@@ -3274,7 +3272,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="41.65" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" ht="42.45" x14ac:dyDescent="0.3">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11" t="s">
@@ -3289,7 +3287,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="20"/>
@@ -3300,7 +3298,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A59" s="19"/>
       <c r="B59" s="19"/>
       <c r="C59" s="11" t="s">
@@ -3323,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A60" s="19"/>
       <c r="B60" s="19"/>
       <c r="C60" s="20"/>
@@ -3332,7 +3330,7 @@
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
     </row>
-    <row r="61" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A61" s="19"/>
       <c r="B61" s="19"/>
       <c r="C61" s="20"/>
@@ -3350,22 +3348,22 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="75" t="s">
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="80" t="s">
+      <c r="C63" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="80"/>
-      <c r="E63" s="80"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A64" s="75" t="s">
         <v>10</v>
       </c>
@@ -3373,89 +3371,89 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="81"/>
-      <c r="E64" s="81"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A65" s="75" t="s">
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="81" t="s">
+      <c r="C65" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A66" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="81" t="s">
+      <c r="C66" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A67" s="75" t="s">
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="81" t="s">
+      <c r="C67" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="81"/>
-      <c r="E67" s="81"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A68" s="75" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="81" t="s">
+      <c r="C68" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A69" s="75" t="s">
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A70" s="38"/>
       <c r="B70" s="38"/>
       <c r="C70" s="39"/>
@@ -3464,7 +3462,7 @@
       <c r="F70" s="40"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -3473,7 +3471,7 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -3482,7 +3480,7 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -3491,7 +3489,7 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -3500,7 +3498,7 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -3509,7 +3507,7 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -3518,7 +3516,7 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -3527,7 +3525,7 @@
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -3536,7 +3534,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -3545,7 +3543,7 @@
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -3554,7 +3552,7 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -3563,7 +3561,7 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
     </row>
-    <row r="82" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -3572,7 +3570,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -3581,7 +3579,7 @@
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -3590,7 +3588,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -3599,7 +3597,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -3608,7 +3606,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -3617,7 +3615,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -3626,7 +3624,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -3635,7 +3633,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -3644,7 +3642,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -3653,7 +3651,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -3662,7 +3660,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -3671,7 +3669,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3680,7 +3678,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3689,7 +3687,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3698,7 +3696,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -3707,7 +3705,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3716,7 +3714,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="59" t="s">
         <v>45</v>
       </c>
@@ -3727,10 +3725,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="79" t="s">
+      <c r="E99" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="79"/>
+      <c r="F99" s="72"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3744,7 +3742,7 @@
       <c r="Q99" s="50"/>
       <c r="R99" s="50"/>
     </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A100" s="60" t="s">
         <v>46</v>
       </c>
@@ -3772,7 +3770,7 @@
       <c r="Q100" s="50"/>
       <c r="R100" s="50"/>
     </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="D101" s="61" t="s">
         <v>32</v>
       </c>
@@ -3793,7 +3791,7 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A102" s="62"/>
       <c r="B102" s="62"/>
       <c r="C102" s="63"/>
@@ -3817,7 +3815,7 @@
       <c r="Q102" s="50"/>
       <c r="R102" s="50"/>
     </row>
-    <row r="103" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="B103" s="60"/>
       <c r="C103" s="60"/>
       <c r="D103" s="64" t="s">
@@ -3840,7 +3838,7 @@
       <c r="Q103" s="50"/>
       <c r="R103" s="50"/>
     </row>
-    <row r="104" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A104" s="60" t="s">
         <v>54</v>
       </c>
@@ -3863,14 +3861,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3884,15 +3883,14 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3910,23 +3908,21 @@
   </sheetPr>
   <dimension ref="A1:R102"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.73046875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="2"/>
+    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.69140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.69140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3828125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.15234375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.23046875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -3940,7 +3936,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3949,7 +3945,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -3962,7 +3958,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -3975,7 +3971,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -3992,7 +3988,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -4001,7 +3997,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -4010,18 +4006,18 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="76" t="s">
+    <row r="8" spans="1:9" ht="17.600000000000001" x14ac:dyDescent="0.35">
+      <c r="A8" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="76"/>
+      <c r="B8" s="79"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -4030,11 +4026,11 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="78" t="s">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -4048,10 +4044,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -4060,11 +4056,11 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="78" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -4073,11 +4069,11 @@
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="78" t="s">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -4086,11 +4082,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="78" t="s">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -4099,11 +4095,11 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="78" t="s">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="81" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="78"/>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -4112,7 +4108,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4121,7 +4117,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4138,11 +4134,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="72" t="s">
+    <row r="18" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -4155,9 +4151,9 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+    <row r="19" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
         <v>142</v>
       </c>
@@ -4168,9 +4164,9 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+    <row r="20" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
         <v>143</v>
       </c>
@@ -4181,9 +4177,9 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+    <row r="21" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
         <v>144</v>
       </c>
@@ -4196,9 +4192,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="74"/>
-      <c r="B22" s="74"/>
+    <row r="22" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="78"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="11" t="s">
         <v>29</v>
       </c>
@@ -4212,7 +4208,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -4223,7 +4219,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
@@ -4242,11 +4238,11 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="72" t="s">
+    <row r="25" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="72" t="s">
+      <c r="B25" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="11" t="s">
@@ -4263,9 +4259,9 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="73"/>
-      <c r="B26" s="73"/>
+    <row r="26" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="11" t="s">
         <v>142</v>
       </c>
@@ -4280,9 +4276,9 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+    <row r="27" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="11" t="s">
         <v>143</v>
       </c>
@@ -4297,9 +4293,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+    <row r="28" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
         <v>144</v>
       </c>
@@ -4314,9 +4310,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="74"/>
-      <c r="B29" s="74"/>
+    <row r="29" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="78"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="11" t="s">
         <v>29</v>
       </c>
@@ -4333,7 +4329,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -4344,7 +4340,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A31" s="14"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -4363,11 +4359,11 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="72" t="s">
+    <row r="32" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="72" t="s">
+      <c r="B32" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="11" t="s">
@@ -4384,9 +4380,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="73"/>
-      <c r="B33" s="73"/>
+    <row r="33" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="77"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="11" t="s">
         <v>142</v>
       </c>
@@ -4401,9 +4397,9 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="73"/>
-      <c r="B34" s="73"/>
+    <row r="34" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="11" t="s">
         <v>143</v>
       </c>
@@ -4418,9 +4414,9 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
+    <row r="35" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="11" t="s">
         <v>144</v>
       </c>
@@ -4435,9 +4431,9 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="74"/>
-      <c r="B36" s="74"/>
+    <row r="36" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="78"/>
+      <c r="B36" s="78"/>
       <c r="C36" s="11" t="s">
         <v>29</v>
       </c>
@@ -4454,7 +4450,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
@@ -4465,7 +4461,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -4476,7 +4472,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A39" s="14"/>
       <c r="B39" s="14"/>
       <c r="C39" s="15"/>
@@ -4495,11 +4491,11 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="72" t="s">
+    <row r="40" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="72" t="s">
+      <c r="B40" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C40" s="11" t="s">
@@ -4516,9 +4512,9 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+    <row r="41" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
         <v>142</v>
       </c>
@@ -4533,9 +4529,9 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="73"/>
-      <c r="B42" s="73"/>
+    <row r="42" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="77"/>
+      <c r="B42" s="77"/>
       <c r="C42" s="11" t="s">
         <v>143</v>
       </c>
@@ -4550,9 +4546,9 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="73"/>
-      <c r="B43" s="73"/>
+    <row r="43" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="77"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="11" t="s">
         <v>144</v>
       </c>
@@ -4567,9 +4563,9 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="74"/>
-      <c r="B44" s="74"/>
+    <row r="44" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="78"/>
+      <c r="B44" s="78"/>
       <c r="C44" s="11" t="s">
         <v>29</v>
       </c>
@@ -4586,7 +4582,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
       <c r="C45" s="20"/>
@@ -4597,7 +4593,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
       <c r="C46" s="20"/>
@@ -4608,7 +4604,7 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
       <c r="C47" s="11" t="s">
@@ -4633,7 +4629,7 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
@@ -4651,22 +4647,22 @@
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
     </row>
-    <row r="50" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="75" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="75"/>
-      <c r="C50" s="80" t="s">
+      <c r="C50" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="80"/>
-      <c r="E50" s="80"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="73"/>
       <c r="F50" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G50" s="9"/>
     </row>
-    <row r="51" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="70" t="s">
         <v>141</v>
       </c>
@@ -4674,14 +4670,14 @@
       <c r="C51" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D51" s="81"/>
-      <c r="E51" s="81"/>
+      <c r="D51" s="74"/>
+      <c r="E51" s="74"/>
       <c r="F51" s="23">
         <v>6108</v>
       </c>
       <c r="G51" s="9"/>
     </row>
-    <row r="52" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="70" t="s">
         <v>142</v>
       </c>
@@ -4689,14 +4685,14 @@
       <c r="C52" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="81"/>
-      <c r="E52" s="81"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
       <c r="F52" s="23">
         <v>5584</v>
       </c>
       <c r="G52" s="9"/>
     </row>
-    <row r="53" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="70" t="s">
         <v>143</v>
       </c>
@@ -4704,14 +4700,14 @@
       <c r="C53" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="81"/>
-      <c r="E53" s="81"/>
+      <c r="D53" s="74"/>
+      <c r="E53" s="74"/>
       <c r="F53" s="23">
         <v>5061</v>
       </c>
       <c r="G53" s="9"/>
     </row>
-    <row r="54" spans="1:7" ht="13.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="70" t="s">
         <v>144</v>
       </c>
@@ -4719,14 +4715,14 @@
       <c r="C54" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="81"/>
-      <c r="E54" s="81"/>
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
       <c r="F54" s="23">
         <v>4363</v>
       </c>
       <c r="G54" s="9"/>
     </row>
-    <row r="55" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A55" s="38"/>
       <c r="B55" s="38"/>
       <c r="C55" s="39"/>
@@ -4735,7 +4731,7 @@
       <c r="F55" s="40"/>
       <c r="G55" s="9"/>
     </row>
-    <row r="56" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -4744,7 +4740,7 @@
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
     </row>
-    <row r="57" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -4753,7 +4749,7 @@
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
     </row>
-    <row r="58" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -4762,7 +4758,7 @@
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -4771,7 +4767,7 @@
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -4780,7 +4776,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -4789,7 +4785,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -4798,7 +4794,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -4807,7 +4803,7 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -4816,7 +4812,7 @@
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -4825,7 +4821,7 @@
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -4834,7 +4830,7 @@
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -4843,7 +4839,7 @@
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -4852,7 +4848,7 @@
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -4861,7 +4857,7 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -4870,7 +4866,7 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -4879,7 +4875,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -4888,7 +4884,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -4897,7 +4893,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -4906,7 +4902,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -4915,7 +4911,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -4924,7 +4920,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -4933,7 +4929,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -4942,7 +4938,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -4951,7 +4947,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -4960,7 +4956,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -4969,7 +4965,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -4978,7 +4974,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -4987,7 +4983,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -4996,7 +4992,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -5005,7 +5001,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -5014,7 +5010,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -5023,7 +5019,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -5032,7 +5028,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -5041,7 +5037,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -5050,7 +5046,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -5059,7 +5055,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" ht="11.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="11.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -5068,7 +5064,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -5077,7 +5073,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -5086,7 +5082,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -5095,7 +5091,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -5104,7 +5100,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="59" t="s">
         <v>45</v>
       </c>
@@ -5115,10 +5111,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
       <c r="H97" s="50"/>
       <c r="I97" s="50"/>
@@ -5132,7 +5128,7 @@
       <c r="Q97" s="50"/>
       <c r="R97" s="50"/>
     </row>
-    <row r="98" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A98" s="60" t="s">
         <v>46</v>
       </c>
@@ -5160,7 +5156,7 @@
       <c r="Q98" s="50"/>
       <c r="R98" s="50"/>
     </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="D99" s="61" t="s">
         <v>32</v>
       </c>
@@ -5181,7 +5177,7 @@
       <c r="Q99" s="50"/>
       <c r="R99" s="50"/>
     </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A100" s="62"/>
       <c r="B100" s="62"/>
       <c r="C100" s="63"/>
@@ -5205,7 +5201,7 @@
       <c r="Q100" s="50"/>
       <c r="R100" s="50"/>
     </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="B101" s="60"/>
       <c r="C101" s="60"/>
       <c r="D101" s="64" t="s">
@@ -5228,7 +5224,7 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A102" s="60" t="s">
         <v>54</v>
       </c>
@@ -5251,12 +5247,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
     <mergeCell ref="E97:F97"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5273,6 +5263,12 @@
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -5287,23 +5283,21 @@
   </sheetPr>
   <dimension ref="A1:R153"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.1328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.1328125" style="2"/>
+    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.69140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.15234375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.69140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3828125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.15234375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.23046875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.15234375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -5317,7 +5311,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5326,7 +5320,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -5339,7 +5333,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -5352,7 +5346,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -5369,7 +5363,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -5378,7 +5372,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -5387,7 +5381,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -5398,7 +5392,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5409,7 +5403,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5420,7 +5414,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -5431,7 +5425,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -5442,7 +5436,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5453,7 +5447,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -5464,7 +5458,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -5475,7 +5469,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5486,7 +5480,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5497,7 +5491,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5508,7 +5502,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5519,7 +5513,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -5530,7 +5524,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -5541,7 +5535,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -5552,7 +5546,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -5561,7 +5555,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -5570,7 +5564,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -5579,7 +5573,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -5588,7 +5582,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -5597,7 +5591,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -5606,7 +5600,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5615,7 +5609,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -5624,7 +5618,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -5633,7 +5627,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -5642,7 +5636,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -5651,7 +5645,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -5660,7 +5654,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -5669,7 +5663,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -5678,7 +5672,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -5687,7 +5681,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -5696,7 +5690,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -5705,7 +5699,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -5714,7 +5708,7 @@
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -5723,7 +5717,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -5732,7 +5726,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -5741,7 +5735,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -5750,7 +5744,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -5759,7 +5753,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -5768,7 +5762,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -5777,7 +5771,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -5786,7 +5780,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -5795,7 +5789,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -5804,7 +5798,7 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -5813,7 +5807,7 @@
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -5822,7 +5816,7 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -5831,7 +5825,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -5840,7 +5834,7 @@
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -5849,7 +5843,7 @@
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -5858,7 +5852,7 @@
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -5867,7 +5861,7 @@
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -5876,7 +5870,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -5885,7 +5879,7 @@
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -5894,7 +5888,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -5903,7 +5897,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -5912,7 +5906,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -5921,7 +5915,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -5930,7 +5924,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -5939,7 +5933,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -5948,7 +5942,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -5957,7 +5951,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -5966,7 +5960,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -5975,7 +5969,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -5984,7 +5978,7 @@
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -5993,7 +5987,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -6002,7 +5996,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -6011,7 +6005,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -6020,7 +6014,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -6029,7 +6023,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -6038,7 +6032,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -6047,7 +6041,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -6056,7 +6050,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -6065,7 +6059,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -6074,7 +6068,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -6083,7 +6077,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -6092,7 +6086,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -6101,7 +6095,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -6110,7 +6104,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -6119,7 +6113,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -6128,7 +6122,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -6137,7 +6131,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -6146,7 +6140,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -6155,7 +6149,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -6164,7 +6158,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -6173,7 +6167,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -6182,7 +6176,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -6191,7 +6185,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -6200,7 +6194,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -6209,7 +6203,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -6218,7 +6212,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A97" s="59" t="s">
         <v>45</v>
       </c>
@@ -6229,13 +6223,13 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
+      <c r="E97" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="79"/>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
     </row>
-    <row r="98" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A98" s="60" t="s">
         <v>46</v>
       </c>
@@ -6252,7 +6246,7 @@
       <c r="F98" s="60"/>
       <c r="G98" s="58"/>
     </row>
-    <row r="99" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A99" s="51"/>
       <c r="B99" s="51"/>
       <c r="C99" s="51"/>
@@ -6265,7 +6259,7 @@
       <c r="F99" s="60"/>
       <c r="G99" s="53"/>
     </row>
-    <row r="100" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A100" s="62"/>
       <c r="B100" s="62"/>
       <c r="C100" s="63"/>
@@ -6278,7 +6272,7 @@
       <c r="F100" s="60"/>
       <c r="G100" s="53"/>
     </row>
-    <row r="101" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A101" s="51"/>
       <c r="B101" s="60"/>
       <c r="C101" s="60"/>
@@ -6291,7 +6285,7 @@
       <c r="F101" s="60"/>
       <c r="G101" s="53"/>
     </row>
-    <row r="102" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
       <c r="A102" s="60" t="s">
         <v>54</v>
       </c>
@@ -6302,8 +6296,8 @@
       <c r="F102" s="58"/>
       <c r="G102" s="52"/>
     </row>
-    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -6323,7 +6317,7 @@
       <c r="Q148" s="50"/>
       <c r="R148" s="50"/>
     </row>
-    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -6343,7 +6337,7 @@
       <c r="Q149" s="50"/>
       <c r="R149" s="50"/>
     </row>
-    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -6363,7 +6357,7 @@
       <c r="Q150" s="50"/>
       <c r="R150" s="50"/>
     </row>
-    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -6383,7 +6377,7 @@
       <c r="Q151" s="50"/>
       <c r="R151" s="50"/>
     </row>
-    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -6403,7 +6397,7 @@
       <c r="Q152" s="50"/>
       <c r="R152" s="50"/>
     </row>
-    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -6433,10 +6427,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6580,39 +6594,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6629,25 +6638,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
104843 16to19 Funding claims band levels change
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFE00A5-8FCA-496C-B313-C283B92E2A87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B61428E-D43C-4794-B578-DF0CB7B71783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="891" yWindow="-103" windowWidth="24926" windowHeight="17349" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="-8580" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Declaration!$A$1:$G$104</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'T Levels'!$A$1:$G$104</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'T Levels'!$A$1:$G$108</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="153">
   <si>
     <t>Provider :</t>
   </si>
@@ -468,6 +468,30 @@
   </si>
   <si>
     <t>1100 hours (T Level Band 6)</t>
+  </si>
+  <si>
+    <t>Band 5 and below</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.DirectFundingStudents.Band1To5StudentNumbers</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsIncludingHNS.Band1To5StudentNumbers</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsIncludingHNS.Band1To5TotalFunding</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsWithEHCPlan.Band1To5StudentNumbers</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsWithEHCPlan.Band1To5TotalFunding</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.ContinuingStudentsExcludingEHCPlan.Band1To5StudentNumbers</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.ContinuingStudentsExcludingEHCPlan.Band1To5TotalFunding</t>
   </si>
 </sst>
 </file>
@@ -480,7 +504,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
     <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -534,6 +558,10 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -933,20 +961,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -956,6 +970,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -963,6 +981,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1359,10 +1387,10 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="9586913" cy="3676652"/>
+    <xdr:ext cx="9586913" cy="4657726"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -1376,8 +1404,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10582" y="20709466"/>
-          <a:ext cx="9586913" cy="3676652"/>
+          <a:off x="9524" y="10734674"/>
+          <a:ext cx="9586913" cy="4657726"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1505,7 +1533,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>4)     This report includes all students who have 16 to 19 funding and are identified in the ILR as 16 to 19 funded (that is, source of funding code = 107).</a:t>
+            <a:t>4)     This page includes all students who have 16 to 19 funding, are identified in the ILR as 16 to 19 funded (that is, source of funding code = 107, funding model = 25) and whose latest programme is a T Level (have a programme aim that is programme type 31 and T Level qualification as the core aim with programme type 31).</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1547,18 +1575,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>6)     Row C includes students aged 19 to 24 on 31</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> August 2020 who are 16 to 19 funded (that is, source of funding code = 107) and have an education health and care plan.</a:t>
+            <a:t>6)     Row C includes students aged 19 to 24 on 31 August 2020, who are 16 to 19 funded (that is, source of funding code = 107, funding model = 25), whose latest programme is a T Level (have a programme aim that is programme type 31 and T Level qualification as the core aim with programme type 31) and have an education health and care plan.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1579,28 +1596,7 @@
               <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>7)     Row D includes students aged 19 or over on 31 August 2020 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>who are 16 to 19 funded </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="0" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>(that is, source of funding code = 107), are funded using 16 to 19 funding (that is, funding model = 25) and are not included in Row C.</a:t>
+            <a:t>7)     Row D includes students aged 19 or over on 31 August 2020, who are 16 to 19 funded (that is, source of funding code = 107, funding model = 25), whose latest programme is a T Level (have a programme aim that is programme type 31 and T Level qualification as the core aim with programme type 31) and are not included in Row C.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2408,21 +2404,21 @@
   </sheetPr>
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="39" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.69140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.3828125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.15234375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.23046875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.15234375" style="2"/>
+    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -2436,7 +2432,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2445,7 +2441,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -2458,7 +2454,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -2471,7 +2467,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -2488,7 +2484,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2497,7 +2493,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2506,18 +2502,18 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A8" s="79" t="s">
+    <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="80"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2526,11 +2522,11 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="81" t="s">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -2544,10 +2540,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -2556,11 +2552,11 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="81" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2569,11 +2565,11 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="81" t="s">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -2582,11 +2578,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81" t="s">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -2595,11 +2591,11 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81" t="s">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -2608,7 +2604,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -2617,7 +2613,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -2634,11 +2630,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="76" t="s">
+    <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2651,9 +2647,9 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+    <row r="19" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2664,9 +2660,9 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+    <row r="20" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2677,9 +2673,9 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+    <row r="21" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2692,9 +2688,9 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
+    <row r="22" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2707,9 +2703,9 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="77"/>
-      <c r="B23" s="77"/>
+    <row r="23" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="73"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2722,9 +2718,9 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="78"/>
-      <c r="B24" s="78"/>
+    <row r="24" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2738,7 +2734,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -2749,7 +2745,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="14"/>
       <c r="C26" s="15"/>
@@ -2768,11 +2764,11 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="76" t="s">
+    <row r="27" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="72" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2789,9 +2785,9 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+    <row r="28" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2806,9 +2802,9 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="77"/>
-      <c r="B29" s="77"/>
+    <row r="29" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2823,9 +2819,9 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
+    <row r="30" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2840,9 +2836,9 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77"/>
+    <row r="31" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2857,9 +2853,9 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+    <row r="32" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2874,9 +2870,9 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="78"/>
-      <c r="B33" s="78"/>
+    <row r="33" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="74"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2893,7 +2889,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -2904,7 +2900,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A35" s="14"/>
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
@@ -2923,11 +2919,11 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="76" t="s">
+    <row r="36" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2944,9 +2940,9 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="77"/>
-      <c r="B37" s="77"/>
+    <row r="37" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2961,9 +2957,9 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+    <row r="38" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="73"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2978,9 +2974,9 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
+    <row r="39" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="73"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2995,9 +2991,9 @@
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77"/>
+    <row r="40" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="73"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -3012,9 +3008,9 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+    <row r="41" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3029,9 +3025,9 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="78"/>
-      <c r="B42" s="78"/>
+    <row r="42" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="74"/>
+      <c r="B42" s="74"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3048,7 +3044,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
@@ -3059,7 +3055,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3070,7 +3066,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A45" s="14"/>
       <c r="B45" s="14"/>
       <c r="C45" s="15"/>
@@ -3089,11 +3085,11 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="76" t="s">
+    <row r="46" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="76" t="s">
+      <c r="B46" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3110,9 +3106,9 @@
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="77"/>
-      <c r="B47" s="77"/>
+    <row r="47" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="73"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3127,9 +3123,9 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="77"/>
-      <c r="B48" s="77"/>
+    <row r="48" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="73"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3144,9 +3140,9 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="77"/>
-      <c r="B49" s="77"/>
+    <row r="49" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3161,9 +3157,9 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="77"/>
-      <c r="B50" s="77"/>
+    <row r="50" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="73"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3178,9 +3174,9 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="77"/>
-      <c r="B51" s="77"/>
+    <row r="51" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="73"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3195,9 +3191,9 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="78"/>
-      <c r="B52" s="78"/>
+    <row r="52" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="74"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3214,7 +3210,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A53" s="19"/>
       <c r="B53" s="19"/>
       <c r="C53" s="20"/>
@@ -3225,7 +3221,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A54" s="19"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
@@ -3236,7 +3232,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A55" s="19"/>
       <c r="B55" s="19"/>
       <c r="C55" s="11" t="s">
@@ -3261,7 +3257,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A56" s="19"/>
       <c r="B56" s="19"/>
       <c r="C56" s="20"/>
@@ -3272,7 +3268,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="42.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="41.65" x14ac:dyDescent="0.35">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11" t="s">
@@ -3287,7 +3283,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
       <c r="C58" s="20"/>
@@ -3298,7 +3294,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A59" s="19"/>
       <c r="B59" s="19"/>
       <c r="C59" s="11" t="s">
@@ -3321,7 +3317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A60" s="19"/>
       <c r="B60" s="19"/>
       <c r="C60" s="20"/>
@@ -3330,7 +3326,7 @@
       <c r="F60" s="37"/>
       <c r="G60" s="37"/>
     </row>
-    <row r="61" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A61" s="19"/>
       <c r="B61" s="19"/>
       <c r="C61" s="20"/>
@@ -3348,22 +3344,22 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="75" t="s">
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="73" t="s">
+      <c r="C63" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="80"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A64" s="75" t="s">
         <v>10</v>
       </c>
@@ -3371,89 +3367,89 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
+      <c r="D64" s="81"/>
+      <c r="E64" s="81"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A65" s="75" t="s">
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="74" t="s">
+      <c r="C65" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="81"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A66" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="74" t="s">
+      <c r="C66" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="81"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A67" s="75" t="s">
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="74" t="s">
+      <c r="C67" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
+      <c r="D67" s="81"/>
+      <c r="E67" s="81"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A68" s="75" t="s">
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="74" t="s">
+      <c r="C68" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
+      <c r="D68" s="81"/>
+      <c r="E68" s="81"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A69" s="75" t="s">
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="74" t="s">
+      <c r="C69" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
+      <c r="D69" s="81"/>
+      <c r="E69" s="81"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A70" s="38"/>
       <c r="B70" s="38"/>
       <c r="C70" s="39"/>
@@ -3462,7 +3458,7 @@
       <c r="F70" s="40"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -3471,7 +3467,7 @@
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
     </row>
-    <row r="72" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -3480,7 +3476,7 @@
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
     </row>
-    <row r="73" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -3489,7 +3485,7 @@
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
     </row>
-    <row r="74" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -3498,7 +3494,7 @@
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
     </row>
-    <row r="75" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -3507,7 +3503,7 @@
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
     </row>
-    <row r="76" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -3516,7 +3512,7 @@
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
     </row>
-    <row r="77" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -3525,7 +3521,7 @@
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
     </row>
-    <row r="78" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -3534,7 +3530,7 @@
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
     </row>
-    <row r="79" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -3543,7 +3539,7 @@
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
     </row>
-    <row r="80" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -3552,7 +3548,7 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
     </row>
-    <row r="81" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -3561,7 +3557,7 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
     </row>
-    <row r="82" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -3570,7 +3566,7 @@
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -3579,7 +3575,7 @@
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
     </row>
-    <row r="84" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -3588,7 +3584,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
     </row>
-    <row r="85" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -3597,7 +3593,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -3606,7 +3602,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -3615,7 +3611,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -3624,7 +3620,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -3633,7 +3629,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -3642,7 +3638,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -3651,7 +3647,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -3660,7 +3656,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -3669,7 +3665,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -3678,7 +3674,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -3687,7 +3683,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -3696,7 +3692,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="C97" s="6"/>
@@ -3705,7 +3701,7 @@
       <c r="F97" s="6"/>
       <c r="G97" s="6"/>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -3714,7 +3710,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="59" t="s">
         <v>45</v>
       </c>
@@ -3725,10 +3721,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="72" t="s">
+      <c r="E99" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F99" s="72"/>
+      <c r="F99" s="79"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3742,7 +3738,7 @@
       <c r="Q99" s="50"/>
       <c r="R99" s="50"/>
     </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A100" s="60" t="s">
         <v>46</v>
       </c>
@@ -3770,7 +3766,7 @@
       <c r="Q100" s="50"/>
       <c r="R100" s="50"/>
     </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="D101" s="61" t="s">
         <v>32</v>
       </c>
@@ -3791,7 +3787,7 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="62"/>
       <c r="B102" s="62"/>
       <c r="C102" s="63"/>
@@ -3815,7 +3811,7 @@
       <c r="Q102" s="50"/>
       <c r="R102" s="50"/>
     </row>
-    <row r="103" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="B103" s="60"/>
       <c r="C103" s="60"/>
       <c r="D103" s="64" t="s">
@@ -3838,7 +3834,7 @@
       <c r="Q103" s="50"/>
       <c r="R103" s="50"/>
     </row>
-    <row r="104" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A104" s="60" t="s">
         <v>54</v>
       </c>
@@ -3861,15 +3857,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3883,14 +3878,15 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3906,23 +3902,25 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R102"/>
+  <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.69140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.69140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.3828125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.15234375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.23046875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.15234375" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -3936,7 +3934,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -3945,7 +3943,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -3958,7 +3956,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -3971,7 +3969,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -3988,7 +3986,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -3997,7 +3995,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -4006,18 +4004,18 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" ht="17.600000000000001" x14ac:dyDescent="0.35">
-      <c r="A8" s="79" t="s">
+    <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
+      <c r="A8" s="76" t="s">
         <v>109</v>
       </c>
-      <c r="B8" s="79"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -4026,11 +4024,11 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="81" t="s">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>59</v>
       </c>
@@ -4044,10 +4042,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>60</v>
       </c>
@@ -4056,11 +4054,11 @@
       <c r="F11" s="56"/>
       <c r="G11" s="57"/>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="81" t="s">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>62</v>
       </c>
@@ -4069,11 +4067,11 @@
       <c r="F12" s="6"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="81" t="s">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>63</v>
       </c>
@@ -4082,11 +4080,11 @@
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="81" t="s">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>61</v>
       </c>
@@ -4095,11 +4093,11 @@
       <c r="F14" s="6"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81" t="s">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
         <v>139</v>
       </c>
@@ -4108,7 +4106,7 @@
       <c r="F15" s="6"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4117,7 +4115,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4134,11 +4132,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="76" t="s">
+    <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -4151,9 +4149,9 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+    <row r="19" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
         <v>142</v>
       </c>
@@ -4164,9 +4162,9 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+    <row r="20" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
         <v>143</v>
       </c>
@@ -4177,9 +4175,9 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+    <row r="21" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
         <v>144</v>
       </c>
@@ -4192,15 +4190,14 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="78"/>
-      <c r="B22" s="78"/>
+    <row r="22" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="11">
-        <f>SUM(D18:D21)</f>
-        <v>0</v>
+        <v>145</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>146</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -4208,566 +4205,597 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+    <row r="23" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="74"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="11">
+        <f>SUM(D18:D22)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F24" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>7</v>
-      </c>
+    <row r="24" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="76" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25" s="76" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D25" s="66" t="s">
-        <v>115</v>
-      </c>
-      <c r="E25" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
+    <row r="25" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
+    <row r="26" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="72" t="s">
+        <v>28</v>
+      </c>
       <c r="C26" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="68" t="s">
-        <v>122</v>
+        <v>141</v>
+      </c>
+      <c r="D26" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="67" t="s">
+        <v>116</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
+    <row r="27" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E27" s="68" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+    <row r="28" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="78"/>
-      <c r="B29" s="78"/>
+    <row r="29" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="46">
-        <f>SUM(D25:D28)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="47">
-        <f>SUM(E25:E28)</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+        <v>144</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+    <row r="30" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="68" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>7</v>
-      </c>
+    <row r="31" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="74"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="46">
+        <f>SUM(D26:D30)</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="47">
+        <f>SUM(E26:E30)</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="76" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="76" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D32" s="66" t="s">
-        <v>117</v>
-      </c>
-      <c r="E32" s="67" t="s">
-        <v>118</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
+    <row r="32" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="68" t="s">
-        <v>124</v>
-      </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
+    <row r="33" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
+    <row r="34" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="72" t="s">
+        <v>41</v>
+      </c>
       <c r="C34" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="68" t="s">
-        <v>130</v>
+        <v>141</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>118</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
+    <row r="35" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E35" s="68" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="78"/>
-      <c r="B36" s="78"/>
+    <row r="36" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="73"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D36" s="46">
-        <f>SUM(D32:D35)</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="47">
-        <f>SUM(E32:E35)</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
+        <v>143</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A37" s="19"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="34"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="9"/>
+    <row r="37" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
+      <c r="C37" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="17"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
+    <row r="38" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="73"/>
+      <c r="B38" s="73"/>
+      <c r="C38" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="68" t="s">
+        <v>150</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F39" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>7</v>
-      </c>
+    <row r="39" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="74"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="46">
+        <f>SUM(D34:D38)</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="47">
+        <f>SUM(E34:E38)</f>
+        <v>0</v>
+      </c>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D40" s="66" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="67" t="s">
-        <v>120</v>
-      </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="18"/>
+    <row r="40" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="9"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
-      <c r="C41" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E41" s="67" t="s">
-        <v>126</v>
-      </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="18"/>
+    <row r="41" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="77"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E42" s="67" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="18"/>
+    <row r="42" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F42" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="77"/>
-      <c r="B43" s="77"/>
+    <row r="43" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="72" t="s">
+        <v>42</v>
+      </c>
       <c r="C43" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="D43" s="66" t="s">
+        <v>119</v>
       </c>
       <c r="E43" s="67" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="78"/>
-      <c r="B44" s="78"/>
+    <row r="44" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="73"/>
+      <c r="B44" s="73"/>
       <c r="C44" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D44" s="46">
-        <f>SUM(D40:D43)</f>
-        <v>0</v>
-      </c>
-      <c r="E44" s="47">
-        <f>SUM(E40:E43)</f>
-        <v>0</v>
-      </c>
-      <c r="F44" s="16"/>
-      <c r="G44" s="16"/>
+        <v>142</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="F44" s="17"/>
+      <c r="G44" s="18"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="9"/>
+    <row r="45" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="73"/>
+      <c r="B45" s="73"/>
+      <c r="C45" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="F45" s="17"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="9"/>
+    <row r="46" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="73"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" s="17"/>
+      <c r="G46" s="18"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
+    <row r="47" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="73"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="36">
-        <f>SUM(D22, D29, D36, D44)</f>
-        <v>0</v>
-      </c>
-      <c r="E47" s="35">
-        <f>SUM(E29, E36, E44)</f>
-        <v>0</v>
-      </c>
-      <c r="F47" s="35">
-        <f>SUM(F25:F28, F32:F35, F40:F43)</f>
-        <v>0</v>
-      </c>
-      <c r="G47" s="35">
-        <f>SUM(G25:G28, G32:G35, G40:G43)</f>
-        <v>0</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="14.15" x14ac:dyDescent="0.3">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="54"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-    </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
+    <row r="48" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="74"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="46">
+        <f>SUM(D43:D47)</f>
+        <v>0</v>
+      </c>
+      <c r="E48" s="47">
+        <f>SUM(E43:E47)</f>
+        <v>0</v>
+      </c>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+    </row>
+    <row r="49" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="22"/>
       <c r="G49" s="9"/>
-    </row>
-    <row r="50" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="75" t="s">
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+    </row>
+    <row r="50" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+    </row>
+    <row r="51" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="36">
+        <f>SUM(D23, D31, D39, D48)</f>
+        <v>0</v>
+      </c>
+      <c r="E51" s="35">
+        <f>SUM(E31, E39, E48)</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="35">
+        <f>SUM(F26:F29, F34:F37, F43:F46)</f>
+        <v>0</v>
+      </c>
+      <c r="G51" s="35">
+        <f>SUM(G26:G29, G34:G37, G43:G46)</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+    </row>
+    <row r="52" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A52" s="19"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+    </row>
+    <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A54" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="73" t="s">
+      <c r="B54" s="75"/>
+      <c r="C54" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="73"/>
-      <c r="E50" s="73"/>
-      <c r="F50" s="31" t="s">
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
+      <c r="F54" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G50" s="9"/>
-    </row>
-    <row r="51" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="70" t="s">
+      <c r="G54" s="9"/>
+    </row>
+    <row r="55" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="70" t="s">
         <v>141</v>
       </c>
-      <c r="B51" s="71"/>
-      <c r="C51" s="75" t="s">
+      <c r="B55" s="71"/>
+      <c r="C55" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="23">
+      <c r="D55" s="81"/>
+      <c r="E55" s="81"/>
+      <c r="F55" s="23">
         <v>6108</v>
       </c>
-      <c r="G51" s="9"/>
-    </row>
-    <row r="52" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="70" t="s">
+      <c r="G55" s="9"/>
+    </row>
+    <row r="56" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="70" t="s">
         <v>142</v>
       </c>
-      <c r="B52" s="71"/>
-      <c r="C52" s="75" t="s">
+      <c r="B56" s="71"/>
+      <c r="C56" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D52" s="74"/>
-      <c r="E52" s="74"/>
-      <c r="F52" s="23">
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
+      <c r="F56" s="23">
         <v>5584</v>
       </c>
-      <c r="G52" s="9"/>
-    </row>
-    <row r="53" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="70" t="s">
+      <c r="G56" s="9"/>
+    </row>
+    <row r="57" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="70" t="s">
         <v>143</v>
       </c>
-      <c r="B53" s="71"/>
-      <c r="C53" s="75" t="s">
+      <c r="B57" s="71"/>
+      <c r="C57" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="74"/>
-      <c r="E53" s="74"/>
-      <c r="F53" s="23">
+      <c r="D57" s="81"/>
+      <c r="E57" s="81"/>
+      <c r="F57" s="23">
         <v>5061</v>
       </c>
-      <c r="G53" s="9"/>
-    </row>
-    <row r="54" spans="1:7" ht="13.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="70" t="s">
+      <c r="G57" s="9"/>
+    </row>
+    <row r="58" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="70" t="s">
         <v>144</v>
       </c>
-      <c r="B54" s="71"/>
-      <c r="C54" s="75" t="s">
+      <c r="B58" s="71"/>
+      <c r="C58" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="23">
+      <c r="D58" s="81"/>
+      <c r="E58" s="81"/>
+      <c r="F58" s="23">
         <v>4363</v>
       </c>
-      <c r="G54" s="9"/>
-    </row>
-    <row r="55" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A55" s="38"/>
-      <c r="B55" s="38"/>
-      <c r="C55" s="39"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="39"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="9"/>
-    </row>
-    <row r="56" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-    </row>
-    <row r="57" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A57" s="9"/>
-      <c r="B57" s="9"/>
-      <c r="C57" s="9"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-    </row>
-    <row r="58" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
       <c r="G58" s="9"/>
     </row>
-    <row r="59" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
+    <row r="59" spans="1:9" ht="13.9" x14ac:dyDescent="0.35">
+      <c r="A59" s="38"/>
+      <c r="B59" s="38"/>
+      <c r="C59" s="39"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="40"/>
       <c r="G59" s="9"/>
     </row>
-    <row r="60" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -4776,7 +4804,7 @@
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
     </row>
-    <row r="61" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -4785,7 +4813,7 @@
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
     </row>
-    <row r="62" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -4794,7 +4822,7 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
     </row>
-    <row r="63" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -4803,7 +4831,7 @@
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
     </row>
-    <row r="64" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -4812,7 +4840,7 @@
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
     </row>
-    <row r="65" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -4821,7 +4849,7 @@
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
     </row>
-    <row r="66" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -4830,7 +4858,7 @@
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
     </row>
-    <row r="67" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -4839,7 +4867,7 @@
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
     </row>
-    <row r="68" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -4848,7 +4876,7 @@
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
     </row>
-    <row r="69" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -4857,7 +4885,7 @@
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
     </row>
-    <row r="70" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -4866,43 +4894,43 @@
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="6"/>
-      <c r="G71" s="6"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="6"/>
-      <c r="G73" s="6"/>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6"/>
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+    </row>
+    <row r="72" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+    </row>
+    <row r="73" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+    </row>
+    <row r="74" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="9"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -4911,7 +4939,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -4920,7 +4948,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -4929,7 +4957,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -4938,7 +4966,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -4947,7 +4975,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -4956,7 +4984,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -4965,7 +4993,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -4974,7 +5002,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -4983,7 +5011,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -4992,7 +5020,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -5001,7 +5029,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -5010,7 +5038,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -5019,7 +5047,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -5028,7 +5056,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -5037,7 +5065,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -5046,7 +5074,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -5055,7 +5083,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" ht="11.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -5064,7 +5092,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -5073,7 +5101,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -5082,7 +5110,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -5091,7 +5119,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -5100,118 +5128,58 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="59" t="s">
+    <row r="97" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A98" s="6"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A99" s="6"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+    </row>
+    <row r="101" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="B97" s="59"/>
-      <c r="C97" s="59" t="s">
+      <c r="B101" s="59"/>
+      <c r="C101" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="D97" s="48" t="s">
+      <c r="D101" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E101" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="72"/>
-      <c r="G97" s="49"/>
-      <c r="H97" s="50"/>
-      <c r="I97" s="50"/>
-      <c r="J97" s="50"/>
-      <c r="K97" s="50"/>
-      <c r="L97" s="50"/>
-      <c r="M97" s="50"/>
-      <c r="N97" s="50"/>
-      <c r="O97" s="50"/>
-      <c r="P97" s="50"/>
-      <c r="Q97" s="50"/>
-      <c r="R97" s="50"/>
-    </row>
-    <row r="98" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
-      <c r="A98" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="B98" s="60"/>
-      <c r="C98" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="D98" s="61" t="s">
-        <v>26</v>
-      </c>
-      <c r="E98" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="F98" s="60"/>
-      <c r="G98" s="58"/>
-      <c r="H98" s="50"/>
-      <c r="I98" s="50"/>
-      <c r="J98" s="50"/>
-      <c r="K98" s="50"/>
-      <c r="L98" s="50"/>
-      <c r="M98" s="50"/>
-      <c r="N98" s="50"/>
-      <c r="O98" s="50"/>
-      <c r="P98" s="50"/>
-      <c r="Q98" s="50"/>
-      <c r="R98" s="50"/>
-    </row>
-    <row r="99" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
-      <c r="D99" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="E99" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="F99" s="60"/>
-      <c r="G99" s="53"/>
-      <c r="H99" s="50"/>
-      <c r="I99" s="50"/>
-      <c r="J99" s="50"/>
-      <c r="K99" s="50"/>
-      <c r="L99" s="50"/>
-      <c r="M99" s="50"/>
-      <c r="N99" s="50"/>
-      <c r="O99" s="50"/>
-      <c r="P99" s="50"/>
-      <c r="Q99" s="50"/>
-      <c r="R99" s="50"/>
-    </row>
-    <row r="100" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
-      <c r="A100" s="62"/>
-      <c r="B100" s="62"/>
-      <c r="C100" s="63"/>
-      <c r="D100" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="E100" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="F100" s="60"/>
-      <c r="G100" s="53"/>
-      <c r="H100" s="50"/>
-      <c r="I100" s="50"/>
-      <c r="J100" s="50"/>
-      <c r="K100" s="50"/>
-      <c r="L100" s="50"/>
-      <c r="M100" s="50"/>
-      <c r="N100" s="50"/>
-      <c r="O100" s="50"/>
-      <c r="P100" s="50"/>
-      <c r="Q100" s="50"/>
-      <c r="R100" s="50"/>
-    </row>
-    <row r="101" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
-      <c r="B101" s="60"/>
-      <c r="C101" s="60"/>
-      <c r="D101" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="E101" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="F101" s="60"/>
-      <c r="G101" s="53"/>
+      <c r="F101" s="79"/>
+      <c r="G101" s="49"/>
       <c r="H101" s="50"/>
       <c r="I101" s="50"/>
       <c r="J101" s="50"/>
@@ -5224,16 +5192,22 @@
       <c r="Q101" s="50"/>
       <c r="R101" s="50"/>
     </row>
-    <row r="102" spans="1:18" s="51" customFormat="1" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="B102" s="58"/>
-      <c r="C102" s="58"/>
-      <c r="D102" s="58"/>
-      <c r="E102" s="58"/>
-      <c r="F102" s="58"/>
-      <c r="G102" s="52"/>
+        <v>46</v>
+      </c>
+      <c r="B102" s="60"/>
+      <c r="C102" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D102" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="E102" s="60" t="s">
+        <v>50</v>
+      </c>
+      <c r="F102" s="60"/>
+      <c r="G102" s="58"/>
       <c r="H102" s="50"/>
       <c r="I102" s="50"/>
       <c r="J102" s="50"/>
@@ -5244,32 +5218,123 @@
       <c r="O102" s="50"/>
       <c r="P102" s="50"/>
       <c r="Q102" s="50"/>
+      <c r="R102" s="50"/>
+    </row>
+    <row r="103" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="D103" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="E103" s="60" t="s">
+        <v>49</v>
+      </c>
+      <c r="F103" s="60"/>
+      <c r="G103" s="53"/>
+      <c r="H103" s="50"/>
+      <c r="I103" s="50"/>
+      <c r="J103" s="50"/>
+      <c r="K103" s="50"/>
+      <c r="L103" s="50"/>
+      <c r="M103" s="50"/>
+      <c r="N103" s="50"/>
+      <c r="O103" s="50"/>
+      <c r="P103" s="50"/>
+      <c r="Q103" s="50"/>
+      <c r="R103" s="50"/>
+    </row>
+    <row r="104" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="62"/>
+      <c r="B104" s="62"/>
+      <c r="C104" s="63"/>
+      <c r="D104" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E104" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="F104" s="60"/>
+      <c r="G104" s="53"/>
+      <c r="H104" s="50"/>
+      <c r="I104" s="50"/>
+      <c r="J104" s="50"/>
+      <c r="K104" s="50"/>
+      <c r="L104" s="50"/>
+      <c r="M104" s="50"/>
+      <c r="N104" s="50"/>
+      <c r="O104" s="50"/>
+      <c r="P104" s="50"/>
+      <c r="Q104" s="50"/>
+      <c r="R104" s="50"/>
+    </row>
+    <row r="105" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="B105" s="60"/>
+      <c r="C105" s="60"/>
+      <c r="D105" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="E105" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="F105" s="60"/>
+      <c r="G105" s="53"/>
+      <c r="H105" s="50"/>
+      <c r="I105" s="50"/>
+      <c r="J105" s="50"/>
+      <c r="K105" s="50"/>
+      <c r="L105" s="50"/>
+      <c r="M105" s="50"/>
+      <c r="N105" s="50"/>
+      <c r="O105" s="50"/>
+      <c r="P105" s="50"/>
+      <c r="Q105" s="50"/>
+      <c r="R105" s="50"/>
+    </row>
+    <row r="106" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B106" s="58"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="58"/>
+      <c r="E106" s="58"/>
+      <c r="F106" s="58"/>
+      <c r="G106" s="52"/>
+      <c r="H106" s="50"/>
+      <c r="I106" s="50"/>
+      <c r="J106" s="50"/>
+      <c r="K106" s="50"/>
+      <c r="L106" s="50"/>
+      <c r="M106" s="50"/>
+      <c r="N106" s="50"/>
+      <c r="O106" s="50"/>
+      <c r="P106" s="50"/>
+      <c r="Q106" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="A25:A29"/>
-    <mergeCell ref="B25:B29"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="B40:B44"/>
-    <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="A34:A39"/>
+    <mergeCell ref="B34:B39"/>
+    <mergeCell ref="A43:A48"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="A10:B10"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -5283,21 +5348,21 @@
   </sheetPr>
   <dimension ref="A1:R153"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.69140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.69140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.15234375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.3828125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.15234375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24.23046875" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.15234375" style="2"/>
+    <col min="1" max="1" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.1328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.3984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="22.1328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.19921875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.1328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>39</v>
       </c>
@@ -5311,7 +5376,7 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -5320,7 +5385,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -5333,7 +5398,7 @@
       <c r="F3" s="27"/>
       <c r="G3" s="27"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.4">
       <c r="A4" s="25" t="s">
         <v>1</v>
       </c>
@@ -5346,7 +5411,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
@@ -5363,7 +5428,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -5372,7 +5437,7 @@
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -5381,7 +5446,7 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -5392,7 +5457,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -5403,7 +5468,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="14.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -5414,7 +5479,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -5425,7 +5490,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -5436,7 +5501,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -5447,7 +5512,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -5458,7 +5523,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -5469,7 +5534,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -5480,7 +5545,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -5491,7 +5556,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -5502,7 +5567,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -5513,7 +5578,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -5524,7 +5589,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -5535,7 +5600,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -5546,7 +5611,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
@@ -5555,7 +5620,7 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
@@ -5564,7 +5629,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -5573,7 +5638,7 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
@@ -5582,7 +5647,7 @@
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
@@ -5591,7 +5656,7 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -5600,7 +5665,7 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
@@ -5609,7 +5674,7 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
@@ -5618,7 +5683,7 @@
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
@@ -5627,7 +5692,7 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
@@ -5636,7 +5701,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -5645,7 +5710,7 @@
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
@@ -5654,7 +5719,7 @@
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
@@ -5663,7 +5728,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
@@ -5672,7 +5737,7 @@
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="6"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
@@ -5681,7 +5746,7 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
@@ -5690,7 +5755,7 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
@@ -5699,7 +5764,7 @@
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -5708,7 +5773,7 @@
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
@@ -5717,7 +5782,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
@@ -5726,7 +5791,7 @@
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -5735,7 +5800,7 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
@@ -5744,7 +5809,7 @@
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
@@ -5753,7 +5818,7 @@
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
@@ -5762,7 +5827,7 @@
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
@@ -5771,7 +5836,7 @@
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
@@ -5780,7 +5845,7 @@
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -5789,7 +5854,7 @@
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -5798,7 +5863,7 @@
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -5807,7 +5872,7 @@
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -5816,7 +5881,7 @@
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -5825,7 +5890,7 @@
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -5834,7 +5899,7 @@
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -5843,7 +5908,7 @@
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
@@ -5852,7 +5917,7 @@
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -5861,7 +5926,7 @@
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -5870,7 +5935,7 @@
       <c r="F58" s="6"/>
       <c r="G58" s="6"/>
     </row>
-    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -5879,7 +5944,7 @@
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -5888,7 +5953,7 @@
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -5897,7 +5962,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -5906,7 +5971,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -5915,7 +5980,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -5924,7 +5989,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -5933,7 +5998,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="6"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -5942,7 +6007,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6"/>
@@ -5951,7 +6016,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -5960,7 +6025,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
@@ -5969,7 +6034,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="6"/>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
@@ -5978,7 +6043,7 @@
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
@@ -5987,7 +6052,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
@@ -5996,7 +6061,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
@@ -6005,7 +6070,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
@@ -6014,7 +6079,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
@@ -6023,7 +6088,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -6032,7 +6097,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
@@ -6041,7 +6106,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
@@ -6050,7 +6115,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="6"/>
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
@@ -6059,7 +6124,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
@@ -6068,7 +6133,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
@@ -6077,7 +6142,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -6086,7 +6151,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
@@ -6095,7 +6160,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
@@ -6104,7 +6169,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
@@ -6113,7 +6178,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
@@ -6122,7 +6187,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
@@ -6131,7 +6196,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -6140,7 +6205,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
@@ -6149,7 +6214,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
@@ -6158,7 +6223,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91" s="6"/>
@@ -6167,7 +6232,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
@@ -6176,7 +6241,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
@@ -6185,7 +6250,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="C94" s="6"/>
@@ -6194,7 +6259,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
@@ -6203,7 +6268,7 @@
       <c r="F95" s="6"/>
       <c r="G95" s="6"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
@@ -6212,7 +6277,7 @@
       <c r="F96" s="6"/>
       <c r="G96" s="6"/>
     </row>
-    <row r="97" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A97" s="59" t="s">
         <v>45</v>
       </c>
@@ -6223,13 +6288,13 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E97" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="F97" s="72"/>
+      <c r="F97" s="79"/>
       <c r="G97" s="49"/>
     </row>
-    <row r="98" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A98" s="60" t="s">
         <v>46</v>
       </c>
@@ -6246,7 +6311,7 @@
       <c r="F98" s="60"/>
       <c r="G98" s="58"/>
     </row>
-    <row r="99" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A99" s="51"/>
       <c r="B99" s="51"/>
       <c r="C99" s="51"/>
@@ -6259,7 +6324,7 @@
       <c r="F99" s="60"/>
       <c r="G99" s="53"/>
     </row>
-    <row r="100" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A100" s="62"/>
       <c r="B100" s="62"/>
       <c r="C100" s="63"/>
@@ -6272,7 +6337,7 @@
       <c r="F100" s="60"/>
       <c r="G100" s="53"/>
     </row>
-    <row r="101" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A101" s="51"/>
       <c r="B101" s="60"/>
       <c r="C101" s="60"/>
@@ -6285,7 +6350,7 @@
       <c r="F101" s="60"/>
       <c r="G101" s="53"/>
     </row>
-    <row r="102" spans="1:7" ht="14.15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="60" t="s">
         <v>54</v>
       </c>
@@ -6296,8 +6361,8 @@
       <c r="F102" s="58"/>
       <c r="G102" s="52"/>
     </row>
-    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="148" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -6317,7 +6382,7 @@
       <c r="Q148" s="50"/>
       <c r="R148" s="50"/>
     </row>
-    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -6337,7 +6402,7 @@
       <c r="Q149" s="50"/>
       <c r="R149" s="50"/>
     </row>
-    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -6357,7 +6422,7 @@
       <c r="Q150" s="50"/>
       <c r="R150" s="50"/>
     </row>
-    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -6377,7 +6442,7 @@
       <c r="Q151" s="50"/>
       <c r="R151" s="50"/>
     </row>
-    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -6397,7 +6462,7 @@
       <c r="Q152" s="50"/>
       <c r="R152" s="50"/>
     </row>
-    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" s="51" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -6427,30 +6492,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6594,34 +6639,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6638,10 +6688,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
105173 1619 funding claim template fix
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B61428E-D43C-4794-B578-DF0CB7B71783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C39953-92C1-4506-9F56-14F733239C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="-8580" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>Year:</t>
   </si>
   <si>
-    <t>1920 Condition of Funding Removal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Application Version: </t>
   </si>
   <si>
@@ -492,6 +489,9 @@
   </si>
   <si>
     <t>&amp;=FundingClaim.ContinuingStudentsExcludingEHCPlan.Band1To5TotalFunding</t>
+  </si>
+  <si>
+    <t>2021 Condition of Funding Removal</t>
   </si>
 </sst>
 </file>
@@ -961,6 +961,20 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -970,10 +984,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -981,16 +991,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2446,7 +2446,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="9"/>
@@ -2459,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="9"/>
@@ -2472,7 +2472,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="9"/>
@@ -2481,7 +2481,7 @@
         <v>43</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
@@ -2503,11 +2503,11 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="76" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="77"/>
+      <c r="A8" s="79" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -2523,12 +2523,12 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -2536,16 +2536,16 @@
         <v>19</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -2553,12 +2553,12 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -2566,12 +2566,12 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -2579,12 +2579,12 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -2592,12 +2592,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="78"/>
+      <c r="A15" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2631,56 +2631,56 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -2689,13 +2689,13 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -2704,13 +2704,13 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="73"/>
-      <c r="B23" s="73"/>
+      <c r="A23" s="77"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E23" s="45"/>
       <c r="F23" s="45"/>
@@ -2719,8 +2719,8 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="74"/>
-      <c r="B24" s="74"/>
+      <c r="A24" s="78"/>
+      <c r="B24" s="78"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2765,20 +2765,20 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="72" t="s">
+      <c r="A27" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="72" t="s">
+      <c r="B27" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D27" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -2786,16 +2786,16 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" s="68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -2803,16 +2803,16 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="68" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
@@ -2820,16 +2820,16 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
@@ -2837,16 +2837,16 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="73"/>
-      <c r="B31" s="73"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
@@ -2854,16 +2854,16 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="73"/>
-      <c r="B32" s="73"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" s="69" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F32" s="16"/>
       <c r="G32" s="16"/>
@@ -2871,8 +2871,8 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
+      <c r="A33" s="78"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2920,20 +2920,20 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="72" t="s">
+      <c r="A36" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="66" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
@@ -2941,16 +2941,16 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E37" s="68" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
@@ -2958,16 +2958,16 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E38" s="68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
@@ -2975,16 +2975,16 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="73"/>
-      <c r="B39" s="73"/>
+      <c r="A39" s="77"/>
+      <c r="B39" s="77"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E39" s="68" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
@@ -2992,16 +2992,16 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="73"/>
-      <c r="B40" s="73"/>
+      <c r="A40" s="77"/>
+      <c r="B40" s="77"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E40" s="68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
@@ -3009,16 +3009,16 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="73"/>
-      <c r="B41" s="73"/>
+      <c r="A41" s="77"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" s="69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
@@ -3026,8 +3026,8 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="74"/>
-      <c r="B42" s="74"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="78"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3086,20 +3086,20 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="72" t="s">
+      <c r="B46" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
@@ -3107,16 +3107,16 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E47" s="67" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
@@ -3124,16 +3124,16 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="73"/>
-      <c r="B48" s="73"/>
+      <c r="A48" s="77"/>
+      <c r="B48" s="77"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E48" s="67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
@@ -3141,16 +3141,16 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="73"/>
-      <c r="B49" s="73"/>
+      <c r="A49" s="77"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E49" s="67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="18"/>
@@ -3158,16 +3158,16 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="73"/>
-      <c r="B50" s="73"/>
+      <c r="A50" s="77"/>
+      <c r="B50" s="77"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E50" s="67" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="18"/>
@@ -3175,16 +3175,16 @@
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="73"/>
-      <c r="B51" s="73"/>
+      <c r="A51" s="77"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E51" s="69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="18"/>
@@ -3192,8 +3192,8 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="74"/>
-      <c r="B52" s="74"/>
+      <c r="A52" s="78"/>
+      <c r="B52" s="78"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3272,11 +3272,11 @@
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11" t="s">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="13"/>
@@ -3349,11 +3349,11 @@
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="80" t="s">
+      <c r="C63" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="80"/>
-      <c r="E63" s="80"/>
+      <c r="D63" s="73"/>
+      <c r="E63" s="73"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
@@ -3367,8 +3367,8 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="81"/>
-      <c r="E64" s="81"/>
+      <c r="D64" s="74"/>
+      <c r="E64" s="74"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
@@ -3379,11 +3379,11 @@
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="81" t="s">
+      <c r="C65" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="81"/>
-      <c r="E65" s="81"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="74"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
@@ -3394,11 +3394,11 @@
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="81" t="s">
+      <c r="C66" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="81"/>
-      <c r="E66" s="81"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
@@ -3409,11 +3409,11 @@
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="81" t="s">
+      <c r="C67" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="81"/>
-      <c r="E67" s="81"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
@@ -3424,11 +3424,11 @@
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="81" t="s">
+      <c r="C68" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="81"/>
-      <c r="E68" s="81"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
@@ -3439,11 +3439,11 @@
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="81" t="s">
+      <c r="C69" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="81"/>
-      <c r="E69" s="81"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="74"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
@@ -3712,19 +3712,19 @@
     </row>
     <row r="99" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B99" s="59"/>
       <c r="C99" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="F99" s="79"/>
+      <c r="E99" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="F99" s="72"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3740,17 +3740,17 @@
     </row>
     <row r="100" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A100" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B100" s="60"/>
       <c r="C100" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D100" s="61" t="s">
         <v>26</v>
       </c>
       <c r="E100" s="60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F100" s="60"/>
       <c r="G100" s="58"/>
@@ -3771,7 +3771,7 @@
         <v>32</v>
       </c>
       <c r="E101" s="60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F101" s="60"/>
       <c r="G101" s="53"/>
@@ -3795,7 +3795,7 @@
         <v>27</v>
       </c>
       <c r="E102" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F102" s="60"/>
       <c r="G102" s="53"/>
@@ -3818,7 +3818,7 @@
         <v>30</v>
       </c>
       <c r="E103" s="60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F103" s="60"/>
       <c r="G103" s="53"/>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="104" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A104" s="60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B104" s="58"/>
       <c r="C104" s="58"/>
@@ -3857,14 +3857,15 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3878,15 +3879,14 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3948,7 +3948,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="9"/>
@@ -3961,7 +3961,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="9"/>
@@ -3974,7 +3974,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="9"/>
@@ -3983,7 +3983,7 @@
         <v>43</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
@@ -4005,10 +4005,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="76"/>
+      <c r="A8" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="79"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -4025,12 +4025,12 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="78" t="s">
+      <c r="A10" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="78"/>
+      <c r="B10" s="81"/>
       <c r="C10" s="32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
@@ -4038,16 +4038,16 @@
         <v>19</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="78"/>
+      <c r="B11" s="81"/>
       <c r="C11" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -4055,12 +4055,12 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="78"/>
+      <c r="B12" s="81"/>
       <c r="C12" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -4068,12 +4068,12 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="78"/>
+      <c r="B13" s="81"/>
       <c r="C13" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -4081,12 +4081,12 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="78"/>
+      <c r="B14" s="81"/>
       <c r="C14" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -4094,12 +4094,12 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="78" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="78"/>
+      <c r="A15" s="81" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="81"/>
       <c r="C15" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4133,56 +4133,56 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="72" t="s">
+      <c r="A18" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="76" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D18" s="66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="73"/>
-      <c r="B19" s="73"/>
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
       <c r="C19" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="73"/>
-      <c r="B20" s="73"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="73"/>
-      <c r="B21" s="73"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
@@ -4191,13 +4191,13 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="73"/>
-      <c r="B22" s="73"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>145</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>146</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -4206,8 +4206,8 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="74"/>
-      <c r="B23" s="74"/>
+      <c r="A23" s="78"/>
+      <c r="B23" s="78"/>
       <c r="C23" s="11" t="s">
         <v>29</v>
       </c>
@@ -4252,20 +4252,20 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="72" t="s">
+      <c r="A26" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="72" t="s">
+      <c r="B26" s="76" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D26" s="66" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="67" t="s">
         <v>115</v>
-      </c>
-      <c r="E26" s="67" t="s">
-        <v>116</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
@@ -4273,16 +4273,16 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="73"/>
-      <c r="B27" s="73"/>
+      <c r="A27" s="77"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D27" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" s="68" t="s">
         <v>121</v>
-      </c>
-      <c r="E27" s="68" t="s">
-        <v>122</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
@@ -4290,16 +4290,16 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="73"/>
-      <c r="B28" s="73"/>
+      <c r="A28" s="77"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D28" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28" s="68" t="s">
         <v>127</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>128</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
@@ -4307,16 +4307,16 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="73"/>
-      <c r="B29" s="73"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D29" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E29" s="68" t="s">
         <v>133</v>
-      </c>
-      <c r="E29" s="68" t="s">
-        <v>134</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
@@ -4324,16 +4324,16 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="73"/>
-      <c r="B30" s="73"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D30" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E30" s="68" t="s">
         <v>147</v>
-      </c>
-      <c r="E30" s="68" t="s">
-        <v>148</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
@@ -4341,8 +4341,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="74"/>
-      <c r="B31" s="74"/>
+      <c r="A31" s="78"/>
+      <c r="B31" s="78"/>
       <c r="C31" s="11" t="s">
         <v>29</v>
       </c>
@@ -4390,20 +4390,20 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="76" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D34" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" s="67" t="s">
         <v>117</v>
-      </c>
-      <c r="E34" s="67" t="s">
-        <v>118</v>
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
@@ -4411,16 +4411,16 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
+      <c r="A35" s="77"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D35" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="68" t="s">
         <v>123</v>
-      </c>
-      <c r="E35" s="68" t="s">
-        <v>124</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
@@ -4428,16 +4428,16 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="73"/>
-      <c r="B36" s="73"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D36" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36" s="68" t="s">
         <v>129</v>
-      </c>
-      <c r="E36" s="68" t="s">
-        <v>130</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
@@ -4445,16 +4445,16 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="73"/>
-      <c r="B37" s="73"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D37" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="68" t="s">
         <v>135</v>
-      </c>
-      <c r="E37" s="68" t="s">
-        <v>136</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
@@ -4462,16 +4462,16 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="73"/>
-      <c r="B38" s="73"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D38" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="68" t="s">
         <v>149</v>
-      </c>
-      <c r="E38" s="68" t="s">
-        <v>150</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
@@ -4479,8 +4479,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="74"/>
-      <c r="B39" s="74"/>
+      <c r="A39" s="78"/>
+      <c r="B39" s="78"/>
       <c r="C39" s="11" t="s">
         <v>29</v>
       </c>
@@ -4539,20 +4539,20 @@
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="72" t="s">
+      <c r="A43" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="72" t="s">
+      <c r="B43" s="76" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D43" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="67" t="s">
         <v>119</v>
-      </c>
-      <c r="E43" s="67" t="s">
-        <v>120</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
@@ -4560,16 +4560,16 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="73"/>
-      <c r="B44" s="73"/>
+      <c r="A44" s="77"/>
+      <c r="B44" s="77"/>
       <c r="C44" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D44" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="67" t="s">
         <v>125</v>
-      </c>
-      <c r="E44" s="67" t="s">
-        <v>126</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
@@ -4577,16 +4577,16 @@
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="73"/>
-      <c r="B45" s="73"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="77"/>
       <c r="C45" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D45" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E45" s="67" t="s">
         <v>131</v>
-      </c>
-      <c r="E45" s="67" t="s">
-        <v>132</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
@@ -4594,16 +4594,16 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="73"/>
-      <c r="B46" s="73"/>
+      <c r="A46" s="77"/>
+      <c r="B46" s="77"/>
       <c r="C46" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D46" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="67" t="s">
         <v>137</v>
-      </c>
-      <c r="E46" s="67" t="s">
-        <v>138</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
@@ -4611,16 +4611,16 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="73"/>
-      <c r="B47" s="73"/>
+      <c r="A47" s="77"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D47" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="E47" s="67" t="s">
         <v>151</v>
-      </c>
-      <c r="E47" s="67" t="s">
-        <v>152</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
@@ -4628,8 +4628,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="74"/>
-      <c r="B48" s="74"/>
+      <c r="A48" s="78"/>
+      <c r="B48" s="78"/>
       <c r="C48" s="11" t="s">
         <v>29</v>
       </c>
@@ -4716,11 +4716,11 @@
         <v>5</v>
       </c>
       <c r="B54" s="75"/>
-      <c r="C54" s="80" t="s">
+      <c r="C54" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="80"/>
-      <c r="E54" s="80"/>
+      <c r="D54" s="73"/>
+      <c r="E54" s="73"/>
       <c r="F54" s="31" t="s">
         <v>4</v>
       </c>
@@ -4728,14 +4728,14 @@
     </row>
     <row r="55" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B55" s="71"/>
       <c r="C55" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="D55" s="81"/>
-      <c r="E55" s="81"/>
+        <v>139</v>
+      </c>
+      <c r="D55" s="74"/>
+      <c r="E55" s="74"/>
       <c r="F55" s="23">
         <v>6108</v>
       </c>
@@ -4743,14 +4743,14 @@
     </row>
     <row r="56" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B56" s="71"/>
       <c r="C56" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="D56" s="81"/>
-      <c r="E56" s="81"/>
+        <v>139</v>
+      </c>
+      <c r="D56" s="74"/>
+      <c r="E56" s="74"/>
       <c r="F56" s="23">
         <v>5584</v>
       </c>
@@ -4758,14 +4758,14 @@
     </row>
     <row r="57" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B57" s="71"/>
       <c r="C57" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" s="81"/>
-      <c r="E57" s="81"/>
+        <v>139</v>
+      </c>
+      <c r="D57" s="74"/>
+      <c r="E57" s="74"/>
       <c r="F57" s="23">
         <v>5061</v>
       </c>
@@ -4773,14 +4773,14 @@
     </row>
     <row r="58" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B58" s="71"/>
       <c r="C58" s="75" t="s">
-        <v>140</v>
-      </c>
-      <c r="D58" s="81"/>
-      <c r="E58" s="81"/>
+        <v>139</v>
+      </c>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
       <c r="F58" s="23">
         <v>4363</v>
       </c>
@@ -5166,19 +5166,19 @@
     </row>
     <row r="101" spans="1:18" s="51" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B101" s="59"/>
       <c r="C101" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D101" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E101" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="F101" s="79"/>
+      <c r="E101" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="F101" s="72"/>
       <c r="G101" s="49"/>
       <c r="H101" s="50"/>
       <c r="I101" s="50"/>
@@ -5194,17 +5194,17 @@
     </row>
     <row r="102" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B102" s="60"/>
       <c r="C102" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D102" s="61" t="s">
         <v>26</v>
       </c>
       <c r="E102" s="60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F102" s="60"/>
       <c r="G102" s="58"/>
@@ -5225,7 +5225,7 @@
         <v>32</v>
       </c>
       <c r="E103" s="60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F103" s="60"/>
       <c r="G103" s="53"/>
@@ -5249,7 +5249,7 @@
         <v>27</v>
       </c>
       <c r="E104" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F104" s="60"/>
       <c r="G104" s="53"/>
@@ -5272,7 +5272,7 @@
         <v>30</v>
       </c>
       <c r="E105" s="60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F105" s="60"/>
       <c r="G105" s="53"/>
@@ -5290,7 +5290,7 @@
     </row>
     <row r="106" spans="1:18" s="51" customFormat="1" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A106" s="60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B106" s="58"/>
       <c r="C106" s="58"/>
@@ -5311,12 +5311,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
     <mergeCell ref="E101:F101"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5333,6 +5327,12 @@
     <mergeCell ref="A43:A48"/>
     <mergeCell ref="B43:B48"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -5390,7 +5390,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="9"/>
@@ -5403,7 +5403,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="9"/>
@@ -5416,7 +5416,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="9"/>
@@ -5425,7 +5425,7 @@
         <v>43</v>
       </c>
       <c r="G5" s="65" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
@@ -6279,34 +6279,34 @@
     </row>
     <row r="97" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A97" s="59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B97" s="59"/>
       <c r="C97" s="59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="79" t="s">
-        <v>51</v>
-      </c>
-      <c r="F97" s="79"/>
+      <c r="E97" s="72" t="s">
+        <v>50</v>
+      </c>
+      <c r="F97" s="72"/>
       <c r="G97" s="49"/>
     </row>
     <row r="98" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A98" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B98" s="60"/>
       <c r="C98" s="60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D98" s="61" t="s">
         <v>26</v>
       </c>
       <c r="E98" s="60" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F98" s="60"/>
       <c r="G98" s="58"/>
@@ -6319,7 +6319,7 @@
         <v>32</v>
       </c>
       <c r="E99" s="60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F99" s="60"/>
       <c r="G99" s="53"/>
@@ -6332,7 +6332,7 @@
         <v>27</v>
       </c>
       <c r="E100" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F100" s="60"/>
       <c r="G100" s="53"/>
@@ -6345,14 +6345,14 @@
         <v>30</v>
       </c>
       <c r="E101" s="60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F101" s="60"/>
       <c r="G101" s="53"/>
     </row>
     <row r="102" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A102" s="60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B102" s="58"/>
       <c r="C102" s="58"/>
@@ -6492,10 +6492,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6639,39 +6659,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6688,25 +6703,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
105469 1619FundingClaim - TLevel learners fixed
</commit_message>
<xml_diff>
--- a/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
+++ b/src/ESFA.DC.ILR.ReportService.Reports/Templates/FundingClaim1619ReportTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C39953-92C1-4506-9F56-14F733239C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB841E65-995F-4957-BF93-A01025649018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study Programmes" sheetId="3" r:id="rId1"/>
@@ -470,28 +470,28 @@
     <t>Band 5 and below</t>
   </si>
   <si>
-    <t>&amp;=FundingClaim.DirectFundingStudents.Band1To5StudentNumbers</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaim.StudentsIncludingHNS.Band1To5StudentNumbers</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaim.StudentsIncludingHNS.Band1To5TotalFunding</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaim.StudentsWithEHCPlan.Band1To5StudentNumbers</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaim.StudentsWithEHCPlan.Band1To5TotalFunding</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaim.ContinuingStudentsExcludingEHCPlan.Band1To5StudentNumbers</t>
-  </si>
-  <si>
-    <t>&amp;=FundingClaim.ContinuingStudentsExcludingEHCPlan.Band1To5TotalFunding</t>
-  </si>
-  <si>
     <t>2021 Condition of Funding Removal</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.DirectFundingStudents.Band1To5StudentNumbersTLevel</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsIncludingHNS.Band1To5StudentNumbersTLevel</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsIncludingHNS.Band1To5TotalFundingTLevel</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsWithEHCPlan.Band1To5StudentNumbersTLevel</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.StudentsWithEHCPlan.Band1To5TotalFundingTLevel</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.ContinuingStudentsExcludingEHCPlan.Band1To5StudentNumbersTLevel</t>
+  </si>
+  <si>
+    <t>&amp;=FundingClaim.ContinuingStudentsExcludingEHCPlan.Band1To5TotalFundingTLevel</t>
   </si>
 </sst>
 </file>
@@ -961,20 +961,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -984,6 +970,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -991,6 +981,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2404,7 +2404,9 @@
   </sheetPr>
   <dimension ref="A1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2503,11 +2505,11 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="79"/>
-      <c r="C8" s="80"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
@@ -2523,10 +2525,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>58</v>
       </c>
@@ -2540,10 +2542,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>59</v>
       </c>
@@ -2553,10 +2555,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>61</v>
       </c>
@@ -2566,10 +2568,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>62</v>
       </c>
@@ -2579,10 +2581,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>60</v>
       </c>
@@ -2592,10 +2594,10 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
         <v>138</v>
       </c>
@@ -2631,10 +2633,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -2648,8 +2650,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
         <v>11</v>
       </c>
@@ -2661,8 +2663,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
         <v>12</v>
       </c>
@@ -2674,8 +2676,8 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
         <v>13</v>
       </c>
@@ -2689,8 +2691,8 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="11" t="s">
         <v>14</v>
       </c>
@@ -2704,8 +2706,8 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="77"/>
-      <c r="B23" s="77"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="73"/>
       <c r="C23" s="43" t="s">
         <v>15</v>
       </c>
@@ -2719,8 +2721,8 @@
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="78"/>
-      <c r="B24" s="78"/>
+      <c r="A24" s="74"/>
+      <c r="B24" s="74"/>
       <c r="C24" s="11" t="s">
         <v>29</v>
       </c>
@@ -2765,10 +2767,10 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="76" t="s">
+      <c r="A27" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="76" t="s">
+      <c r="B27" s="72" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="11" t="s">
@@ -2786,8 +2788,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
         <v>11</v>
       </c>
@@ -2803,8 +2805,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="77"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="11" t="s">
         <v>12</v>
       </c>
@@ -2820,8 +2822,8 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -2837,8 +2839,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="77"/>
-      <c r="B31" s="77"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
       <c r="C31" s="11" t="s">
         <v>14</v>
       </c>
@@ -2854,8 +2856,8 @@
       <c r="I31" s="1"/>
     </row>
     <row r="32" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="77"/>
-      <c r="B32" s="77"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
       <c r="C32" s="11" t="s">
         <v>15</v>
       </c>
@@ -2871,8 +2873,8 @@
       <c r="I32" s="1"/>
     </row>
     <row r="33" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="78"/>
-      <c r="B33" s="78"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="74"/>
       <c r="C33" s="11" t="s">
         <v>29</v>
       </c>
@@ -2920,10 +2922,10 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="76" t="s">
+      <c r="A36" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="76" t="s">
+      <c r="B36" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="11" t="s">
@@ -2941,8 +2943,8 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="77"/>
-      <c r="B37" s="77"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="11" t="s">
         <v>11</v>
       </c>
@@ -2958,8 +2960,8 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="73"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="11" t="s">
         <v>12</v>
       </c>
@@ -2975,8 +2977,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
+      <c r="A39" s="73"/>
+      <c r="B39" s="73"/>
       <c r="C39" s="11" t="s">
         <v>13</v>
       </c>
@@ -2992,8 +2994,8 @@
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="73"/>
       <c r="C40" s="11" t="s">
         <v>14</v>
       </c>
@@ -3009,8 +3011,8 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
       <c r="C41" s="11" t="s">
         <v>15</v>
       </c>
@@ -3026,8 +3028,8 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="78"/>
-      <c r="B42" s="78"/>
+      <c r="A42" s="74"/>
+      <c r="B42" s="74"/>
       <c r="C42" s="11" t="s">
         <v>29</v>
       </c>
@@ -3086,10 +3088,10 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="76" t="s">
+      <c r="A46" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B46" s="76" t="s">
+      <c r="B46" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="11" t="s">
@@ -3107,8 +3109,8 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="77"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="11" t="s">
         <v>11</v>
       </c>
@@ -3124,8 +3126,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="77"/>
-      <c r="B48" s="77"/>
+      <c r="A48" s="73"/>
+      <c r="B48" s="73"/>
       <c r="C48" s="11" t="s">
         <v>12</v>
       </c>
@@ -3141,8 +3143,8 @@
       <c r="I48" s="1"/>
     </row>
     <row r="49" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="77"/>
-      <c r="B49" s="77"/>
+      <c r="A49" s="73"/>
+      <c r="B49" s="73"/>
       <c r="C49" s="11" t="s">
         <v>13</v>
       </c>
@@ -3158,8 +3160,8 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="77"/>
-      <c r="B50" s="77"/>
+      <c r="A50" s="73"/>
+      <c r="B50" s="73"/>
       <c r="C50" s="11" t="s">
         <v>14</v>
       </c>
@@ -3175,8 +3177,8 @@
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="77"/>
-      <c r="B51" s="77"/>
+      <c r="A51" s="73"/>
+      <c r="B51" s="73"/>
       <c r="C51" s="11" t="s">
         <v>15</v>
       </c>
@@ -3192,8 +3194,8 @@
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="78"/>
-      <c r="B52" s="78"/>
+      <c r="A52" s="74"/>
+      <c r="B52" s="74"/>
       <c r="C52" s="11" t="s">
         <v>29</v>
       </c>
@@ -3272,7 +3274,7 @@
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
       <c r="C57" s="11" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="35" t="s">
@@ -3349,11 +3351,11 @@
         <v>5</v>
       </c>
       <c r="B63" s="75"/>
-      <c r="C63" s="73" t="s">
+      <c r="C63" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D63" s="73"/>
-      <c r="E63" s="73"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="80"/>
       <c r="F63" s="31" t="s">
         <v>4</v>
       </c>
@@ -3367,8 +3369,8 @@
       <c r="C64" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="74"/>
-      <c r="E64" s="74"/>
+      <c r="D64" s="81"/>
+      <c r="E64" s="81"/>
       <c r="F64" s="23">
         <v>4188</v>
       </c>
@@ -3379,11 +3381,11 @@
         <v>11</v>
       </c>
       <c r="B65" s="75"/>
-      <c r="C65" s="74" t="s">
+      <c r="C65" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="D65" s="74"/>
-      <c r="E65" s="74"/>
+      <c r="D65" s="81"/>
+      <c r="E65" s="81"/>
       <c r="F65" s="23">
         <v>3455</v>
       </c>
@@ -3394,11 +3396,11 @@
         <v>12</v>
       </c>
       <c r="B66" s="75"/>
-      <c r="C66" s="74" t="s">
+      <c r="C66" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="74"/>
-      <c r="E66" s="74"/>
+      <c r="D66" s="81"/>
+      <c r="E66" s="81"/>
       <c r="F66" s="23">
         <v>3455</v>
       </c>
@@ -3409,11 +3411,11 @@
         <v>13</v>
       </c>
       <c r="B67" s="75"/>
-      <c r="C67" s="74" t="s">
+      <c r="C67" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
+      <c r="D67" s="81"/>
+      <c r="E67" s="81"/>
       <c r="F67" s="23">
         <v>2827</v>
       </c>
@@ -3424,11 +3426,11 @@
         <v>14</v>
       </c>
       <c r="B68" s="75"/>
-      <c r="C68" s="74" t="s">
+      <c r="C68" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
+      <c r="D68" s="81"/>
+      <c r="E68" s="81"/>
       <c r="F68" s="23">
         <v>2234</v>
       </c>
@@ -3439,11 +3441,11 @@
         <v>15</v>
       </c>
       <c r="B69" s="75"/>
-      <c r="C69" s="74" t="s">
+      <c r="C69" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
+      <c r="D69" s="81"/>
+      <c r="E69" s="81"/>
       <c r="F69" s="23">
         <v>4188</v>
       </c>
@@ -3721,10 +3723,10 @@
       <c r="D99" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E99" s="72" t="s">
+      <c r="E99" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="F99" s="72"/>
+      <c r="F99" s="79"/>
       <c r="G99" s="49"/>
       <c r="H99" s="50"/>
       <c r="I99" s="50"/>
@@ -3857,15 +3859,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:B52"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="C68:E68"/>
     <mergeCell ref="A27:A33"/>
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A36:A42"/>
@@ -3879,14 +3880,15 @@
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="B46:B52"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="38" orientation="portrait" r:id="rId1"/>
@@ -3904,9 +3906,7 @@
   </sheetPr>
   <dimension ref="A1:R106"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4005,10 +4005,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="17.649999999999999" x14ac:dyDescent="0.35">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="76" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="79"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="30"/>
       <c r="D8" s="30"/>
       <c r="E8" s="30"/>
@@ -4025,10 +4025,10 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="32" t="s">
         <v>58</v>
       </c>
@@ -4042,10 +4042,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="81"/>
+      <c r="B11" s="78"/>
       <c r="C11" s="32" t="s">
         <v>59</v>
       </c>
@@ -4055,10 +4055,10 @@
       <c r="G11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="32" t="s">
         <v>61</v>
       </c>
@@ -4068,10 +4068,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="81"/>
+      <c r="B13" s="78"/>
       <c r="C13" s="32" t="s">
         <v>62</v>
       </c>
@@ -4081,10 +4081,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="81"/>
+      <c r="B14" s="78"/>
       <c r="C14" s="32" t="s">
         <v>60</v>
       </c>
@@ -4094,10 +4094,10 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="81" t="s">
+      <c r="A15" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="32" t="s">
         <v>138</v>
       </c>
@@ -4133,10 +4133,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="76" t="s">
+      <c r="B18" s="72" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="11" t="s">
@@ -4150,8 +4150,8 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="77"/>
-      <c r="B19" s="77"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="11" t="s">
         <v>141</v>
       </c>
@@ -4163,8 +4163,8 @@
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="77"/>
-      <c r="B20" s="77"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="73"/>
       <c r="C20" s="11" t="s">
         <v>142</v>
       </c>
@@ -4176,8 +4176,8 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="77"/>
-      <c r="B21" s="77"/>
+      <c r="A21" s="73"/>
+      <c r="B21" s="73"/>
       <c r="C21" s="11" t="s">
         <v>143</v>
       </c>
@@ -4191,13 +4191,13 @@
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="77"/>
-      <c r="B22" s="77"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="73"/>
       <c r="C22" s="11" t="s">
         <v>144</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
@@ -4206,8 +4206,8 @@
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="78"/>
-      <c r="B23" s="78"/>
+      <c r="A23" s="74"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="11" t="s">
         <v>29</v>
       </c>
@@ -4252,10 +4252,10 @@
       <c r="I25" s="1"/>
     </row>
     <row r="26" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="76" t="s">
+      <c r="A26" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="72" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="11" t="s">
@@ -4273,8 +4273,8 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="73"/>
       <c r="C27" s="11" t="s">
         <v>141</v>
       </c>
@@ -4290,8 +4290,8 @@
       <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
+      <c r="A28" s="73"/>
+      <c r="B28" s="73"/>
       <c r="C28" s="11" t="s">
         <v>142</v>
       </c>
@@ -4307,8 +4307,8 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="77"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="73"/>
       <c r="C29" s="11" t="s">
         <v>143</v>
       </c>
@@ -4324,16 +4324,16 @@
       <c r="I29" s="1"/>
     </row>
     <row r="30" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="77"/>
-      <c r="B30" s="77"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
       <c r="C30" s="11" t="s">
         <v>144</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E30" s="68" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
@@ -4341,8 +4341,8 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="78"/>
-      <c r="B31" s="78"/>
+      <c r="A31" s="74"/>
+      <c r="B31" s="74"/>
       <c r="C31" s="11" t="s">
         <v>29</v>
       </c>
@@ -4390,10 +4390,10 @@
       <c r="I33" s="1"/>
     </row>
     <row r="34" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="72" t="s">
         <v>41</v>
       </c>
       <c r="C34" s="11" t="s">
@@ -4411,8 +4411,8 @@
       <c r="I34" s="1"/>
     </row>
     <row r="35" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="11" t="s">
         <v>141</v>
       </c>
@@ -4428,8 +4428,8 @@
       <c r="I35" s="1"/>
     </row>
     <row r="36" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="77"/>
-      <c r="B36" s="77"/>
+      <c r="A36" s="73"/>
+      <c r="B36" s="73"/>
       <c r="C36" s="11" t="s">
         <v>142</v>
       </c>
@@ -4445,8 +4445,8 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="77"/>
-      <c r="B37" s="77"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="73"/>
       <c r="C37" s="11" t="s">
         <v>143</v>
       </c>
@@ -4462,16 +4462,16 @@
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
+      <c r="A38" s="73"/>
+      <c r="B38" s="73"/>
       <c r="C38" s="11" t="s">
         <v>144</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E38" s="68" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
@@ -4479,8 +4479,8 @@
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="78"/>
-      <c r="B39" s="78"/>
+      <c r="A39" s="74"/>
+      <c r="B39" s="74"/>
       <c r="C39" s="11" t="s">
         <v>29</v>
       </c>
@@ -4539,10 +4539,10 @@
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="76" t="s">
+      <c r="B43" s="72" t="s">
         <v>42</v>
       </c>
       <c r="C43" s="11" t="s">
@@ -4560,8 +4560,8 @@
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="77"/>
-      <c r="B44" s="77"/>
+      <c r="A44" s="73"/>
+      <c r="B44" s="73"/>
       <c r="C44" s="11" t="s">
         <v>141</v>
       </c>
@@ -4577,8 +4577,8 @@
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="77"/>
-      <c r="B45" s="77"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="73"/>
       <c r="C45" s="11" t="s">
         <v>142</v>
       </c>
@@ -4594,8 +4594,8 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="77"/>
-      <c r="B46" s="77"/>
+      <c r="A46" s="73"/>
+      <c r="B46" s="73"/>
       <c r="C46" s="11" t="s">
         <v>143</v>
       </c>
@@ -4611,16 +4611,16 @@
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="77"/>
-      <c r="B47" s="77"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="73"/>
       <c r="C47" s="11" t="s">
         <v>144</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E47" s="67" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
@@ -4628,8 +4628,8 @@
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="78"/>
-      <c r="B48" s="78"/>
+      <c r="A48" s="74"/>
+      <c r="B48" s="74"/>
       <c r="C48" s="11" t="s">
         <v>29</v>
       </c>
@@ -4716,11 +4716,11 @@
         <v>5</v>
       </c>
       <c r="B54" s="75"/>
-      <c r="C54" s="73" t="s">
+      <c r="C54" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="73"/>
-      <c r="E54" s="73"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="80"/>
       <c r="F54" s="31" t="s">
         <v>4</v>
       </c>
@@ -4734,8 +4734,8 @@
       <c r="C55" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="74"/>
-      <c r="E55" s="74"/>
+      <c r="D55" s="81"/>
+      <c r="E55" s="81"/>
       <c r="F55" s="23">
         <v>6108</v>
       </c>
@@ -4749,8 +4749,8 @@
       <c r="C56" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="74"/>
-      <c r="E56" s="74"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="81"/>
       <c r="F56" s="23">
         <v>5584</v>
       </c>
@@ -4764,8 +4764,8 @@
       <c r="C57" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="74"/>
-      <c r="E57" s="74"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="81"/>
       <c r="F57" s="23">
         <v>5061</v>
       </c>
@@ -4779,8 +4779,8 @@
       <c r="C58" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="D58" s="74"/>
-      <c r="E58" s="74"/>
+      <c r="D58" s="81"/>
+      <c r="E58" s="81"/>
       <c r="F58" s="23">
         <v>4363</v>
       </c>
@@ -5175,10 +5175,10 @@
       <c r="D101" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E101" s="72" t="s">
+      <c r="E101" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="F101" s="72"/>
+      <c r="F101" s="79"/>
       <c r="G101" s="49"/>
       <c r="H101" s="50"/>
       <c r="I101" s="50"/>
@@ -5311,6 +5311,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
     <mergeCell ref="E101:F101"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
@@ -5327,12 +5333,6 @@
     <mergeCell ref="A43:A48"/>
     <mergeCell ref="B43:B48"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A18:A23"/>
-    <mergeCell ref="B18:B23"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -6288,10 +6288,10 @@
       <c r="D97" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E97" s="72" t="s">
+      <c r="E97" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="F97" s="72"/>
+      <c r="F97" s="79"/>
       <c r="G97" s="49"/>
     </row>
     <row r="98" spans="1:7" ht="13.5" x14ac:dyDescent="0.35">
@@ -6492,30 +6492,10 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="LSC Office Document" ma:contentTypeID="0x010100E4FE8612EC394E3690F102C0A1A07561006D4FE4F5DA52754EADB7699CD775C80000276A6CD12789A54A801089F3050C193D" ma:contentTypeVersion="0" ma:contentTypeDescription="The LSC Office Document content type is used by the documents in libraries throughout LSC's sites." ma:contentTypeScope="" ma:versionID="b893b1e7c5db64194e7bbe2166059f39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8494e17d-b33d-40a5-bfb5-2205ff88b06a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64166444d08279df21762ba0236a24f3" ns2:_="">
     <xsd:import namespace="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
@@ -6659,34 +6639,39 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <DocumentPublisher xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentKeywords xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentSecurityClassification xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentAuthor xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentPublishedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentCreatedDate xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentType xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+    <DocumentDescription xmlns="8494e17d-b33d-40a5-bfb5-2205ff88b06a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85F5FD82-8629-4CA9-BF0A-1592810000E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6703,10 +6688,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39C700E6-C50B-440C-9C6F-D75020AA789E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B2B7905-31E5-4ECB-8F07-15754D30164D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38CBE44C-A816-4A08-BCBD-FDABCF2781A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="8494e17d-b33d-40a5-bfb5-2205ff88b06a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>